<commit_message>
issue #191: I forgot this (I did not use it to generate code [because I don't know how], I commit it just to keep everything in sync)
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laurent\OneDrive\Dev\Github\TypeCobol\TypeCobol.Grammar\Grammars\Cobol\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14325" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="470">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1428,6 +1423,12 @@
   </si>
   <si>
     <t>YYYYMMDD</t>
+  </si>
+  <si>
+    <t>TYPEDEF</t>
+  </si>
+  <si>
+    <t>STRONG</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1738,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1745,13 +1746,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D450"/>
+  <dimension ref="A1:D452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="C451" sqref="C451"/>
+    <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
+      <selection activeCell="C453" sqref="C453"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
@@ -7938,7 +7939,7 @@
         <v>450</v>
       </c>
       <c r="B387">
-        <f t="shared" ref="B387:B450" si="13">B386+1</f>
+        <f t="shared" ref="B387:B451" si="13">B386+1</f>
         <v>387</v>
       </c>
       <c r="C387" t="s">
@@ -8953,8 +8954,40 @@
         <v>467</v>
       </c>
       <c r="D450" t="str">
-        <f t="shared" ref="D450" si="14">"        "&amp;C450&amp;"="&amp;B450&amp;","</f>
+        <f t="shared" ref="D450:D451" si="14">"        "&amp;C450&amp;"="&amp;B450&amp;","</f>
         <v xml:space="preserve">        YYYYMMDD=450,</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>450</v>
+      </c>
+      <c r="B451">
+        <f t="shared" si="13"/>
+        <v>451</v>
+      </c>
+      <c r="C451" t="s">
+        <v>468</v>
+      </c>
+      <c r="D451" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        TYPEDEF=451,</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>450</v>
+      </c>
+      <c r="B452">
+        <f t="shared" ref="B452" si="15">B451+1</f>
+        <v>452</v>
+      </c>
+      <c r="C452" t="s">
+        <v>469</v>
+      </c>
+      <c r="D452" t="str">
+        <f t="shared" ref="D452" si="16">"        "&amp;C452&amp;"="&amp;B452&amp;","</f>
+        <v xml:space="preserve">        STRONG=452,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue #210: create UNSAFE keyword
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="471">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1429,6 +1429,9 @@
   </si>
   <si>
     <t>STRONG</t>
+  </si>
+  <si>
+    <t>UNSAFE</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1746,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D452"/>
+  <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
-      <selection activeCell="C453" sqref="C453"/>
+      <selection activeCell="D454" sqref="D454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8979,7 +8982,7 @@
         <v>450</v>
       </c>
       <c r="B452">
-        <f t="shared" ref="B452" si="15">B451+1</f>
+        <f t="shared" ref="B452:B453" si="15">B451+1</f>
         <v>452</v>
       </c>
       <c r="C452" t="s">
@@ -8988,6 +8991,19 @@
       <c r="D452" t="str">
         <f t="shared" ref="D452" si="16">"        "&amp;C452&amp;"="&amp;B452&amp;","</f>
         <v xml:space="preserve">        STRONG=452,</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B453">
+        <f t="shared" si="15"/>
+        <v>453</v>
+      </c>
+      <c r="C453" t="s">
+        <v>470</v>
+      </c>
+      <c r="D453" t="str">
+        <f t="shared" ref="D453" si="17">"        "&amp;C453&amp;"="&amp;B453&amp;","</f>
+        <v xml:space="preserve">        UNSAFE=453,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue #245: add DECLARE and END-DECLARE keywords to the TypeCobol languge
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="473">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1432,6 +1432,12 @@
   </si>
   <si>
     <t>UNSAFE</t>
+  </si>
+  <si>
+    <t>END_DECLARE</t>
+  </si>
+  <si>
+    <t>DECLARE</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1747,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1749,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D453"/>
+  <dimension ref="A1:D455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
-      <selection activeCell="D454" sqref="D454"/>
+    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
+      <selection activeCell="B457" sqref="B457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8982,7 +8988,7 @@
         <v>450</v>
       </c>
       <c r="B452">
-        <f t="shared" ref="B452:B453" si="15">B451+1</f>
+        <f t="shared" ref="B452:B455" si="15">B451+1</f>
         <v>452</v>
       </c>
       <c r="C452" t="s">
@@ -8999,11 +9005,36 @@
         <v>453</v>
       </c>
       <c r="C453" t="s">
+        <v>472</v>
+      </c>
+      <c r="D453" t="str">
+        <f t="shared" ref="D453:D454" si="17">"        "&amp;C453&amp;"="&amp;B453&amp;","</f>
+        <v xml:space="preserve">        DECLARE=453,</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B454">
+        <v>454</v>
+      </c>
+      <c r="C454" t="s">
+        <v>471</v>
+      </c>
+      <c r="D454" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">        END_DECLARE=454,</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B455">
+        <f t="shared" si="15"/>
+        <v>455</v>
+      </c>
+      <c r="C455" t="s">
         <v>470</v>
       </c>
-      <c r="D453" t="str">
-        <f t="shared" ref="D453" si="17">"        "&amp;C453&amp;"="&amp;B453&amp;","</f>
-        <v xml:space="preserve">        UNSAFE=453,</v>
+      <c r="D455" t="str">
+        <f t="shared" ref="D455" si="18">"        "&amp;C455&amp;"="&amp;B455&amp;","</f>
+        <v xml:space="preserve">        UNSAFE=455,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
issue #245: add PRIVATE and PUBLIC keywords to grammar
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="475">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1438,6 +1438,12 @@
   </si>
   <si>
     <t>DECLARE</t>
+  </si>
+  <si>
+    <t>PUBLIC</t>
+  </si>
+  <si>
+    <t>PRIVATE</t>
   </si>
 </sst>
 </file>
@@ -1747,7 +1753,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1755,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D455"/>
+  <dimension ref="A1:D457"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
-      <selection activeCell="B457" sqref="B457"/>
+    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="C458" sqref="C458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8988,7 +8994,7 @@
         <v>450</v>
       </c>
       <c r="B452">
-        <f t="shared" ref="B452:B455" si="15">B451+1</f>
+        <f t="shared" ref="B452:B457" si="15">B451+1</f>
         <v>452</v>
       </c>
       <c r="C452" t="s">
@@ -9037,6 +9043,32 @@
         <v xml:space="preserve">        UNSAFE=455,</v>
       </c>
     </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B456">
+        <f t="shared" si="15"/>
+        <v>456</v>
+      </c>
+      <c r="C456" t="s">
+        <v>473</v>
+      </c>
+      <c r="D456" t="str">
+        <f t="shared" ref="D456:D457" si="19">"        "&amp;C456&amp;"="&amp;B456&amp;","</f>
+        <v xml:space="preserve">        PUBLIC=456,</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B457">
+        <f t="shared" si="15"/>
+        <v>457</v>
+      </c>
+      <c r="C457" t="s">
+        <v>474</v>
+      </c>
+      <c r="D457" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">        PRIVATE=457,</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
issue #245: create INOUT keyword
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="476">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1444,6 +1444,9 @@
   </si>
   <si>
     <t>PRIVATE</t>
+  </si>
+  <si>
+    <t>INOUT</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1756,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1761,10 +1764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D457"/>
+  <dimension ref="A1:D458"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="C458" sqref="C458"/>
+      <selection activeCell="C459" sqref="C459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8994,7 +8997,7 @@
         <v>450</v>
       </c>
       <c r="B452">
-        <f t="shared" ref="B452:B457" si="15">B451+1</f>
+        <f t="shared" ref="B452:B458" si="15">B451+1</f>
         <v>452</v>
       </c>
       <c r="C452" t="s">
@@ -9069,6 +9072,19 @@
         <v xml:space="preserve">        PRIVATE=457,</v>
       </c>
     </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B458">
+        <f t="shared" si="15"/>
+        <v>458</v>
+      </c>
+      <c r="C458" t="s">
+        <v>475</v>
+      </c>
+      <c r="D458" t="str">
+        <f t="shared" ref="D458" si="20">"        "&amp;C458&amp;"="&amp;B458&amp;","</f>
+        <v xml:space="preserve">        INOUT=458,</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#578, remove XML_DECLARATION Token, add predicate on XmlGenerate rule
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="480">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1338,9 +1338,6 @@
   </si>
   <si>
     <t>WRITE_ONLY</t>
-  </si>
-  <si>
-    <t>XML_DECLARATION</t>
   </si>
   <si>
     <t>XML_SCHEMA</t>
@@ -1878,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D463"/>
+  <dimension ref="A1:D462"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A439" workbookViewId="0">
-      <selection activeCell="C467" sqref="C467"/>
+      <selection activeCell="C465" sqref="C465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,7 +1893,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B1" s="1">
         <v>-1</v>
@@ -1911,14 +1908,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B2" s="1">
         <f>B1+1</f>
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D2" t="str">
         <f>"        "&amp;C2&amp;"="&amp;B2&amp;","</f>
@@ -1927,7 +1924,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B3" s="1">
         <f>B2+1</f>
@@ -1943,7 +1940,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B67" si="1">B3+1</f>
@@ -1959,7 +1956,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="1"/>
@@ -1975,7 +1972,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="1"/>
@@ -1991,7 +1988,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="1"/>
@@ -2007,7 +2004,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="1"/>
@@ -2023,7 +2020,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="1"/>
@@ -2039,14 +2036,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2055,7 +2052,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="1"/>
@@ -2071,7 +2068,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="1"/>
@@ -2087,7 +2084,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="1"/>
@@ -2103,7 +2100,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
@@ -2119,7 +2116,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
@@ -2135,7 +2132,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
@@ -2151,7 +2148,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
@@ -2167,7 +2164,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
@@ -2183,7 +2180,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
@@ -2199,7 +2196,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="1"/>
@@ -2215,7 +2212,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="1"/>
@@ -2231,7 +2228,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="1"/>
@@ -2247,7 +2244,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="1"/>
@@ -2263,7 +2260,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="1"/>
@@ -2279,7 +2276,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="1"/>
@@ -2295,7 +2292,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="1"/>
@@ -2311,7 +2308,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="1"/>
@@ -2327,7 +2324,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="1"/>
@@ -2356,14 +2353,14 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2372,7 +2369,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" si="1"/>
@@ -2388,7 +2385,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="1"/>
@@ -2404,7 +2401,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" si="1"/>
@@ -2420,7 +2417,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" si="1"/>
@@ -2436,7 +2433,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" si="1"/>
@@ -2465,14 +2462,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2481,14 +2478,14 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2497,7 +2494,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="1"/>
@@ -2513,14 +2510,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2529,7 +2526,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="1"/>
@@ -2545,7 +2542,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" si="1"/>
@@ -2561,7 +2558,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" si="1"/>
@@ -2577,7 +2574,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="1"/>
@@ -2593,7 +2590,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" si="1"/>
@@ -2609,7 +2606,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" si="1"/>
@@ -2625,7 +2622,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" si="1"/>
@@ -2641,7 +2638,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" si="1"/>
@@ -2657,7 +2654,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B49" s="1">
         <f t="shared" si="1"/>
@@ -2673,7 +2670,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" si="1"/>
@@ -2689,7 +2686,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B51" s="1">
         <f t="shared" si="1"/>
@@ -2705,7 +2702,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" si="1"/>
@@ -2721,7 +2718,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B53" s="1">
         <f t="shared" si="1"/>
@@ -2737,7 +2734,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B54" s="1">
         <f t="shared" si="1"/>
@@ -2753,7 +2750,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B55" s="1">
         <f t="shared" si="1"/>
@@ -2769,14 +2766,14 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2785,7 +2782,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B57" s="1">
         <f t="shared" si="1"/>
@@ -2801,7 +2798,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B58" s="1">
         <f t="shared" si="1"/>
@@ -2817,7 +2814,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B59" s="1">
         <f t="shared" si="1"/>
@@ -2833,7 +2830,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B60" s="1">
         <f t="shared" si="1"/>
@@ -2849,7 +2846,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B61" s="1">
         <f t="shared" si="1"/>
@@ -2865,7 +2862,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B62" s="1">
         <f t="shared" si="1"/>
@@ -2881,7 +2878,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B63" s="1">
         <f t="shared" si="1"/>
@@ -2897,7 +2894,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B64" s="1">
         <f t="shared" si="1"/>
@@ -2913,7 +2910,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B65" s="1">
         <f t="shared" si="1"/>
@@ -2929,7 +2926,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B66" s="1">
         <f t="shared" si="1"/>
@@ -2945,7 +2942,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B67" s="1">
         <f t="shared" si="1"/>
@@ -2961,7 +2958,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B68" s="1">
         <f t="shared" ref="B68:B131" si="3">B67+1</f>
@@ -2977,7 +2974,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
@@ -2993,7 +2990,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
@@ -3009,7 +3006,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
@@ -3025,7 +3022,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
@@ -3041,14 +3038,14 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -3057,7 +3054,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
@@ -3073,7 +3070,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
@@ -3089,7 +3086,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
@@ -3121,7 +3118,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
@@ -3137,7 +3134,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
@@ -3153,7 +3150,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B80" s="1">
         <f t="shared" si="3"/>
@@ -3169,7 +3166,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B81" s="1">
         <f t="shared" si="3"/>
@@ -3185,14 +3182,14 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B82" s="1">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3201,7 +3198,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B83" s="1">
         <f t="shared" si="3"/>
@@ -3217,7 +3214,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B84" s="1">
         <f t="shared" si="3"/>
@@ -3233,7 +3230,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B85" s="1">
         <f t="shared" si="3"/>
@@ -3249,7 +3246,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B86" s="1">
         <f t="shared" si="3"/>
@@ -3265,7 +3262,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B87" s="1">
         <f t="shared" si="3"/>
@@ -3281,7 +3278,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B88" s="1">
         <f t="shared" si="3"/>
@@ -3297,7 +3294,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B89" s="1">
         <f t="shared" si="3"/>
@@ -3313,7 +3310,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B90" s="1">
         <f t="shared" si="3"/>
@@ -3329,7 +3326,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B91" s="1">
         <f t="shared" si="3"/>
@@ -3345,7 +3342,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B92" s="1">
         <f t="shared" si="3"/>
@@ -3361,7 +3358,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B93" s="1">
         <f t="shared" si="3"/>
@@ -3377,7 +3374,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B94" s="1">
         <f t="shared" si="3"/>
@@ -3393,7 +3390,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B95" s="1">
         <f t="shared" si="3"/>
@@ -3409,7 +3406,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B96" s="1">
         <f t="shared" si="3"/>
@@ -3425,7 +3422,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B97" s="1">
         <f t="shared" si="3"/>
@@ -3441,7 +3438,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B98" s="1">
         <f t="shared" si="3"/>
@@ -3457,7 +3454,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B99" s="1">
         <f t="shared" si="3"/>
@@ -3473,7 +3470,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B100" s="1">
         <f t="shared" si="3"/>
@@ -3489,7 +3486,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B101" s="1">
         <f t="shared" si="3"/>
@@ -3505,7 +3502,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B102" s="1">
         <f t="shared" si="3"/>
@@ -3521,7 +3518,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B103" s="1">
         <f t="shared" si="3"/>
@@ -3537,7 +3534,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B104" s="1">
         <f t="shared" si="3"/>
@@ -3553,7 +3550,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B105" s="1">
         <f t="shared" si="3"/>
@@ -3569,7 +3566,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B106" s="1">
         <f t="shared" si="3"/>
@@ -3585,7 +3582,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B107" s="1">
         <f t="shared" si="3"/>
@@ -3601,7 +3598,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B108" s="1">
         <f t="shared" si="3"/>
@@ -3617,7 +3614,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B109" s="1">
         <f t="shared" si="3"/>
@@ -3633,7 +3630,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B110" s="1">
         <f t="shared" si="3"/>
@@ -3649,7 +3646,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B111" s="1">
         <f t="shared" si="3"/>
@@ -3665,7 +3662,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B112" s="1">
         <f t="shared" si="3"/>
@@ -3681,7 +3678,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B113" s="1">
         <f t="shared" si="3"/>
@@ -3697,7 +3694,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B114" s="1">
         <f t="shared" si="3"/>
@@ -3713,7 +3710,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B115" s="1">
         <f t="shared" si="3"/>
@@ -3729,7 +3726,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B116" s="1">
         <f t="shared" si="3"/>
@@ -3745,7 +3742,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B117" s="1">
         <f t="shared" si="3"/>
@@ -3761,7 +3758,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B118" s="1">
         <f t="shared" si="3"/>
@@ -3777,7 +3774,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B119" s="1">
         <f t="shared" si="3"/>
@@ -3793,7 +3790,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B120" s="1">
         <f t="shared" si="3"/>
@@ -3809,7 +3806,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B121" s="1">
         <f t="shared" si="3"/>
@@ -3825,7 +3822,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B122" s="1">
         <f t="shared" si="3"/>
@@ -3841,7 +3838,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B123" s="1">
         <f t="shared" si="3"/>
@@ -3857,7 +3854,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B124" s="1">
         <f t="shared" si="3"/>
@@ -3873,7 +3870,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B125" s="1">
         <f t="shared" si="3"/>
@@ -3889,7 +3886,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B126" s="1">
         <f t="shared" si="3"/>
@@ -3905,7 +3902,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B127" s="1">
         <f t="shared" si="3"/>
@@ -3921,7 +3918,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B128" s="1">
         <f t="shared" si="3"/>
@@ -3937,7 +3934,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B129" s="1">
         <f t="shared" si="3"/>
@@ -3953,7 +3950,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B130" s="1">
         <f t="shared" si="3"/>
@@ -3969,7 +3966,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B131" s="1">
         <f t="shared" si="3"/>
@@ -3985,7 +3982,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B132" s="1">
         <f t="shared" ref="B132:B195" si="5">B131+1</f>
@@ -4001,7 +3998,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B133" s="1">
         <f t="shared" si="5"/>
@@ -4017,7 +4014,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B134" s="1">
         <f t="shared" si="5"/>
@@ -4033,7 +4030,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B135" s="1">
         <f t="shared" si="5"/>
@@ -4049,7 +4046,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B136" s="1">
         <f t="shared" si="5"/>
@@ -4065,7 +4062,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B137" s="1">
         <f t="shared" si="5"/>
@@ -4081,7 +4078,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B138" s="1">
         <f t="shared" si="5"/>
@@ -4097,7 +4094,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B139" s="1">
         <f t="shared" si="5"/>
@@ -4113,7 +4110,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B140" s="1">
         <f t="shared" si="5"/>
@@ -4129,7 +4126,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B141" s="1">
         <f t="shared" si="5"/>
@@ -4145,7 +4142,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B142" s="1">
         <f t="shared" si="5"/>
@@ -4161,7 +4158,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B143" s="1">
         <f t="shared" si="5"/>
@@ -4177,7 +4174,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B144" s="1">
         <f t="shared" si="5"/>
@@ -4193,7 +4190,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B145" s="1">
         <f t="shared" si="5"/>
@@ -4209,7 +4206,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B146" s="1">
         <f t="shared" si="5"/>
@@ -4225,7 +4222,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B147" s="1">
         <f t="shared" si="5"/>
@@ -4241,7 +4238,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B148" s="1">
         <f t="shared" si="5"/>
@@ -4257,7 +4254,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B149" s="1">
         <f t="shared" si="5"/>
@@ -4273,7 +4270,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B150" s="1">
         <f t="shared" si="5"/>
@@ -4289,7 +4286,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B151" s="1">
         <f t="shared" si="5"/>
@@ -4305,7 +4302,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B152" s="1">
         <f t="shared" si="5"/>
@@ -4321,7 +4318,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B153" s="1">
         <f t="shared" si="5"/>
@@ -4337,7 +4334,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B154" s="1">
         <f t="shared" si="5"/>
@@ -4353,7 +4350,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B155" s="1">
         <f t="shared" si="5"/>
@@ -4369,7 +4366,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B156" s="1">
         <f t="shared" si="5"/>
@@ -4385,7 +4382,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B157" s="1">
         <f t="shared" si="5"/>
@@ -4401,7 +4398,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B158" s="1">
         <f t="shared" si="5"/>
@@ -4417,7 +4414,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B159" s="1">
         <f t="shared" si="5"/>
@@ -4433,7 +4430,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B160" s="1">
         <f t="shared" si="5"/>
@@ -4449,7 +4446,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B161" s="1">
         <f t="shared" si="5"/>
@@ -4465,7 +4462,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B162" s="1">
         <f t="shared" si="5"/>
@@ -4481,7 +4478,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B163" s="1">
         <f t="shared" si="5"/>
@@ -4497,7 +4494,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B164" s="1">
         <f t="shared" si="5"/>
@@ -4513,7 +4510,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B165" s="1">
         <f t="shared" si="5"/>
@@ -4529,7 +4526,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B166" s="1">
         <f t="shared" si="5"/>
@@ -4545,7 +4542,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B167" s="1">
         <f t="shared" si="5"/>
@@ -4561,7 +4558,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B168" s="1">
         <f t="shared" si="5"/>
@@ -4577,7 +4574,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B169" s="1">
         <f t="shared" si="5"/>
@@ -4593,7 +4590,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B170" s="1">
         <f t="shared" si="5"/>
@@ -4609,7 +4606,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B171" s="1">
         <f t="shared" si="5"/>
@@ -4625,7 +4622,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B172" s="1">
         <f t="shared" si="5"/>
@@ -4641,7 +4638,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B173" s="1">
         <f t="shared" si="5"/>
@@ -4657,7 +4654,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B174" s="1">
         <f t="shared" si="5"/>
@@ -4673,7 +4670,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B175" s="1">
         <f t="shared" si="5"/>
@@ -4689,7 +4686,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B176" s="1">
         <f t="shared" si="5"/>
@@ -4705,7 +4702,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B177" s="1">
         <f t="shared" si="5"/>
@@ -4721,7 +4718,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B178" s="1">
         <f t="shared" si="5"/>
@@ -4737,7 +4734,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B179" s="1">
         <f t="shared" si="5"/>
@@ -4753,7 +4750,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B180" s="1">
         <f t="shared" si="5"/>
@@ -4769,7 +4766,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B181" s="1">
         <f t="shared" si="5"/>
@@ -4785,7 +4782,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B182" s="1">
         <f t="shared" si="5"/>
@@ -4801,7 +4798,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B183" s="1">
         <f t="shared" si="5"/>
@@ -4817,7 +4814,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B184" s="1">
         <f t="shared" si="5"/>
@@ -4833,7 +4830,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B185" s="1">
         <f t="shared" si="5"/>
@@ -4849,7 +4846,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B186" s="1">
         <f t="shared" si="5"/>
@@ -4865,7 +4862,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B187" s="1">
         <f t="shared" si="5"/>
@@ -4881,7 +4878,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B188" s="1">
         <f t="shared" si="5"/>
@@ -4897,7 +4894,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B189" s="1">
         <f t="shared" si="5"/>
@@ -4913,7 +4910,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B190" s="1">
         <f t="shared" si="5"/>
@@ -4929,7 +4926,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B191" s="1">
         <f t="shared" si="5"/>
@@ -4945,7 +4942,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B192" s="1">
         <f t="shared" si="5"/>
@@ -4961,7 +4958,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B193" s="1">
         <f t="shared" si="5"/>
@@ -4977,7 +4974,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B194" s="1">
         <f t="shared" si="5"/>
@@ -4993,7 +4990,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B195" s="1">
         <f t="shared" si="5"/>
@@ -5009,7 +5006,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B196" s="1">
         <f t="shared" ref="B196:B258" si="7">B195+1</f>
@@ -5025,7 +5022,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B197" s="1">
         <f t="shared" si="7"/>
@@ -5041,7 +5038,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B198" s="1">
         <f t="shared" si="7"/>
@@ -5057,7 +5054,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B199" s="1">
         <f t="shared" si="7"/>
@@ -5073,7 +5070,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B200" s="1">
         <f t="shared" si="7"/>
@@ -5089,7 +5086,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B201" s="1">
         <f t="shared" si="7"/>
@@ -5105,7 +5102,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B202" s="1">
         <f t="shared" si="7"/>
@@ -5121,7 +5118,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B203" s="1">
         <f t="shared" si="7"/>
@@ -5137,7 +5134,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B204" s="1">
         <f t="shared" si="7"/>
@@ -5153,7 +5150,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B205" s="1">
         <f t="shared" si="7"/>
@@ -5169,7 +5166,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B206" s="1">
         <f t="shared" si="7"/>
@@ -5185,7 +5182,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B207" s="1">
         <f t="shared" si="7"/>
@@ -5201,7 +5198,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B208" s="1">
         <f t="shared" si="7"/>
@@ -5217,7 +5214,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B209" s="1">
         <f t="shared" si="7"/>
@@ -5233,7 +5230,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B210" s="1">
         <f t="shared" si="7"/>
@@ -5249,7 +5246,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B211" s="1">
         <f t="shared" si="7"/>
@@ -5265,7 +5262,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B212" s="1">
         <f t="shared" si="7"/>
@@ -5281,7 +5278,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B213" s="1">
         <f t="shared" si="7"/>
@@ -5297,7 +5294,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B214" s="1">
         <f t="shared" si="7"/>
@@ -5313,7 +5310,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B215" s="1">
         <f t="shared" si="7"/>
@@ -5329,7 +5326,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B216" s="1">
         <f t="shared" si="7"/>
@@ -5345,7 +5342,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B217" s="1">
         <f t="shared" si="7"/>
@@ -5361,7 +5358,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B218" s="1">
         <f t="shared" si="7"/>
@@ -5377,7 +5374,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B219" s="1">
         <f t="shared" si="7"/>
@@ -5393,7 +5390,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B220" s="1">
         <f t="shared" si="7"/>
@@ -5409,7 +5406,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B221" s="1">
         <f t="shared" si="7"/>
@@ -5425,7 +5422,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B222" s="1">
         <f t="shared" si="7"/>
@@ -5441,7 +5438,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B223" s="1">
         <f t="shared" si="7"/>
@@ -5457,7 +5454,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B224" s="1">
         <f t="shared" si="7"/>
@@ -5473,7 +5470,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B225" s="1">
         <f t="shared" si="7"/>
@@ -5489,7 +5486,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B226" s="1">
         <f t="shared" si="7"/>
@@ -5505,7 +5502,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B227" s="1">
         <f t="shared" si="7"/>
@@ -5521,7 +5518,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B228" s="1">
         <f t="shared" si="7"/>
@@ -5537,7 +5534,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B229" s="1">
         <f t="shared" si="7"/>
@@ -5553,7 +5550,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B230" s="1">
         <f t="shared" si="7"/>
@@ -5569,7 +5566,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B231" s="1">
         <f t="shared" si="7"/>
@@ -5585,7 +5582,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B232" s="1">
         <f t="shared" si="7"/>
@@ -5601,7 +5598,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B233" s="1">
         <f t="shared" si="7"/>
@@ -5617,7 +5614,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B234" s="1">
         <f t="shared" si="7"/>
@@ -5633,7 +5630,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B235" s="1">
         <f t="shared" si="7"/>
@@ -5649,7 +5646,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B236" s="1">
         <f t="shared" si="7"/>
@@ -5665,7 +5662,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B237" s="1">
         <f t="shared" si="7"/>
@@ -5681,7 +5678,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B238" s="1">
         <f t="shared" si="7"/>
@@ -5697,7 +5694,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B239" s="1">
         <f t="shared" si="7"/>
@@ -5713,7 +5710,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B240" s="1">
         <f t="shared" si="7"/>
@@ -5729,7 +5726,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B241" s="1">
         <f t="shared" si="7"/>
@@ -5745,7 +5742,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B242" s="1">
         <f t="shared" si="7"/>
@@ -5761,7 +5758,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B243" s="1">
         <f t="shared" si="7"/>
@@ -5777,7 +5774,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B244" s="1">
         <f t="shared" si="7"/>
@@ -5793,7 +5790,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B245" s="1">
         <f t="shared" si="7"/>
@@ -5809,7 +5806,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B246" s="1">
         <f t="shared" si="7"/>
@@ -5825,7 +5822,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B247" s="1">
         <f t="shared" si="7"/>
@@ -5841,7 +5838,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B248" s="1">
         <f t="shared" si="7"/>
@@ -5857,7 +5854,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B249" s="1">
         <f t="shared" si="7"/>
@@ -5873,7 +5870,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B250" s="1">
         <f t="shared" si="7"/>
@@ -5889,7 +5886,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B251" s="1">
         <f t="shared" si="7"/>
@@ -5905,7 +5902,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B252" s="1">
         <f t="shared" si="7"/>
@@ -5921,7 +5918,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B253" s="1">
         <f t="shared" si="7"/>
@@ -5937,7 +5934,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B254" s="1">
         <f t="shared" si="7"/>
@@ -5953,7 +5950,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B255" s="1">
         <f t="shared" si="7"/>
@@ -5969,7 +5966,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B256" s="1">
         <f t="shared" si="7"/>
@@ -5985,7 +5982,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B257" s="1">
         <f t="shared" si="7"/>
@@ -6001,7 +5998,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B258" s="1">
         <f t="shared" si="7"/>
@@ -6017,7 +6014,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B259" s="1">
         <f t="shared" ref="B259:B321" si="9">B258+1</f>
@@ -6033,7 +6030,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B260" s="1">
         <f t="shared" si="9"/>
@@ -6049,7 +6046,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B261" s="1">
         <f t="shared" si="9"/>
@@ -6065,7 +6062,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B262" s="1">
         <f t="shared" si="9"/>
@@ -6081,7 +6078,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B263" s="1">
         <f t="shared" si="9"/>
@@ -6097,7 +6094,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B264" s="1">
         <f t="shared" si="9"/>
@@ -6113,7 +6110,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B265" s="1">
         <f t="shared" si="9"/>
@@ -6129,7 +6126,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B266" s="1">
         <f t="shared" si="9"/>
@@ -6145,7 +6142,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B267" s="1">
         <f t="shared" si="9"/>
@@ -6161,7 +6158,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B268" s="1">
         <f t="shared" si="9"/>
@@ -6177,7 +6174,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B269" s="1">
         <f t="shared" si="9"/>
@@ -6193,7 +6190,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B270" s="1">
         <f t="shared" si="9"/>
@@ -6209,7 +6206,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B271" s="1">
         <f t="shared" si="9"/>
@@ -6225,7 +6222,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B272" s="1">
         <f t="shared" si="9"/>
@@ -6241,7 +6238,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B273" s="1">
         <f t="shared" si="9"/>
@@ -6257,7 +6254,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B274" s="1">
         <f t="shared" si="9"/>
@@ -6273,7 +6270,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B275" s="1">
         <f t="shared" si="9"/>
@@ -6289,7 +6286,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B276" s="1">
         <f t="shared" si="9"/>
@@ -6305,7 +6302,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B277" s="1">
         <f t="shared" si="9"/>
@@ -6321,7 +6318,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B278" s="1">
         <f t="shared" si="9"/>
@@ -6337,7 +6334,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B279" s="1">
         <f t="shared" si="9"/>
@@ -6353,7 +6350,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B280" s="1">
         <f t="shared" si="9"/>
@@ -6369,7 +6366,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B281" s="1">
         <f t="shared" si="9"/>
@@ -6385,7 +6382,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B282" s="1">
         <f t="shared" si="9"/>
@@ -6401,7 +6398,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B283" s="1">
         <f t="shared" si="9"/>
@@ -6417,7 +6414,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B284" s="1">
         <f t="shared" si="9"/>
@@ -6433,7 +6430,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B285" s="1">
         <f t="shared" si="9"/>
@@ -6449,7 +6446,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B286" s="1">
         <f t="shared" si="9"/>
@@ -6465,7 +6462,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B287" s="1">
         <f t="shared" si="9"/>
@@ -6481,7 +6478,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B288" s="1">
         <f t="shared" si="9"/>
@@ -6497,7 +6494,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B289" s="1">
         <f t="shared" si="9"/>
@@ -6513,7 +6510,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B290" s="1">
         <f t="shared" si="9"/>
@@ -6529,7 +6526,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B291" s="1">
         <f t="shared" si="9"/>
@@ -6545,7 +6542,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B292" s="1">
         <f t="shared" si="9"/>
@@ -6561,7 +6558,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B293" s="1">
         <f t="shared" si="9"/>
@@ -6577,7 +6574,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B294" s="1">
         <f t="shared" si="9"/>
@@ -6593,7 +6590,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B295" s="1">
         <f t="shared" si="9"/>
@@ -6609,7 +6606,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B296" s="1">
         <f t="shared" si="9"/>
@@ -6625,7 +6622,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B297" s="1">
         <f t="shared" si="9"/>
@@ -6641,7 +6638,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B298" s="1">
         <f t="shared" si="9"/>
@@ -6657,7 +6654,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B299" s="1">
         <f t="shared" si="9"/>
@@ -6673,7 +6670,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B300" s="1">
         <f t="shared" si="9"/>
@@ -6689,7 +6686,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B301" s="1">
         <f t="shared" si="9"/>
@@ -6705,7 +6702,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B302" s="1">
         <f t="shared" si="9"/>
@@ -6721,7 +6718,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B303" s="1">
         <f t="shared" si="9"/>
@@ -6737,7 +6734,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B304" s="1">
         <f t="shared" si="9"/>
@@ -6753,7 +6750,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B305" s="1">
         <f t="shared" si="9"/>
@@ -6769,7 +6766,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B306" s="1">
         <f t="shared" si="9"/>
@@ -6785,7 +6782,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B307" s="1">
         <f t="shared" si="9"/>
@@ -6801,7 +6798,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B308" s="1">
         <f t="shared" si="9"/>
@@ -6817,7 +6814,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B309" s="1">
         <f t="shared" si="9"/>
@@ -6833,7 +6830,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B310" s="1">
         <f t="shared" si="9"/>
@@ -6849,7 +6846,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B311" s="1">
         <f t="shared" si="9"/>
@@ -6865,7 +6862,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B312" s="1">
         <f t="shared" si="9"/>
@@ -6881,7 +6878,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B313" s="1">
         <f t="shared" si="9"/>
@@ -6897,7 +6894,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B314" s="1">
         <f t="shared" si="9"/>
@@ -6913,7 +6910,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B315" s="1">
         <f t="shared" si="9"/>
@@ -6929,7 +6926,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B316" s="1">
         <f t="shared" si="9"/>
@@ -6945,7 +6942,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B317" s="1">
         <f t="shared" si="9"/>
@@ -6961,7 +6958,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B318" s="1">
         <f t="shared" si="9"/>
@@ -6977,7 +6974,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B319" s="1">
         <f t="shared" si="9"/>
@@ -6993,7 +6990,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B320" s="1">
         <f t="shared" si="9"/>
@@ -7009,7 +7006,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B321" s="1">
         <f t="shared" si="9"/>
@@ -7025,7 +7022,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B322" s="1">
         <f t="shared" ref="B322:B385" si="11">B321+1</f>
@@ -7041,7 +7038,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B323" s="1">
         <f t="shared" si="11"/>
@@ -7057,7 +7054,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B324" s="1">
         <f t="shared" si="11"/>
@@ -7073,7 +7070,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B325" s="1">
         <f t="shared" si="11"/>
@@ -7089,7 +7086,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B326" s="1">
         <f t="shared" si="11"/>
@@ -7105,7 +7102,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B327" s="1">
         <f t="shared" si="11"/>
@@ -7121,7 +7118,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B328" s="1">
         <f t="shared" si="11"/>
@@ -7137,7 +7134,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B329" s="1">
         <f t="shared" si="11"/>
@@ -7153,7 +7150,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B330" s="1">
         <f t="shared" si="11"/>
@@ -7169,7 +7166,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B331" s="1">
         <f t="shared" si="11"/>
@@ -7185,7 +7182,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B332" s="1">
         <f t="shared" si="11"/>
@@ -7201,7 +7198,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B333" s="1">
         <f t="shared" si="11"/>
@@ -7217,7 +7214,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B334" s="1">
         <f t="shared" si="11"/>
@@ -7233,7 +7230,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B335" s="1">
         <f t="shared" si="11"/>
@@ -7249,7 +7246,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B336" s="1">
         <f t="shared" si="11"/>
@@ -7265,7 +7262,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B337" s="1">
         <f t="shared" si="11"/>
@@ -7281,7 +7278,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B338" s="1">
         <f t="shared" si="11"/>
@@ -7297,7 +7294,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B339" s="1">
         <f t="shared" si="11"/>
@@ -7313,7 +7310,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B340" s="1">
         <f t="shared" si="11"/>
@@ -7329,7 +7326,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B341" s="1">
         <f t="shared" si="11"/>
@@ -7345,7 +7342,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B342" s="1">
         <f t="shared" si="11"/>
@@ -7361,7 +7358,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B343" s="1">
         <f t="shared" si="11"/>
@@ -7377,7 +7374,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B344" s="1">
         <f t="shared" si="11"/>
@@ -7393,7 +7390,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B345" s="1">
         <f t="shared" si="11"/>
@@ -7409,7 +7406,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B346" s="1">
         <f t="shared" si="11"/>
@@ -7425,7 +7422,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B347" s="1">
         <f t="shared" si="11"/>
@@ -7441,7 +7438,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B348" s="1">
         <f t="shared" si="11"/>
@@ -7457,7 +7454,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B349" s="1">
         <f t="shared" si="11"/>
@@ -7473,7 +7470,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B350" s="1">
         <f t="shared" si="11"/>
@@ -7489,7 +7486,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B351" s="1">
         <f t="shared" si="11"/>
@@ -7505,7 +7502,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B352" s="1">
         <f t="shared" si="11"/>
@@ -7521,7 +7518,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B353" s="1">
         <f t="shared" si="11"/>
@@ -7537,7 +7534,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B354" s="1">
         <f t="shared" si="11"/>
@@ -7553,7 +7550,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B355" s="1">
         <f t="shared" si="11"/>
@@ -7569,7 +7566,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B356" s="1">
         <f t="shared" si="11"/>
@@ -7585,7 +7582,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B357" s="1">
         <f t="shared" si="11"/>
@@ -7601,7 +7598,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B358" s="1">
         <f t="shared" si="11"/>
@@ -7617,7 +7614,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B359" s="1">
         <f t="shared" si="11"/>
@@ -7633,7 +7630,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B360" s="1">
         <f t="shared" si="11"/>
@@ -7649,7 +7646,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B361" s="1">
         <f t="shared" si="11"/>
@@ -7665,7 +7662,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B362" s="1">
         <f t="shared" si="11"/>
@@ -7681,7 +7678,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B363" s="1">
         <f t="shared" si="11"/>
@@ -7697,7 +7694,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B364" s="1">
         <f t="shared" si="11"/>
@@ -7713,7 +7710,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B365" s="1">
         <f t="shared" si="11"/>
@@ -7729,7 +7726,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B366" s="1">
         <f t="shared" si="11"/>
@@ -7745,7 +7742,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B367" s="1">
         <f t="shared" si="11"/>
@@ -7761,7 +7758,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B368" s="1">
         <f t="shared" si="11"/>
@@ -7777,7 +7774,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B369" s="1">
         <f t="shared" si="11"/>
@@ -7793,7 +7790,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B370" s="1">
         <f t="shared" si="11"/>
@@ -7809,7 +7806,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B371" s="1">
         <f t="shared" si="11"/>
@@ -7825,7 +7822,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B372" s="1">
         <f t="shared" si="11"/>
@@ -7841,7 +7838,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B373" s="1">
         <f t="shared" si="11"/>
@@ -7857,7 +7854,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B374" s="1">
         <f t="shared" si="11"/>
@@ -7873,7 +7870,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B375" s="1">
         <f t="shared" si="11"/>
@@ -7889,7 +7886,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B376" s="1">
         <f t="shared" si="11"/>
@@ -7905,7 +7902,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B377" s="1">
         <f t="shared" si="11"/>
@@ -7921,7 +7918,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B378" s="1">
         <f t="shared" si="11"/>
@@ -7937,7 +7934,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B379" s="1">
         <f t="shared" si="11"/>
@@ -7953,7 +7950,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B380" s="1">
         <f t="shared" si="11"/>
@@ -7969,7 +7966,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B381" s="1">
         <f t="shared" si="11"/>
@@ -7985,7 +7982,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B382" s="1">
         <f t="shared" si="11"/>
@@ -8001,7 +7998,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B383" s="1">
         <f t="shared" si="11"/>
@@ -8017,7 +8014,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B384" s="1">
         <f t="shared" si="11"/>
@@ -8033,7 +8030,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B385" s="1">
         <f t="shared" si="11"/>
@@ -8049,10 +8046,10 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B386" s="1">
-        <f t="shared" ref="B386:B449" si="13">B385+1</f>
+        <f t="shared" ref="B386:B448" si="13">B385+1</f>
         <v>384</v>
       </c>
       <c r="C386" t="s">
@@ -8065,7 +8062,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B387" s="1">
         <f t="shared" si="13"/>
@@ -8081,7 +8078,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B388" s="1">
         <f t="shared" si="13"/>
@@ -8097,7 +8094,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B389" s="1">
         <f t="shared" si="13"/>
@@ -8113,7 +8110,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B390" s="1">
         <f t="shared" si="13"/>
@@ -8129,7 +8126,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B391" s="1">
         <f t="shared" si="13"/>
@@ -8145,7 +8142,7 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B392" s="1">
         <f t="shared" si="13"/>
@@ -8161,7 +8158,7 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B393" s="1">
         <f t="shared" si="13"/>
@@ -8177,7 +8174,7 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B394" s="1">
         <f t="shared" si="13"/>
@@ -8193,7 +8190,7 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B395" s="1">
         <f t="shared" si="13"/>
@@ -8209,7 +8206,7 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B396" s="1">
         <f t="shared" si="13"/>
@@ -8225,7 +8222,7 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B397" s="1">
         <f t="shared" si="13"/>
@@ -8241,7 +8238,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B398" s="1">
         <f t="shared" si="13"/>
@@ -8257,7 +8254,7 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B399" s="1">
         <f t="shared" si="13"/>
@@ -8273,7 +8270,7 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B400" s="1">
         <f t="shared" si="13"/>
@@ -8289,7 +8286,7 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B401" s="1">
         <f t="shared" si="13"/>
@@ -8305,7 +8302,7 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B402" s="1">
         <f t="shared" si="13"/>
@@ -8321,7 +8318,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B403" s="1">
         <f t="shared" si="13"/>
@@ -8337,7 +8334,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B404" s="1">
         <f t="shared" si="13"/>
@@ -8353,7 +8350,7 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B405" s="1">
         <f t="shared" si="13"/>
@@ -8369,7 +8366,7 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B406" s="1">
         <f t="shared" si="13"/>
@@ -8385,7 +8382,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B407" s="1">
         <f t="shared" si="13"/>
@@ -8401,7 +8398,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B408" s="1">
         <f t="shared" si="13"/>
@@ -8417,7 +8414,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B409" s="1">
         <f t="shared" si="13"/>
@@ -8433,7 +8430,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B410" s="1">
         <f t="shared" si="13"/>
@@ -8449,7 +8446,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B411" s="1">
         <f t="shared" si="13"/>
@@ -8465,7 +8462,7 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B412" s="1">
         <f t="shared" si="13"/>
@@ -8481,7 +8478,7 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B413" s="1">
         <f t="shared" si="13"/>
@@ -8497,7 +8494,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B414" s="1">
         <f t="shared" si="13"/>
@@ -8513,7 +8510,7 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B415" s="1">
         <f t="shared" si="13"/>
@@ -8529,7 +8526,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B416" s="1">
         <f t="shared" si="13"/>
@@ -8545,7 +8542,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B417" s="1">
         <f t="shared" si="13"/>
@@ -8561,7 +8558,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B418" s="1">
         <f t="shared" si="13"/>
@@ -8577,7 +8574,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B419" s="1">
         <f t="shared" si="13"/>
@@ -8593,7 +8590,7 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B420" s="1">
         <f t="shared" si="13"/>
@@ -8609,7 +8606,7 @@
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B421" s="1">
         <f t="shared" si="13"/>
@@ -8625,7 +8622,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B422" s="1">
         <f t="shared" si="13"/>
@@ -8641,7 +8638,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B423" s="1">
         <f t="shared" si="13"/>
@@ -8657,7 +8654,7 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B424" s="1">
         <f t="shared" si="13"/>
@@ -8673,7 +8670,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B425" s="1">
         <f t="shared" si="13"/>
@@ -8689,7 +8686,7 @@
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B426" s="1">
         <f t="shared" si="13"/>
@@ -8705,7 +8702,7 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B427" s="1">
         <f t="shared" si="13"/>
@@ -8721,7 +8718,7 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B428" s="1">
         <f t="shared" si="13"/>
@@ -8737,7 +8734,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B429" s="1">
         <f t="shared" si="13"/>
@@ -8753,7 +8750,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B430" s="1">
         <f t="shared" si="13"/>
@@ -8769,7 +8766,7 @@
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B431" s="1">
         <f t="shared" si="13"/>
@@ -8785,7 +8782,7 @@
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B432" s="1">
         <f t="shared" si="13"/>
@@ -8801,7 +8798,7 @@
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B433" s="1">
         <f t="shared" si="13"/>
@@ -8817,7 +8814,7 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B434" s="1">
         <f t="shared" si="13"/>
@@ -8833,7 +8830,7 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B435" s="1">
         <f t="shared" si="13"/>
@@ -8849,7 +8846,7 @@
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B436" s="1">
         <f t="shared" si="13"/>
@@ -8865,7 +8862,7 @@
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B437" s="1">
         <f t="shared" si="13"/>
@@ -8881,7 +8878,7 @@
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B438" s="1">
         <f t="shared" si="13"/>
@@ -8897,7 +8894,7 @@
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B439" s="1">
         <f t="shared" si="13"/>
@@ -8913,7 +8910,7 @@
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B440" s="1">
         <f t="shared" si="13"/>
@@ -8929,7 +8926,7 @@
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B441" s="1">
         <f t="shared" si="13"/>
@@ -8945,7 +8942,7 @@
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B442" s="1">
         <f t="shared" si="13"/>
@@ -8961,7 +8958,7 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B443" s="1">
         <f t="shared" si="13"/>
@@ -8977,7 +8974,7 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B444" s="1">
         <f t="shared" si="13"/>
@@ -8993,7 +8990,7 @@
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B445" s="1">
         <f t="shared" si="13"/>
@@ -9009,7 +9006,7 @@
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B446" s="1">
         <f t="shared" si="13"/>
@@ -9025,7 +9022,7 @@
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B447" s="1">
         <f t="shared" si="13"/>
@@ -9035,13 +9032,13 @@
         <v>437</v>
       </c>
       <c r="D447" t="str">
-        <f t="shared" ref="D447:D458" si="14">"        "&amp;C447&amp;"="&amp;B447&amp;","</f>
+        <f t="shared" ref="D447:D457" si="14">"        "&amp;C447&amp;"="&amp;B447&amp;","</f>
         <v xml:space="preserve">        WRITE_ONLY=445,</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B448" s="1">
         <f t="shared" si="13"/>
@@ -9052,15 +9049,15 @@
       </c>
       <c r="D448" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        XML_DECLARATION=446,</v>
+        <v xml:space="preserve">        XML_SCHEMA=446,</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B449" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="B449:B457" si="15">B448+1</f>
         <v>447</v>
       </c>
       <c r="C449" t="s">
@@ -9068,29 +9065,26 @@
       </c>
       <c r="D449" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        XML_SCHEMA=447,</v>
+        <v xml:space="preserve">        YYYYDDD=447,</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B450" s="1">
-        <f t="shared" ref="B450:B458" si="15">B449+1</f>
+        <f t="shared" si="15"/>
         <v>448</v>
       </c>
       <c r="C450" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D450" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYDDD=448,</v>
+        <v xml:space="preserve">        YYYYMMDD=448,</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A451" t="s">
-        <v>442</v>
-      </c>
       <c r="B451" s="1">
         <f t="shared" si="15"/>
         <v>449</v>
@@ -9100,7 +9094,7 @@
       </c>
       <c r="D451" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYMMDD=449,</v>
+        <v xml:space="preserve">        TYPEDEF=449,</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.25">
@@ -9113,7 +9107,7 @@
       </c>
       <c r="D452" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        TYPEDEF=450,</v>
+        <v xml:space="preserve">        STRONG=450,</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.25">
@@ -9126,7 +9120,7 @@
       </c>
       <c r="D453" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRONG=451,</v>
+        <v xml:space="preserve">        UNSAFE=451,</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.25">
@@ -9135,11 +9129,11 @@
         <v>452</v>
       </c>
       <c r="C454" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D454" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        UNSAFE=452,</v>
+        <v xml:space="preserve">        PUBLIC=452,</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.25">
@@ -9152,7 +9146,7 @@
       </c>
       <c r="D455" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PUBLIC=453,</v>
+        <v xml:space="preserve">        PRIVATE=453,</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.25">
@@ -9161,11 +9155,11 @@
         <v>454</v>
       </c>
       <c r="C456" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="D456" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PRIVATE=454,</v>
+        <v xml:space="preserve">        IN_OUT=454,</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.25">
@@ -9178,33 +9172,33 @@
       </c>
       <c r="D457" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        IN_OUT=455,</v>
+        <v xml:space="preserve">        STRICT=455,</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B458" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B458:B461" si="16">B457+1</f>
         <v>456</v>
       </c>
       <c r="C458" t="s">
         <v>475</v>
       </c>
       <c r="D458" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRICT=456,</v>
+        <f t="shared" ref="D458:D461" si="17">"        "&amp;C458&amp;"="&amp;B458&amp;","</f>
+        <v xml:space="preserve">        QuestionMark=456,</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B459" s="1">
-        <f t="shared" ref="B459:B462" si="16">B458+1</f>
+        <f t="shared" si="16"/>
         <v>457</v>
       </c>
       <c r="C459" t="s">
         <v>476</v>
       </c>
       <c r="D459" t="str">
-        <f t="shared" ref="D459:D462" si="17">"        "&amp;C459&amp;"="&amp;B459&amp;","</f>
-        <v xml:space="preserve">        QuestionMark=457,</v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">        CompilerDirective=457,</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.25">
@@ -9217,7 +9211,7 @@
       </c>
       <c r="D460" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CompilerDirective=458,</v>
+        <v xml:space="preserve">        CopyImportDirective=458,</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.25">
@@ -9230,42 +9224,29 @@
       </c>
       <c r="D461" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CopyImportDirective=459,</v>
+        <v xml:space="preserve">        ReplaceDirective=459,</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B462" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="B462" si="18">B461+1</f>
         <v>460</v>
       </c>
       <c r="C462" t="s">
         <v>479</v>
       </c>
       <c r="D462" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        ReplaceDirective=460,</v>
-      </c>
-    </row>
-    <row r="463" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B463" s="1">
-        <f t="shared" ref="B463" si="18">B462+1</f>
-        <v>461</v>
-      </c>
-      <c r="C463" t="s">
-        <v>480</v>
-      </c>
-      <c r="D463" t="str">
-        <f t="shared" ref="D463" si="19">"        "&amp;C463&amp;"="&amp;B463&amp;","</f>
-        <v xml:space="preserve">        ContinuationTokenGroup=461,</v>
+        <f t="shared" ref="D462" si="19">"        "&amp;C462&amp;"="&amp;B462&amp;","</f>
+        <v xml:space="preserve">        ContinuationTokenGroup=460,</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#578, remove PARSE Token, add predicate for Xml Parse Context
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="474">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1062,9 +1062,6 @@
   </si>
   <si>
     <t>PAGE</t>
-  </si>
-  <si>
-    <t>PARSE</t>
   </si>
   <si>
     <t>PASSWORD</t>
@@ -1860,10 +1857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D457"/>
+  <dimension ref="A1:D456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="A280" sqref="A280"/>
+    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="E358" sqref="E358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1875,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B1" s="1">
         <v>-1</v>
@@ -1893,14 +1890,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B2" s="1">
         <f>B1+1</f>
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D2" t="str">
         <f>"        "&amp;C2&amp;"="&amp;B2&amp;","</f>
@@ -1909,7 +1906,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B3" s="1">
         <f>B2+1</f>
@@ -1925,7 +1922,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B67" si="1">B3+1</f>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="1"/>
@@ -1957,7 +1954,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="1"/>
@@ -1973,7 +1970,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="1"/>
@@ -1989,7 +1986,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="1"/>
@@ -2005,7 +2002,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="1"/>
@@ -2021,14 +2018,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2037,7 +2034,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="1"/>
@@ -2053,7 +2050,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="1"/>
@@ -2069,7 +2066,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="1"/>
@@ -2085,7 +2082,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
@@ -2101,7 +2098,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
@@ -2117,7 +2114,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
@@ -2133,7 +2130,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
@@ -2149,7 +2146,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
@@ -2165,7 +2162,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
@@ -2181,7 +2178,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="1"/>
@@ -2197,7 +2194,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="1"/>
@@ -2213,7 +2210,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="1"/>
@@ -2229,7 +2226,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="1"/>
@@ -2245,7 +2242,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="1"/>
@@ -2261,7 +2258,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="1"/>
@@ -2277,7 +2274,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="1"/>
@@ -2293,7 +2290,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="1"/>
@@ -2309,7 +2306,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="1"/>
@@ -2338,14 +2335,14 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2354,7 +2351,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" si="1"/>
@@ -2370,7 +2367,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="1"/>
@@ -2386,7 +2383,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" si="1"/>
@@ -2402,7 +2399,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" si="1"/>
@@ -2418,7 +2415,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" si="1"/>
@@ -2447,14 +2444,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2463,14 +2460,14 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2479,7 +2476,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="1"/>
@@ -2495,14 +2492,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2511,7 +2508,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="1"/>
@@ -2527,7 +2524,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" si="1"/>
@@ -2543,7 +2540,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" si="1"/>
@@ -2559,7 +2556,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="1"/>
@@ -2575,7 +2572,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" si="1"/>
@@ -2591,7 +2588,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" si="1"/>
@@ -2607,7 +2604,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" si="1"/>
@@ -2623,7 +2620,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" si="1"/>
@@ -2639,7 +2636,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B49" s="1">
         <f t="shared" si="1"/>
@@ -2655,7 +2652,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" si="1"/>
@@ -2671,7 +2668,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B51" s="1">
         <f t="shared" si="1"/>
@@ -2687,7 +2684,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" si="1"/>
@@ -2703,7 +2700,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B53" s="1">
         <f t="shared" si="1"/>
@@ -2719,7 +2716,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B54" s="1">
         <f t="shared" si="1"/>
@@ -2735,7 +2732,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B55" s="1">
         <f t="shared" si="1"/>
@@ -2751,14 +2748,14 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2767,7 +2764,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B57" s="1">
         <f t="shared" si="1"/>
@@ -2783,7 +2780,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B58" s="1">
         <f t="shared" si="1"/>
@@ -2799,7 +2796,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B59" s="1">
         <f t="shared" si="1"/>
@@ -2815,7 +2812,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B60" s="1">
         <f t="shared" si="1"/>
@@ -2831,7 +2828,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B61" s="1">
         <f t="shared" si="1"/>
@@ -2847,7 +2844,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B62" s="1">
         <f t="shared" si="1"/>
@@ -2863,7 +2860,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B63" s="1">
         <f t="shared" si="1"/>
@@ -2879,7 +2876,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B64" s="1">
         <f t="shared" si="1"/>
@@ -2895,7 +2892,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B65" s="1">
         <f t="shared" si="1"/>
@@ -2911,7 +2908,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B66" s="1">
         <f t="shared" si="1"/>
@@ -2927,7 +2924,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B67" s="1">
         <f t="shared" si="1"/>
@@ -2943,7 +2940,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B68" s="1">
         <f t="shared" ref="B68:B131" si="3">B67+1</f>
@@ -2959,7 +2956,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
@@ -2975,7 +2972,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
@@ -2991,7 +2988,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
@@ -3007,7 +3004,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
@@ -3023,14 +3020,14 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -3039,7 +3036,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
@@ -3055,7 +3052,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
@@ -3071,7 +3068,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
@@ -3087,7 +3084,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
@@ -3103,7 +3100,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
@@ -3119,7 +3116,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
@@ -3135,7 +3132,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B80" s="1">
         <f t="shared" si="3"/>
@@ -3151,7 +3148,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B81" s="1">
         <f t="shared" si="3"/>
@@ -3167,14 +3164,14 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B82" s="1">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3183,7 +3180,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B83" s="1">
         <f t="shared" si="3"/>
@@ -3199,7 +3196,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B84" s="1">
         <f t="shared" si="3"/>
@@ -3215,7 +3212,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B85" s="1">
         <f t="shared" si="3"/>
@@ -3231,7 +3228,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B86" s="1">
         <f t="shared" si="3"/>
@@ -3247,7 +3244,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B87" s="1">
         <f t="shared" si="3"/>
@@ -3263,7 +3260,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B88" s="1">
         <f t="shared" si="3"/>
@@ -3279,7 +3276,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B89" s="1">
         <f t="shared" si="3"/>
@@ -3295,7 +3292,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B90" s="1">
         <f t="shared" si="3"/>
@@ -3311,7 +3308,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B91" s="1">
         <f t="shared" si="3"/>
@@ -3327,7 +3324,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B92" s="1">
         <f t="shared" si="3"/>
@@ -3343,7 +3340,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B93" s="1">
         <f t="shared" si="3"/>
@@ -3359,7 +3356,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B94" s="1">
         <f t="shared" si="3"/>
@@ -3375,7 +3372,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B95" s="1">
         <f t="shared" si="3"/>
@@ -3391,7 +3388,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B96" s="1">
         <f t="shared" si="3"/>
@@ -3407,7 +3404,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B97" s="1">
         <f t="shared" si="3"/>
@@ -3423,7 +3420,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B98" s="1">
         <f t="shared" si="3"/>
@@ -3439,7 +3436,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B99" s="1">
         <f t="shared" si="3"/>
@@ -3455,7 +3452,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B100" s="1">
         <f t="shared" si="3"/>
@@ -3471,7 +3468,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B101" s="1">
         <f t="shared" si="3"/>
@@ -3487,7 +3484,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B102" s="1">
         <f t="shared" si="3"/>
@@ -3503,7 +3500,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B103" s="1">
         <f t="shared" si="3"/>
@@ -3519,7 +3516,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B104" s="1">
         <f t="shared" si="3"/>
@@ -3535,7 +3532,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B105" s="1">
         <f t="shared" si="3"/>
@@ -3551,7 +3548,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B106" s="1">
         <f t="shared" si="3"/>
@@ -3567,7 +3564,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B107" s="1">
         <f t="shared" si="3"/>
@@ -3583,7 +3580,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B108" s="1">
         <f t="shared" si="3"/>
@@ -3599,7 +3596,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B109" s="1">
         <f t="shared" si="3"/>
@@ -3615,7 +3612,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B110" s="1">
         <f t="shared" si="3"/>
@@ -3631,7 +3628,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B111" s="1">
         <f t="shared" si="3"/>
@@ -3647,7 +3644,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B112" s="1">
         <f t="shared" si="3"/>
@@ -3663,7 +3660,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B113" s="1">
         <f t="shared" si="3"/>
@@ -3679,7 +3676,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B114" s="1">
         <f t="shared" si="3"/>
@@ -3695,7 +3692,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B115" s="1">
         <f t="shared" si="3"/>
@@ -3711,7 +3708,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B116" s="1">
         <f t="shared" si="3"/>
@@ -3727,7 +3724,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B117" s="1">
         <f t="shared" si="3"/>
@@ -3743,7 +3740,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B118" s="1">
         <f t="shared" si="3"/>
@@ -3759,7 +3756,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B119" s="1">
         <f t="shared" si="3"/>
@@ -3775,7 +3772,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B120" s="1">
         <f t="shared" si="3"/>
@@ -3791,7 +3788,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B121" s="1">
         <f t="shared" si="3"/>
@@ -3807,7 +3804,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B122" s="1">
         <f t="shared" si="3"/>
@@ -3823,7 +3820,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B123" s="1">
         <f t="shared" si="3"/>
@@ -3839,7 +3836,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B124" s="1">
         <f t="shared" si="3"/>
@@ -3855,7 +3852,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B125" s="1">
         <f t="shared" si="3"/>
@@ -3871,7 +3868,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B126" s="1">
         <f t="shared" si="3"/>
@@ -3887,7 +3884,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B127" s="1">
         <f t="shared" si="3"/>
@@ -3903,7 +3900,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B128" s="1">
         <f t="shared" si="3"/>
@@ -3919,7 +3916,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B129" s="1">
         <f t="shared" si="3"/>
@@ -3935,14 +3932,14 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B130" s="1">
         <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="C130" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D130" t="str">
         <f t="shared" ref="D130:D193" si="4">"        "&amp;C130&amp;"="&amp;B130&amp;","</f>
@@ -3951,7 +3948,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B131" s="1">
         <f t="shared" si="3"/>
@@ -3967,7 +3964,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B132" s="1">
         <f t="shared" ref="B132:B195" si="5">B131+1</f>
@@ -3983,7 +3980,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B133" s="1">
         <f t="shared" si="5"/>
@@ -3999,7 +3996,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B134" s="1">
         <f t="shared" si="5"/>
@@ -4015,7 +4012,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B135" s="1">
         <f t="shared" si="5"/>
@@ -4031,7 +4028,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B136" s="1">
         <f t="shared" si="5"/>
@@ -4047,7 +4044,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B137" s="1">
         <f t="shared" si="5"/>
@@ -4063,7 +4060,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B138" s="1">
         <f t="shared" si="5"/>
@@ -4079,7 +4076,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B139" s="1">
         <f t="shared" si="5"/>
@@ -4095,7 +4092,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B140" s="1">
         <f t="shared" si="5"/>
@@ -4111,7 +4108,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B141" s="1">
         <f t="shared" si="5"/>
@@ -4127,7 +4124,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B142" s="1">
         <f t="shared" si="5"/>
@@ -4143,7 +4140,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B143" s="1">
         <f t="shared" si="5"/>
@@ -4159,7 +4156,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B144" s="1">
         <f t="shared" si="5"/>
@@ -4175,7 +4172,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B145" s="1">
         <f t="shared" si="5"/>
@@ -4191,7 +4188,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B146" s="1">
         <f t="shared" si="5"/>
@@ -4207,7 +4204,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B147" s="1">
         <f t="shared" si="5"/>
@@ -4223,7 +4220,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B148" s="1">
         <f t="shared" si="5"/>
@@ -4239,7 +4236,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B149" s="1">
         <f t="shared" si="5"/>
@@ -4255,7 +4252,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B150" s="1">
         <f t="shared" si="5"/>
@@ -4271,7 +4268,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B151" s="1">
         <f t="shared" si="5"/>
@@ -4287,14 +4284,14 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B152" s="1">
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="C152" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="4"/>
@@ -4303,7 +4300,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B153" s="1">
         <f t="shared" si="5"/>
@@ -4319,7 +4316,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B154" s="1">
         <f t="shared" si="5"/>
@@ -4335,7 +4332,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B155" s="1">
         <f t="shared" si="5"/>
@@ -4351,7 +4348,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B156" s="1">
         <f t="shared" si="5"/>
@@ -4367,7 +4364,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B157" s="1">
         <f t="shared" si="5"/>
@@ -4383,7 +4380,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B158" s="1">
         <f t="shared" si="5"/>
@@ -4399,7 +4396,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B159" s="1">
         <f t="shared" si="5"/>
@@ -4415,7 +4412,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B160" s="1">
         <f t="shared" si="5"/>
@@ -4431,7 +4428,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B161" s="1">
         <f t="shared" si="5"/>
@@ -4447,7 +4444,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B162" s="1">
         <f t="shared" si="5"/>
@@ -4463,7 +4460,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B163" s="1">
         <f t="shared" si="5"/>
@@ -4479,7 +4476,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B164" s="1">
         <f t="shared" si="5"/>
@@ -4495,7 +4492,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B165" s="1">
         <f t="shared" si="5"/>
@@ -4511,7 +4508,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B166" s="1">
         <f t="shared" si="5"/>
@@ -4527,7 +4524,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B167" s="1">
         <f t="shared" si="5"/>
@@ -4543,7 +4540,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B168" s="1">
         <f t="shared" si="5"/>
@@ -4559,7 +4556,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B169" s="1">
         <f t="shared" si="5"/>
@@ -4575,7 +4572,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B170" s="1">
         <f t="shared" si="5"/>
@@ -4591,7 +4588,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B171" s="1">
         <f t="shared" si="5"/>
@@ -4607,7 +4604,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B172" s="1">
         <f t="shared" si="5"/>
@@ -4623,7 +4620,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B173" s="1">
         <f t="shared" si="5"/>
@@ -4639,7 +4636,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B174" s="1">
         <f t="shared" si="5"/>
@@ -4655,7 +4652,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B175" s="1">
         <f t="shared" si="5"/>
@@ -4671,7 +4668,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B176" s="1">
         <f t="shared" si="5"/>
@@ -4687,7 +4684,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B177" s="1">
         <f t="shared" si="5"/>
@@ -4703,7 +4700,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B178" s="1">
         <f t="shared" si="5"/>
@@ -4719,7 +4716,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B179" s="1">
         <f t="shared" si="5"/>
@@ -4735,7 +4732,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B180" s="1">
         <f t="shared" si="5"/>
@@ -4751,7 +4748,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B181" s="1">
         <f t="shared" si="5"/>
@@ -4767,7 +4764,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B182" s="1">
         <f t="shared" si="5"/>
@@ -4783,7 +4780,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B183" s="1">
         <f>B182+1</f>
@@ -4799,7 +4796,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B184" s="1">
         <f t="shared" si="5"/>
@@ -4815,7 +4812,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B185" s="1">
         <f t="shared" si="5"/>
@@ -4831,7 +4828,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B186" s="1">
         <f t="shared" si="5"/>
@@ -4847,7 +4844,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B187" s="1">
         <f t="shared" si="5"/>
@@ -4863,7 +4860,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B188" s="1">
         <f t="shared" si="5"/>
@@ -4879,7 +4876,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B189" s="1">
         <f t="shared" si="5"/>
@@ -4895,7 +4892,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B190" s="1">
         <f t="shared" si="5"/>
@@ -4911,7 +4908,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B191" s="1">
         <f t="shared" si="5"/>
@@ -4927,7 +4924,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B192" s="1">
         <f t="shared" si="5"/>
@@ -4943,7 +4940,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B193" s="1">
         <f t="shared" si="5"/>
@@ -4959,7 +4956,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B194" s="1">
         <f t="shared" si="5"/>
@@ -4975,7 +4972,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B195" s="1">
         <f t="shared" si="5"/>
@@ -4991,7 +4988,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B196" s="1">
         <f t="shared" ref="B196:B257" si="7">B195+1</f>
@@ -5007,7 +5004,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B197" s="1">
         <f t="shared" si="7"/>
@@ -5023,7 +5020,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B198" s="1">
         <f t="shared" si="7"/>
@@ -5039,7 +5036,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B199" s="1">
         <f t="shared" si="7"/>
@@ -5055,7 +5052,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B200" s="1">
         <f t="shared" si="7"/>
@@ -5071,7 +5068,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B201" s="1">
         <f t="shared" si="7"/>
@@ -5087,7 +5084,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B202" s="1">
         <f t="shared" si="7"/>
@@ -5103,7 +5100,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B203" s="1">
         <f t="shared" si="7"/>
@@ -5119,7 +5116,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B204" s="1">
         <f t="shared" si="7"/>
@@ -5135,7 +5132,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B205" s="1">
         <f t="shared" si="7"/>
@@ -5151,7 +5148,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B206" s="1">
         <f t="shared" si="7"/>
@@ -5167,7 +5164,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B207" s="1">
         <f t="shared" si="7"/>
@@ -5183,7 +5180,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B208" s="1">
         <f t="shared" si="7"/>
@@ -5199,7 +5196,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B209" s="1">
         <f t="shared" si="7"/>
@@ -5215,7 +5212,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B210" s="1">
         <f t="shared" si="7"/>
@@ -5231,7 +5228,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B211" s="1">
         <f t="shared" si="7"/>
@@ -5247,7 +5244,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B212" s="1">
         <f t="shared" si="7"/>
@@ -5263,7 +5260,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B213" s="1">
         <f t="shared" si="7"/>
@@ -5279,7 +5276,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B214" s="1">
         <f t="shared" si="7"/>
@@ -5295,7 +5292,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B215" s="1">
         <f t="shared" si="7"/>
@@ -5311,7 +5308,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B216" s="1">
         <f t="shared" si="7"/>
@@ -5327,7 +5324,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B217" s="1">
         <f t="shared" si="7"/>
@@ -5343,7 +5340,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B218" s="1">
         <f t="shared" si="7"/>
@@ -5359,7 +5356,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B219" s="1">
         <f t="shared" si="7"/>
@@ -5375,7 +5372,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B220" s="1">
         <f t="shared" si="7"/>
@@ -5391,7 +5388,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B221" s="1">
         <f t="shared" si="7"/>
@@ -5407,7 +5404,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B222" s="1">
         <f t="shared" si="7"/>
@@ -5423,7 +5420,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B223" s="1">
         <f t="shared" si="7"/>
@@ -5439,7 +5436,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B224" s="1">
         <f t="shared" si="7"/>
@@ -5455,7 +5452,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B225" s="1">
         <f t="shared" si="7"/>
@@ -5471,7 +5468,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B226" s="1">
         <f t="shared" si="7"/>
@@ -5487,7 +5484,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B227" s="1">
         <f t="shared" si="7"/>
@@ -5503,7 +5500,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B228" s="1">
         <f t="shared" si="7"/>
@@ -5519,7 +5516,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B229" s="1">
         <f t="shared" si="7"/>
@@ -5535,7 +5532,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B230" s="1">
         <f t="shared" si="7"/>
@@ -5551,7 +5548,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B231" s="1">
         <f t="shared" si="7"/>
@@ -5567,7 +5564,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B232" s="1">
         <f t="shared" si="7"/>
@@ -5583,7 +5580,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B233" s="1">
         <f t="shared" si="7"/>
@@ -5599,7 +5596,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B234" s="1">
         <f t="shared" si="7"/>
@@ -5615,7 +5612,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B235" s="1">
         <f t="shared" si="7"/>
@@ -5631,7 +5628,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B236" s="1">
         <f t="shared" si="7"/>
@@ -5647,7 +5644,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B237" s="1">
         <f t="shared" si="7"/>
@@ -5663,7 +5660,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B238" s="1">
         <f t="shared" si="7"/>
@@ -5679,7 +5676,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B239" s="1">
         <f t="shared" si="7"/>
@@ -5695,7 +5692,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B240" s="1">
         <f t="shared" si="7"/>
@@ -5711,7 +5708,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B241" s="1">
         <f t="shared" si="7"/>
@@ -5727,7 +5724,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B242" s="1">
         <f t="shared" si="7"/>
@@ -5743,7 +5740,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B243" s="1">
         <f t="shared" si="7"/>
@@ -5759,7 +5756,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B244" s="1">
         <f t="shared" si="7"/>
@@ -5775,7 +5772,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B245" s="1">
         <f t="shared" si="7"/>
@@ -5791,7 +5788,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B246" s="1">
         <f t="shared" si="7"/>
@@ -5807,7 +5804,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B247" s="1">
         <f t="shared" si="7"/>
@@ -5823,7 +5820,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B248" s="1">
         <f t="shared" si="7"/>
@@ -5839,7 +5836,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B249" s="1">
         <f t="shared" si="7"/>
@@ -5855,7 +5852,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B250" s="1">
         <f t="shared" si="7"/>
@@ -5871,7 +5868,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B251" s="1">
         <f t="shared" si="7"/>
@@ -5887,7 +5884,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B252" s="1">
         <f t="shared" si="7"/>
@@ -5903,7 +5900,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B253" s="1">
         <f t="shared" si="7"/>
@@ -5919,7 +5916,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B254" s="1">
         <f t="shared" si="7"/>
@@ -5935,7 +5932,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B255" s="1">
         <f t="shared" si="7"/>
@@ -5951,7 +5948,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B256" s="1">
         <f t="shared" si="7"/>
@@ -5967,7 +5964,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B257" s="1">
         <f t="shared" si="7"/>
@@ -5983,7 +5980,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B258" s="1">
         <f t="shared" ref="B258:B319" si="9">B257+1</f>
@@ -5999,7 +5996,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B259" s="1">
         <f t="shared" si="9"/>
@@ -6015,7 +6012,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B260" s="1">
         <f t="shared" si="9"/>
@@ -6031,7 +6028,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B261" s="1">
         <f t="shared" si="9"/>
@@ -6047,7 +6044,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B262" s="1">
         <f t="shared" si="9"/>
@@ -6063,7 +6060,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B263" s="1">
         <f t="shared" si="9"/>
@@ -6079,7 +6076,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B264" s="1">
         <f t="shared" si="9"/>
@@ -6095,7 +6092,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B265" s="1">
         <f t="shared" si="9"/>
@@ -6111,7 +6108,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B266" s="1">
         <f t="shared" si="9"/>
@@ -6127,7 +6124,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B267" s="1">
         <f t="shared" si="9"/>
@@ -6143,7 +6140,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B268" s="1">
         <f t="shared" si="9"/>
@@ -6159,7 +6156,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B269" s="1">
         <f t="shared" si="9"/>
@@ -6175,7 +6172,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B270" s="1">
         <f t="shared" si="9"/>
@@ -6191,7 +6188,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B271" s="1">
         <f t="shared" si="9"/>
@@ -6207,7 +6204,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B272" s="1">
         <f t="shared" si="9"/>
@@ -6223,7 +6220,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B273" s="1">
         <f t="shared" si="9"/>
@@ -6239,7 +6236,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B274" s="1">
         <f t="shared" si="9"/>
@@ -6255,7 +6252,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B275" s="1">
         <f t="shared" si="9"/>
@@ -6271,7 +6268,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B276" s="1">
         <f t="shared" si="9"/>
@@ -6287,7 +6284,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B277" s="1">
         <f t="shared" si="9"/>
@@ -6303,7 +6300,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B278" s="1">
         <f t="shared" si="9"/>
@@ -6319,7 +6316,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B279" s="1">
         <f t="shared" si="9"/>
@@ -6335,7 +6332,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B280" s="1">
         <f t="shared" si="9"/>
@@ -6351,7 +6348,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B281" s="1">
         <f t="shared" si="9"/>
@@ -6367,7 +6364,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B282" s="1">
         <f t="shared" si="9"/>
@@ -6383,7 +6380,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B283" s="1">
         <f t="shared" si="9"/>
@@ -6399,7 +6396,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B284" s="1">
         <f t="shared" si="9"/>
@@ -6415,7 +6412,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B285" s="1">
         <f t="shared" si="9"/>
@@ -6431,7 +6428,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B286" s="1">
         <f t="shared" si="9"/>
@@ -6447,7 +6444,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B287" s="1">
         <f t="shared" si="9"/>
@@ -6463,7 +6460,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B288" s="1">
         <f t="shared" si="9"/>
@@ -6479,7 +6476,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B289" s="1">
         <f t="shared" si="9"/>
@@ -6495,7 +6492,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B290" s="1">
         <f t="shared" si="9"/>
@@ -6511,7 +6508,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B291" s="1">
         <f t="shared" si="9"/>
@@ -6527,7 +6524,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B292" s="1">
         <f t="shared" si="9"/>
@@ -6543,7 +6540,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B293" s="1">
         <f t="shared" si="9"/>
@@ -6559,7 +6556,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B294" s="1">
         <f t="shared" si="9"/>
@@ -6575,7 +6572,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B295" s="1">
         <f t="shared" si="9"/>
@@ -6591,7 +6588,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B296" s="1">
         <f t="shared" si="9"/>
@@ -6607,7 +6604,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B297" s="1">
         <f t="shared" si="9"/>
@@ -6623,7 +6620,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B298" s="1">
         <f t="shared" si="9"/>
@@ -6639,7 +6636,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B299" s="1">
         <f t="shared" si="9"/>
@@ -6655,7 +6652,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B300" s="1">
         <f t="shared" si="9"/>
@@ -6671,7 +6668,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B301" s="1">
         <f t="shared" si="9"/>
@@ -6687,7 +6684,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B302" s="1">
         <f t="shared" si="9"/>
@@ -6703,7 +6700,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B303" s="1">
         <f t="shared" si="9"/>
@@ -6719,7 +6716,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B304" s="1">
         <f t="shared" si="9"/>
@@ -6735,7 +6732,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B305" s="1">
         <f t="shared" si="9"/>
@@ -6751,7 +6748,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B306" s="1">
         <f t="shared" si="9"/>
@@ -6767,7 +6764,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B307" s="1">
         <f t="shared" si="9"/>
@@ -6783,7 +6780,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B308" s="1">
         <f t="shared" si="9"/>
@@ -6799,7 +6796,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B309" s="1">
         <f t="shared" si="9"/>
@@ -6815,7 +6812,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B310" s="1">
         <f t="shared" si="9"/>
@@ -6831,7 +6828,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B311" s="1">
         <f t="shared" si="9"/>
@@ -6847,7 +6844,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B312" s="1">
         <f t="shared" si="9"/>
@@ -6863,7 +6860,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B313" s="1">
         <f t="shared" si="9"/>
@@ -6879,7 +6876,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B314" s="1">
         <f t="shared" si="9"/>
@@ -6895,7 +6892,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B315" s="1">
         <f t="shared" si="9"/>
@@ -6911,7 +6908,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B316" s="1">
         <f t="shared" si="9"/>
@@ -6927,7 +6924,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B317" s="1">
         <f t="shared" si="9"/>
@@ -6937,13 +6934,13 @@
         <v>304</v>
       </c>
       <c r="D317" t="str">
-        <f t="shared" ref="D317:D377" si="10">"        "&amp;C317&amp;"="&amp;B317&amp;","</f>
+        <f t="shared" ref="D317:D376" si="10">"        "&amp;C317&amp;"="&amp;B317&amp;","</f>
         <v xml:space="preserve">        LABEL=315,</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B318" s="1">
         <f t="shared" si="9"/>
@@ -6959,7 +6956,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B319" s="1">
         <f t="shared" si="9"/>
@@ -6975,10 +6972,10 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B320" s="1">
-        <f t="shared" ref="B320:B380" si="11">B319+1</f>
+        <f t="shared" ref="B320:B379" si="11">B319+1</f>
         <v>318</v>
       </c>
       <c r="C320" t="s">
@@ -6991,7 +6988,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B321" s="1">
         <f t="shared" si="11"/>
@@ -7007,7 +7004,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B322" s="1">
         <f t="shared" si="11"/>
@@ -7023,7 +7020,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B323" s="1">
         <f t="shared" si="11"/>
@@ -7039,7 +7036,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B324" s="1">
         <f t="shared" si="11"/>
@@ -7055,7 +7052,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B325" s="1">
         <f t="shared" si="11"/>
@@ -7071,7 +7068,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B326" s="1">
         <f t="shared" si="11"/>
@@ -7087,7 +7084,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B327" s="1">
         <f t="shared" si="11"/>
@@ -7103,7 +7100,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B328" s="1">
         <f t="shared" si="11"/>
@@ -7119,7 +7116,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B329" s="1">
         <f t="shared" si="11"/>
@@ -7135,7 +7132,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B330" s="1">
         <f t="shared" si="11"/>
@@ -7151,7 +7148,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B331" s="1">
         <f t="shared" si="11"/>
@@ -7167,7 +7164,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B332" s="1">
         <f t="shared" si="11"/>
@@ -7183,7 +7180,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B333" s="1">
         <f t="shared" si="11"/>
@@ -7199,7 +7196,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B334" s="1">
         <f t="shared" si="11"/>
@@ -7215,7 +7212,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B335" s="1">
         <f t="shared" si="11"/>
@@ -7231,7 +7228,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B336" s="1">
         <f t="shared" si="11"/>
@@ -7247,7 +7244,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B337" s="1">
         <f t="shared" si="11"/>
@@ -7263,7 +7260,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B338" s="1">
         <f t="shared" si="11"/>
@@ -7279,7 +7276,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B339" s="1">
         <f t="shared" si="11"/>
@@ -7295,7 +7292,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B340" s="1">
         <f t="shared" si="11"/>
@@ -7311,7 +7308,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B341" s="1">
         <f t="shared" si="11"/>
@@ -7327,7 +7324,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B342" s="1">
         <f t="shared" si="11"/>
@@ -7343,7 +7340,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B343" s="1">
         <f t="shared" si="11"/>
@@ -7359,7 +7356,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B344" s="1">
         <f t="shared" si="11"/>
@@ -7375,7 +7372,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B345" s="1">
         <f t="shared" si="11"/>
@@ -7391,7 +7388,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B346" s="1">
         <f t="shared" si="11"/>
@@ -7407,7 +7404,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B347" s="1">
         <f t="shared" si="11"/>
@@ -7423,7 +7420,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B348" s="1">
         <f t="shared" si="11"/>
@@ -7439,7 +7436,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B349" s="1">
         <f t="shared" si="11"/>
@@ -7455,7 +7452,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B350" s="1">
         <f t="shared" si="11"/>
@@ -7471,7 +7468,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B351" s="1">
         <f t="shared" si="11"/>
@@ -7487,7 +7484,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B352" s="1">
         <f t="shared" si="11"/>
@@ -7503,7 +7500,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B353" s="1">
         <f t="shared" si="11"/>
@@ -7519,7 +7516,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B354" s="1">
         <f t="shared" si="11"/>
@@ -7535,7 +7532,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B355" s="1">
         <f t="shared" si="11"/>
@@ -7551,7 +7548,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B356" s="1">
         <f t="shared" si="11"/>
@@ -7567,7 +7564,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B357" s="1">
         <f t="shared" si="11"/>
@@ -7583,7 +7580,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B358" s="1">
         <f t="shared" si="11"/>
@@ -7594,12 +7591,12 @@
       </c>
       <c r="D358" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PARSE=356,</v>
+        <v xml:space="preserve">        PASSWORD=356,</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B359" s="1">
         <f t="shared" si="11"/>
@@ -7610,12 +7607,12 @@
       </c>
       <c r="D359" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PASSWORD=357,</v>
+        <v xml:space="preserve">        PIC=357,</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B360" s="1">
         <f t="shared" si="11"/>
@@ -7626,12 +7623,12 @@
       </c>
       <c r="D360" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PIC=358,</v>
+        <v xml:space="preserve">        PICTURE=358,</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B361" s="1">
         <f t="shared" si="11"/>
@@ -7642,12 +7639,12 @@
       </c>
       <c r="D361" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PICTURE=359,</v>
+        <v xml:space="preserve">        POINTER=359,</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B362" s="1">
         <f t="shared" si="11"/>
@@ -7658,12 +7655,12 @@
       </c>
       <c r="D362" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        POINTER=360,</v>
+        <v xml:space="preserve">        POSITION=360,</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B363" s="1">
         <f t="shared" si="11"/>
@@ -7674,28 +7671,28 @@
       </c>
       <c r="D363" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        POSITION=361,</v>
+        <v xml:space="preserve">        POSITIVE=361,</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B364" s="1">
         <f t="shared" si="11"/>
         <v>362</v>
       </c>
       <c r="C364" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D364" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        POSITIVE=362,</v>
+        <v xml:space="preserve">        PROCEDURE_POINTER=362,</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B365" s="1">
         <f t="shared" si="11"/>
@@ -7706,12 +7703,12 @@
       </c>
       <c r="D365" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCEDURE_POINTER=363,</v>
+        <v xml:space="preserve">        PROCEDURES=363,</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B366" s="1">
         <f t="shared" si="11"/>
@@ -7722,12 +7719,12 @@
       </c>
       <c r="D366" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCEDURES=364,</v>
+        <v xml:space="preserve">        PROCEED=364,</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B367" s="1">
         <f t="shared" si="11"/>
@@ -7738,12 +7735,12 @@
       </c>
       <c r="D367" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCEED=365,</v>
+        <v xml:space="preserve">        PROCESSING=365,</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B368" s="1">
         <f t="shared" si="11"/>
@@ -7754,12 +7751,12 @@
       </c>
       <c r="D368" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCESSING=366,</v>
+        <v xml:space="preserve">        PROGRAM=366,</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B369" s="1">
         <f t="shared" si="11"/>
@@ -7770,12 +7767,12 @@
       </c>
       <c r="D369" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROGRAM=367,</v>
+        <v xml:space="preserve">        PROGRAM_ID=367,</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B370" s="1">
         <f t="shared" si="11"/>
@@ -7786,12 +7783,12 @@
       </c>
       <c r="D370" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROGRAM_ID=368,</v>
+        <v xml:space="preserve">        RANDOM=368,</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B371" s="1">
         <f t="shared" si="11"/>
@@ -7802,12 +7799,12 @@
       </c>
       <c r="D371" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RANDOM=369,</v>
+        <v xml:space="preserve">        RECORD=369,</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B372" s="1">
         <f t="shared" si="11"/>
@@ -7818,12 +7815,12 @@
       </c>
       <c r="D372" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECORD=370,</v>
+        <v xml:space="preserve">        RECORDING=370,</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B373" s="1">
         <f t="shared" si="11"/>
@@ -7834,12 +7831,12 @@
       </c>
       <c r="D373" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECORDING=371,</v>
+        <v xml:space="preserve">        RECORDS=371,</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B374" s="1">
         <f t="shared" si="11"/>
@@ -7850,12 +7847,12 @@
       </c>
       <c r="D374" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECORDS=372,</v>
+        <v xml:space="preserve">        RECURSIVE=372,</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B375" s="1">
         <f t="shared" si="11"/>
@@ -7866,12 +7863,12 @@
       </c>
       <c r="D375" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECURSIVE=373,</v>
+        <v xml:space="preserve">        REDEFINES=373,</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B376" s="1">
         <f t="shared" si="11"/>
@@ -7882,12 +7879,12 @@
       </c>
       <c r="D376" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        REDEFINES=374,</v>
+        <v xml:space="preserve">        REEL=374,</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B377" s="1">
         <f t="shared" si="11"/>
@@ -7897,13 +7894,13 @@
         <v>366</v>
       </c>
       <c r="D377" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">        REEL=375,</v>
+        <f t="shared" ref="D377:D440" si="12">"        "&amp;C377&amp;"="&amp;B377&amp;","</f>
+        <v xml:space="preserve">        REFERENCE=375,</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B378" s="1">
         <f t="shared" si="11"/>
@@ -7913,13 +7910,13 @@
         <v>367</v>
       </c>
       <c r="D378" t="str">
-        <f t="shared" ref="D378:D441" si="12">"        "&amp;C378&amp;"="&amp;B378&amp;","</f>
-        <v xml:space="preserve">        REFERENCE=376,</v>
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">        REFERENCES=376,</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B379" s="1">
         <f t="shared" si="11"/>
@@ -7930,15 +7927,15 @@
       </c>
       <c r="D379" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REFERENCES=377,</v>
+        <v xml:space="preserve">        RELATIVE=377,</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B380" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="B380:B442" si="13">B379+1</f>
         <v>378</v>
       </c>
       <c r="C380" t="s">
@@ -7946,15 +7943,15 @@
       </c>
       <c r="D380" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RELATIVE=378,</v>
+        <v xml:space="preserve">        RELOAD=378,</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B381" s="1">
-        <f t="shared" ref="B381:B443" si="13">B380+1</f>
+        <f t="shared" si="13"/>
         <v>379</v>
       </c>
       <c r="C381" t="s">
@@ -7962,12 +7959,12 @@
       </c>
       <c r="D381" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RELOAD=379,</v>
+        <v xml:space="preserve">        REMAINDER=379,</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B382" s="1">
         <f t="shared" si="13"/>
@@ -7978,12 +7975,12 @@
       </c>
       <c r="D382" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REMAINDER=380,</v>
+        <v xml:space="preserve">        REMOVAL=380,</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B383" s="1">
         <f t="shared" si="13"/>
@@ -7994,12 +7991,12 @@
       </c>
       <c r="D383" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REMOVAL=381,</v>
+        <v xml:space="preserve">        RENAMES=381,</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B384" s="1">
         <f t="shared" si="13"/>
@@ -8010,12 +8007,12 @@
       </c>
       <c r="D384" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RENAMES=382,</v>
+        <v xml:space="preserve">        REPLACING=382,</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B385" s="1">
         <f t="shared" si="13"/>
@@ -8026,12 +8023,12 @@
       </c>
       <c r="D385" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REPLACING=383,</v>
+        <v xml:space="preserve">        RESERVE=383,</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B386" s="1">
         <f t="shared" si="13"/>
@@ -8042,12 +8039,12 @@
       </c>
       <c r="D386" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RESERVE=384,</v>
+        <v xml:space="preserve">        RETURNING=384,</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B387" s="1">
         <f t="shared" si="13"/>
@@ -8058,12 +8055,12 @@
       </c>
       <c r="D387" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RETURNING=385,</v>
+        <v xml:space="preserve">        REVERSED=385,</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B388" s="1">
         <f t="shared" si="13"/>
@@ -8074,12 +8071,12 @@
       </c>
       <c r="D388" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REVERSED=386,</v>
+        <v xml:space="preserve">        REWIND=386,</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B389" s="1">
         <f t="shared" si="13"/>
@@ -8090,12 +8087,12 @@
       </c>
       <c r="D389" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REWIND=387,</v>
+        <v xml:space="preserve">        RIGHT=387,</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B390" s="1">
         <f t="shared" si="13"/>
@@ -8106,12 +8103,12 @@
       </c>
       <c r="D390" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RIGHT=388,</v>
+        <v xml:space="preserve">        ROUNDED=388,</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B391" s="1">
         <f t="shared" si="13"/>
@@ -8122,12 +8119,12 @@
       </c>
       <c r="D391" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        ROUNDED=389,</v>
+        <v xml:space="preserve">        RUN=389,</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B392" s="1">
         <f t="shared" si="13"/>
@@ -8138,12 +8135,12 @@
       </c>
       <c r="D392" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RUN=390,</v>
+        <v xml:space="preserve">        SECTION=390,</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B393" s="1">
         <f t="shared" si="13"/>
@@ -8154,12 +8151,12 @@
       </c>
       <c r="D393" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SECTION=391,</v>
+        <v xml:space="preserve">        SECURITY=391,</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B394" s="1">
         <f t="shared" si="13"/>
@@ -8170,12 +8167,12 @@
       </c>
       <c r="D394" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SECURITY=392,</v>
+        <v xml:space="preserve">        SEGMENT_LIMIT=392,</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B395" s="1">
         <f t="shared" si="13"/>
@@ -8186,12 +8183,12 @@
       </c>
       <c r="D395" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEGMENT_LIMIT=393,</v>
+        <v xml:space="preserve">        SENTENCE=393,</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B396" s="1">
         <f t="shared" si="13"/>
@@ -8202,12 +8199,12 @@
       </c>
       <c r="D396" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SENTENCE=394,</v>
+        <v xml:space="preserve">        SEPARATE=394,</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B397" s="1">
         <f t="shared" si="13"/>
@@ -8218,12 +8215,12 @@
       </c>
       <c r="D397" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEPARATE=395,</v>
+        <v xml:space="preserve">        SEQUENCE=395,</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B398" s="1">
         <f t="shared" si="13"/>
@@ -8234,12 +8231,12 @@
       </c>
       <c r="D398" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEQUENCE=396,</v>
+        <v xml:space="preserve">        SEQUENTIAL=396,</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B399" s="1">
         <f t="shared" si="13"/>
@@ -8250,12 +8247,12 @@
       </c>
       <c r="D399" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEQUENTIAL=397,</v>
+        <v xml:space="preserve">        SIGN=397,</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B400" s="1">
         <f t="shared" si="13"/>
@@ -8266,12 +8263,12 @@
       </c>
       <c r="D400" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SIGN=398,</v>
+        <v xml:space="preserve">        SIZE=398,</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B401" s="1">
         <f t="shared" si="13"/>
@@ -8282,12 +8279,12 @@
       </c>
       <c r="D401" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SIZE=399,</v>
+        <v xml:space="preserve">        SORT_MERGE=399,</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B402" s="1">
         <f t="shared" si="13"/>
@@ -8298,12 +8295,12 @@
       </c>
       <c r="D402" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SORT_MERGE=400,</v>
+        <v xml:space="preserve">        SQL=400,</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B403" s="1">
         <f t="shared" si="13"/>
@@ -8314,12 +8311,12 @@
       </c>
       <c r="D403" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SQL=401,</v>
+        <v xml:space="preserve">        SQLIMS=401,</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B404" s="1">
         <f t="shared" si="13"/>
@@ -8330,12 +8327,12 @@
       </c>
       <c r="D404" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SQLIMS=402,</v>
+        <v xml:space="preserve">        STANDARD=402,</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B405" s="1">
         <f t="shared" si="13"/>
@@ -8346,12 +8343,12 @@
       </c>
       <c r="D405" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STANDARD=403,</v>
+        <v xml:space="preserve">        STANDARD_1=403,</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B406" s="1">
         <f t="shared" si="13"/>
@@ -8362,12 +8359,12 @@
       </c>
       <c r="D406" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STANDARD_1=404,</v>
+        <v xml:space="preserve">        STANDARD_2=404,</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B407" s="1">
         <f t="shared" si="13"/>
@@ -8378,12 +8375,12 @@
       </c>
       <c r="D407" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STANDARD_2=405,</v>
+        <v xml:space="preserve">        STATUS=405,</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B408" s="1">
         <f t="shared" si="13"/>
@@ -8394,12 +8391,12 @@
       </c>
       <c r="D408" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STATUS=406,</v>
+        <v xml:space="preserve">        SUPPRESS=406,</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B409" s="1">
         <f t="shared" si="13"/>
@@ -8410,12 +8407,12 @@
       </c>
       <c r="D409" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SUPPRESS=407,</v>
+        <v xml:space="preserve">        SYMBOL=407,</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B410" s="1">
         <f t="shared" si="13"/>
@@ -8426,12 +8423,12 @@
       </c>
       <c r="D410" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYMBOL=408,</v>
+        <v xml:space="preserve">        SYMBOLIC=408,</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B411" s="1">
         <f t="shared" si="13"/>
@@ -8442,12 +8439,12 @@
       </c>
       <c r="D411" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYMBOLIC=409,</v>
+        <v xml:space="preserve">        SYNC=409,</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B412" s="1">
         <f t="shared" si="13"/>
@@ -8458,12 +8455,12 @@
       </c>
       <c r="D412" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYNC=410,</v>
+        <v xml:space="preserve">        SYNCHRONIZED=410,</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B413" s="1">
         <f t="shared" si="13"/>
@@ -8474,12 +8471,12 @@
       </c>
       <c r="D413" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYNCHRONIZED=411,</v>
+        <v xml:space="preserve">        TALLYING=411,</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B414" s="1">
         <f t="shared" si="13"/>
@@ -8490,12 +8487,12 @@
       </c>
       <c r="D414" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TALLYING=412,</v>
+        <v xml:space="preserve">        TAPE=412,</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B415" s="1">
         <f t="shared" si="13"/>
@@ -8506,12 +8503,12 @@
       </c>
       <c r="D415" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TAPE=413,</v>
+        <v xml:space="preserve">        TEST=413,</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B416" s="1">
         <f t="shared" si="13"/>
@@ -8522,12 +8519,12 @@
       </c>
       <c r="D416" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TEST=414,</v>
+        <v xml:space="preserve">        THAN=414,</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B417" s="1">
         <f t="shared" si="13"/>
@@ -8538,12 +8535,12 @@
       </c>
       <c r="D417" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THAN=415,</v>
+        <v xml:space="preserve">        THEN=415,</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B418" s="1">
         <f t="shared" si="13"/>
@@ -8554,12 +8551,12 @@
       </c>
       <c r="D418" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THEN=416,</v>
+        <v xml:space="preserve">        THROUGH=416,</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B419" s="1">
         <f t="shared" si="13"/>
@@ -8570,12 +8567,12 @@
       </c>
       <c r="D419" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THROUGH=417,</v>
+        <v xml:space="preserve">        THRU=417,</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B420" s="1">
         <f t="shared" si="13"/>
@@ -8586,12 +8583,12 @@
       </c>
       <c r="D420" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THRU=418,</v>
+        <v xml:space="preserve">        TIME=418,</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B421" s="1">
         <f t="shared" si="13"/>
@@ -8602,12 +8599,12 @@
       </c>
       <c r="D421" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TIME=419,</v>
+        <v xml:space="preserve">        TIMES=419,</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B422" s="1">
         <f t="shared" si="13"/>
@@ -8618,12 +8615,12 @@
       </c>
       <c r="D422" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TIMES=420,</v>
+        <v xml:space="preserve">        TO=420,</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B423" s="1">
         <f t="shared" si="13"/>
@@ -8634,12 +8631,12 @@
       </c>
       <c r="D423" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TO=421,</v>
+        <v xml:space="preserve">        TOP=421,</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B424" s="1">
         <f t="shared" si="13"/>
@@ -8650,12 +8647,12 @@
       </c>
       <c r="D424" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TOP=422,</v>
+        <v xml:space="preserve">        TRACE=422,</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B425" s="1">
         <f t="shared" si="13"/>
@@ -8666,12 +8663,12 @@
       </c>
       <c r="D425" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TRACE=423,</v>
+        <v xml:space="preserve">        TRAILING=423,</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B426" s="1">
         <f t="shared" si="13"/>
@@ -8682,12 +8679,12 @@
       </c>
       <c r="D426" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TRAILING=424,</v>
+        <v xml:space="preserve">        TRUE=424,</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B427" s="1">
         <f t="shared" si="13"/>
@@ -8698,12 +8695,12 @@
       </c>
       <c r="D427" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TRUE=425,</v>
+        <v xml:space="preserve">        TYPE=425,</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B428" s="1">
         <f t="shared" si="13"/>
@@ -8714,12 +8711,12 @@
       </c>
       <c r="D428" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TYPE=426,</v>
+        <v xml:space="preserve">        UNBOUNDED=426,</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B429" s="1">
         <f t="shared" si="13"/>
@@ -8730,12 +8727,12 @@
       </c>
       <c r="D429" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UNBOUNDED=427,</v>
+        <v xml:space="preserve">        UNIT=427,</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B430" s="1">
         <f t="shared" si="13"/>
@@ -8746,12 +8743,12 @@
       </c>
       <c r="D430" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UNIT=428,</v>
+        <v xml:space="preserve">        UNTIL=428,</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B431" s="1">
         <f t="shared" si="13"/>
@@ -8762,12 +8759,12 @@
       </c>
       <c r="D431" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UNTIL=429,</v>
+        <v xml:space="preserve">        UP=429,</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B432" s="1">
         <f t="shared" si="13"/>
@@ -8778,12 +8775,12 @@
       </c>
       <c r="D432" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UP=430,</v>
+        <v xml:space="preserve">        UPON=430,</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B433" s="1">
         <f t="shared" si="13"/>
@@ -8794,12 +8791,12 @@
       </c>
       <c r="D433" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UPON=431,</v>
+        <v xml:space="preserve">        USAGE=431,</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B434" s="1">
         <f t="shared" si="13"/>
@@ -8810,12 +8807,12 @@
       </c>
       <c r="D434" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        USAGE=432,</v>
+        <v xml:space="preserve">        USING=432,</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B435" s="1">
         <f t="shared" si="13"/>
@@ -8826,12 +8823,12 @@
       </c>
       <c r="D435" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        USING=433,</v>
+        <v xml:space="preserve">        VALIDATING=433,</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B436" s="1">
         <f t="shared" si="13"/>
@@ -8842,12 +8839,12 @@
       </c>
       <c r="D436" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALIDATING=434,</v>
+        <v xml:space="preserve">        VALUE=434,</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B437" s="1">
         <f t="shared" si="13"/>
@@ -8858,12 +8855,12 @@
       </c>
       <c r="D437" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALUE=435,</v>
+        <v xml:space="preserve">        VALUES=435,</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B438" s="1">
         <f t="shared" si="13"/>
@@ -8874,28 +8871,28 @@
       </c>
       <c r="D438" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALUES=436,</v>
+        <v xml:space="preserve">        VARYING=436,</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B439" s="1">
         <f t="shared" si="13"/>
         <v>437</v>
       </c>
       <c r="C439" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D439" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VARYING=437,</v>
+        <v xml:space="preserve">        WITH=437,</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B440" s="1">
         <f t="shared" si="13"/>
@@ -8906,12 +8903,12 @@
       </c>
       <c r="D440" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        WITH=438,</v>
+        <v xml:space="preserve">        WORDS=438,</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B441" s="1">
         <f t="shared" si="13"/>
@@ -8921,13 +8918,13 @@
         <v>431</v>
       </c>
       <c r="D441" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">        WORDS=439,</v>
+        <f t="shared" ref="D441:D451" si="14">"        "&amp;C441&amp;"="&amp;B441&amp;","</f>
+        <v xml:space="preserve">        WRITE_ONLY=439,</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B442" s="1">
         <f t="shared" si="13"/>
@@ -8937,16 +8934,16 @@
         <v>432</v>
       </c>
       <c r="D442" t="str">
-        <f t="shared" ref="D442:D452" si="14">"        "&amp;C442&amp;"="&amp;B442&amp;","</f>
-        <v xml:space="preserve">        WRITE_ONLY=440,</v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        XML_SCHEMA=440,</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B443" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="B443:B451" si="15">B442+1</f>
         <v>441</v>
       </c>
       <c r="C443" t="s">
@@ -8954,29 +8951,26 @@
       </c>
       <c r="D443" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        XML_SCHEMA=441,</v>
+        <v xml:space="preserve">        YYYYDDD=441,</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B444" s="1">
-        <f t="shared" ref="B444:B452" si="15">B443+1</f>
+        <f t="shared" si="15"/>
         <v>442</v>
       </c>
       <c r="C444" t="s">
-        <v>434</v>
+        <v>452</v>
       </c>
       <c r="D444" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYDDD=442,</v>
+        <v xml:space="preserve">        YYYYMMDD=442,</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A445" t="s">
-        <v>436</v>
-      </c>
       <c r="B445" s="1">
         <f t="shared" si="15"/>
         <v>443</v>
@@ -8986,7 +8980,7 @@
       </c>
       <c r="D445" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYMMDD=443,</v>
+        <v xml:space="preserve">        TYPEDEF=443,</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8999,7 +8993,7 @@
       </c>
       <c r="D446" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        TYPEDEF=444,</v>
+        <v xml:space="preserve">        STRONG=444,</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -9012,7 +9006,7 @@
       </c>
       <c r="D447" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRONG=445,</v>
+        <v xml:space="preserve">        UNSAFE=445,</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -9021,11 +9015,11 @@
         <v>446</v>
       </c>
       <c r="C448" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D448" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        UNSAFE=446,</v>
+        <v xml:space="preserve">        PUBLIC=446,</v>
       </c>
     </row>
     <row r="449" spans="2:4" x14ac:dyDescent="0.25">
@@ -9038,7 +9032,7 @@
       </c>
       <c r="D449" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PUBLIC=447,</v>
+        <v xml:space="preserve">        PRIVATE=447,</v>
       </c>
     </row>
     <row r="450" spans="2:4" x14ac:dyDescent="0.25">
@@ -9047,11 +9041,11 @@
         <v>448</v>
       </c>
       <c r="C450" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="D450" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PRIVATE=448,</v>
+        <v xml:space="preserve">        IN_OUT=448,</v>
       </c>
     </row>
     <row r="451" spans="2:4" x14ac:dyDescent="0.25">
@@ -9064,33 +9058,33 @@
       </c>
       <c r="D451" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        IN_OUT=449,</v>
+        <v xml:space="preserve">        STRICT=449,</v>
       </c>
     </row>
     <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B452:B455" si="16">B451+1</f>
         <v>450</v>
       </c>
       <c r="C452" t="s">
         <v>469</v>
       </c>
       <c r="D452" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRICT=450,</v>
+        <f t="shared" ref="D452:D455" si="17">"        "&amp;C452&amp;"="&amp;B452&amp;","</f>
+        <v xml:space="preserve">        QuestionMark=450,</v>
       </c>
     </row>
     <row r="453" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B453" s="1">
-        <f t="shared" ref="B453:B456" si="16">B452+1</f>
+        <f t="shared" si="16"/>
         <v>451</v>
       </c>
       <c r="C453" t="s">
         <v>470</v>
       </c>
       <c r="D453" t="str">
-        <f t="shared" ref="D453:D456" si="17">"        "&amp;C453&amp;"="&amp;B453&amp;","</f>
-        <v xml:space="preserve">        QuestionMark=451,</v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">        CompilerDirective=451,</v>
       </c>
     </row>
     <row r="454" spans="2:4" x14ac:dyDescent="0.25">
@@ -9103,7 +9097,7 @@
       </c>
       <c r="D454" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CompilerDirective=452,</v>
+        <v xml:space="preserve">        CopyImportDirective=452,</v>
       </c>
     </row>
     <row r="455" spans="2:4" x14ac:dyDescent="0.25">
@@ -9116,33 +9110,20 @@
       </c>
       <c r="D455" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CopyImportDirective=453,</v>
+        <v xml:space="preserve">        ReplaceDirective=453,</v>
       </c>
     </row>
     <row r="456" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B456" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="B456" si="18">B455+1</f>
         <v>454</v>
       </c>
       <c r="C456" t="s">
         <v>473</v>
       </c>
       <c r="D456" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        ReplaceDirective=454,</v>
-      </c>
-    </row>
-    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B457" s="1">
-        <f t="shared" ref="B457" si="18">B456+1</f>
-        <v>455</v>
-      </c>
-      <c r="C457" t="s">
-        <v>474</v>
-      </c>
-      <c r="D457" t="str">
-        <f t="shared" ref="D457" si="19">"        "&amp;C457&amp;"="&amp;B457&amp;","</f>
-        <v xml:space="preserve">        ContinuationTokenGroup=455,</v>
+        <f t="shared" ref="D456" si="19">"        "&amp;C456&amp;"="&amp;B456&amp;","</f>
+        <v xml:space="preserve">        ContinuationTokenGroup=454,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#578, remove VALIDATING Token, add predicate on XML parse context
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="473">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1296,9 +1296,6 @@
   </si>
   <si>
     <t>USING</t>
-  </si>
-  <si>
-    <t>VALIDATING</t>
   </si>
   <si>
     <t>VALUE</t>
@@ -1857,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D456"/>
+  <dimension ref="A1:D455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="E358" sqref="E358"/>
+    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
+      <selection activeCell="A442" sqref="A442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,7 +1872,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B1" s="1">
         <v>-1</v>
@@ -1890,14 +1887,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B2" s="1">
         <f>B1+1</f>
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D2" t="str">
         <f>"        "&amp;C2&amp;"="&amp;B2&amp;","</f>
@@ -1906,7 +1903,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B3" s="1">
         <f>B2+1</f>
@@ -1922,7 +1919,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B67" si="1">B3+1</f>
@@ -1938,7 +1935,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="1"/>
@@ -1954,7 +1951,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="1"/>
@@ -1970,7 +1967,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="1"/>
@@ -1986,7 +1983,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="1"/>
@@ -2002,7 +1999,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="1"/>
@@ -2018,14 +2015,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2034,7 +2031,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="1"/>
@@ -2050,7 +2047,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="1"/>
@@ -2066,7 +2063,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="1"/>
@@ -2082,7 +2079,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
@@ -2098,7 +2095,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
@@ -2114,7 +2111,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
@@ -2130,7 +2127,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
@@ -2146,7 +2143,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
@@ -2162,7 +2159,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
@@ -2178,7 +2175,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="1"/>
@@ -2194,7 +2191,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="1"/>
@@ -2210,7 +2207,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="1"/>
@@ -2226,7 +2223,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="1"/>
@@ -2242,7 +2239,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="1"/>
@@ -2258,7 +2255,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="1"/>
@@ -2274,7 +2271,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="1"/>
@@ -2290,7 +2287,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="1"/>
@@ -2306,7 +2303,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="1"/>
@@ -2335,14 +2332,14 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2351,7 +2348,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" si="1"/>
@@ -2367,7 +2364,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="1"/>
@@ -2383,7 +2380,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" si="1"/>
@@ -2399,7 +2396,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" si="1"/>
@@ -2415,7 +2412,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" si="1"/>
@@ -2444,14 +2441,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2460,14 +2457,14 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2476,7 +2473,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="1"/>
@@ -2492,14 +2489,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2508,7 +2505,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="1"/>
@@ -2524,7 +2521,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" si="1"/>
@@ -2540,7 +2537,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" si="1"/>
@@ -2556,7 +2553,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="1"/>
@@ -2572,7 +2569,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" si="1"/>
@@ -2588,7 +2585,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" si="1"/>
@@ -2604,7 +2601,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" si="1"/>
@@ -2620,7 +2617,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" si="1"/>
@@ -2636,7 +2633,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B49" s="1">
         <f t="shared" si="1"/>
@@ -2652,7 +2649,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" si="1"/>
@@ -2668,7 +2665,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B51" s="1">
         <f t="shared" si="1"/>
@@ -2684,7 +2681,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" si="1"/>
@@ -2700,7 +2697,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B53" s="1">
         <f t="shared" si="1"/>
@@ -2716,7 +2713,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B54" s="1">
         <f t="shared" si="1"/>
@@ -2732,7 +2729,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B55" s="1">
         <f t="shared" si="1"/>
@@ -2748,14 +2745,14 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2764,7 +2761,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B57" s="1">
         <f t="shared" si="1"/>
@@ -2780,7 +2777,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B58" s="1">
         <f t="shared" si="1"/>
@@ -2796,7 +2793,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B59" s="1">
         <f t="shared" si="1"/>
@@ -2812,7 +2809,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B60" s="1">
         <f t="shared" si="1"/>
@@ -2828,7 +2825,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B61" s="1">
         <f t="shared" si="1"/>
@@ -2844,7 +2841,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B62" s="1">
         <f t="shared" si="1"/>
@@ -2860,7 +2857,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B63" s="1">
         <f t="shared" si="1"/>
@@ -2876,7 +2873,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B64" s="1">
         <f t="shared" si="1"/>
@@ -2892,7 +2889,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B65" s="1">
         <f t="shared" si="1"/>
@@ -2908,7 +2905,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B66" s="1">
         <f t="shared" si="1"/>
@@ -2924,7 +2921,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B67" s="1">
         <f t="shared" si="1"/>
@@ -2940,7 +2937,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B68" s="1">
         <f t="shared" ref="B68:B131" si="3">B67+1</f>
@@ -2956,7 +2953,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
@@ -2972,7 +2969,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
@@ -2988,7 +2985,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
@@ -3004,7 +3001,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
@@ -3020,14 +3017,14 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -3036,7 +3033,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
@@ -3052,7 +3049,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
@@ -3068,7 +3065,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
@@ -3084,7 +3081,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
@@ -3100,7 +3097,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
@@ -3116,7 +3113,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
@@ -3132,7 +3129,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B80" s="1">
         <f t="shared" si="3"/>
@@ -3148,7 +3145,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B81" s="1">
         <f t="shared" si="3"/>
@@ -3164,14 +3161,14 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B82" s="1">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3180,7 +3177,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B83" s="1">
         <f t="shared" si="3"/>
@@ -3196,7 +3193,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B84" s="1">
         <f t="shared" si="3"/>
@@ -3212,7 +3209,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B85" s="1">
         <f t="shared" si="3"/>
@@ -3228,7 +3225,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B86" s="1">
         <f t="shared" si="3"/>
@@ -3244,7 +3241,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B87" s="1">
         <f t="shared" si="3"/>
@@ -3260,7 +3257,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B88" s="1">
         <f t="shared" si="3"/>
@@ -3276,7 +3273,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B89" s="1">
         <f t="shared" si="3"/>
@@ -3292,7 +3289,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B90" s="1">
         <f t="shared" si="3"/>
@@ -3308,7 +3305,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B91" s="1">
         <f t="shared" si="3"/>
@@ -3324,7 +3321,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B92" s="1">
         <f t="shared" si="3"/>
@@ -3340,7 +3337,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B93" s="1">
         <f t="shared" si="3"/>
@@ -3356,7 +3353,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B94" s="1">
         <f t="shared" si="3"/>
@@ -3372,7 +3369,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B95" s="1">
         <f t="shared" si="3"/>
@@ -3388,7 +3385,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B96" s="1">
         <f t="shared" si="3"/>
@@ -3404,7 +3401,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B97" s="1">
         <f t="shared" si="3"/>
@@ -3420,7 +3417,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B98" s="1">
         <f t="shared" si="3"/>
@@ -3436,7 +3433,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B99" s="1">
         <f t="shared" si="3"/>
@@ -3452,7 +3449,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B100" s="1">
         <f t="shared" si="3"/>
@@ -3468,7 +3465,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B101" s="1">
         <f t="shared" si="3"/>
@@ -3484,7 +3481,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B102" s="1">
         <f t="shared" si="3"/>
@@ -3500,7 +3497,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B103" s="1">
         <f t="shared" si="3"/>
@@ -3516,7 +3513,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B104" s="1">
         <f t="shared" si="3"/>
@@ -3532,7 +3529,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B105" s="1">
         <f t="shared" si="3"/>
@@ -3548,7 +3545,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B106" s="1">
         <f t="shared" si="3"/>
@@ -3564,7 +3561,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B107" s="1">
         <f t="shared" si="3"/>
@@ -3580,7 +3577,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B108" s="1">
         <f t="shared" si="3"/>
@@ -3596,7 +3593,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B109" s="1">
         <f t="shared" si="3"/>
@@ -3612,7 +3609,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B110" s="1">
         <f t="shared" si="3"/>
@@ -3628,7 +3625,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B111" s="1">
         <f t="shared" si="3"/>
@@ -3644,7 +3641,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B112" s="1">
         <f t="shared" si="3"/>
@@ -3660,7 +3657,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B113" s="1">
         <f t="shared" si="3"/>
@@ -3676,7 +3673,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B114" s="1">
         <f t="shared" si="3"/>
@@ -3692,7 +3689,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B115" s="1">
         <f t="shared" si="3"/>
@@ -3708,7 +3705,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B116" s="1">
         <f t="shared" si="3"/>
@@ -3724,7 +3721,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B117" s="1">
         <f t="shared" si="3"/>
@@ -3740,7 +3737,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B118" s="1">
         <f t="shared" si="3"/>
@@ -3756,7 +3753,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B119" s="1">
         <f t="shared" si="3"/>
@@ -3772,7 +3769,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B120" s="1">
         <f t="shared" si="3"/>
@@ -3788,7 +3785,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B121" s="1">
         <f t="shared" si="3"/>
@@ -3804,7 +3801,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B122" s="1">
         <f t="shared" si="3"/>
@@ -3820,7 +3817,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B123" s="1">
         <f t="shared" si="3"/>
@@ -3836,7 +3833,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B124" s="1">
         <f t="shared" si="3"/>
@@ -3852,7 +3849,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B125" s="1">
         <f t="shared" si="3"/>
@@ -3868,7 +3865,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B126" s="1">
         <f t="shared" si="3"/>
@@ -3884,7 +3881,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B127" s="1">
         <f t="shared" si="3"/>
@@ -3900,7 +3897,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B128" s="1">
         <f t="shared" si="3"/>
@@ -3916,7 +3913,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B129" s="1">
         <f t="shared" si="3"/>
@@ -3932,7 +3929,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B130" s="1">
         <f t="shared" si="3"/>
@@ -3948,7 +3945,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B131" s="1">
         <f t="shared" si="3"/>
@@ -3964,7 +3961,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B132" s="1">
         <f t="shared" ref="B132:B195" si="5">B131+1</f>
@@ -3980,7 +3977,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B133" s="1">
         <f t="shared" si="5"/>
@@ -3996,7 +3993,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B134" s="1">
         <f t="shared" si="5"/>
@@ -4012,7 +4009,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B135" s="1">
         <f t="shared" si="5"/>
@@ -4028,7 +4025,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B136" s="1">
         <f t="shared" si="5"/>
@@ -4044,7 +4041,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B137" s="1">
         <f t="shared" si="5"/>
@@ -4060,7 +4057,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B138" s="1">
         <f t="shared" si="5"/>
@@ -4076,7 +4073,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B139" s="1">
         <f t="shared" si="5"/>
@@ -4092,7 +4089,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B140" s="1">
         <f t="shared" si="5"/>
@@ -4108,7 +4105,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B141" s="1">
         <f t="shared" si="5"/>
@@ -4124,7 +4121,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B142" s="1">
         <f t="shared" si="5"/>
@@ -4140,7 +4137,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B143" s="1">
         <f t="shared" si="5"/>
@@ -4156,7 +4153,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B144" s="1">
         <f t="shared" si="5"/>
@@ -4172,7 +4169,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B145" s="1">
         <f t="shared" si="5"/>
@@ -4188,7 +4185,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B146" s="1">
         <f t="shared" si="5"/>
@@ -4204,7 +4201,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B147" s="1">
         <f t="shared" si="5"/>
@@ -4220,7 +4217,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B148" s="1">
         <f t="shared" si="5"/>
@@ -4236,7 +4233,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B149" s="1">
         <f t="shared" si="5"/>
@@ -4252,7 +4249,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B150" s="1">
         <f t="shared" si="5"/>
@@ -4268,7 +4265,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B151" s="1">
         <f t="shared" si="5"/>
@@ -4284,14 +4281,14 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B152" s="1">
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="C152" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="4"/>
@@ -4300,7 +4297,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B153" s="1">
         <f t="shared" si="5"/>
@@ -4316,7 +4313,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B154" s="1">
         <f t="shared" si="5"/>
@@ -4332,7 +4329,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B155" s="1">
         <f t="shared" si="5"/>
@@ -4348,7 +4345,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B156" s="1">
         <f t="shared" si="5"/>
@@ -4364,7 +4361,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B157" s="1">
         <f t="shared" si="5"/>
@@ -4380,7 +4377,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B158" s="1">
         <f t="shared" si="5"/>
@@ -4396,7 +4393,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B159" s="1">
         <f t="shared" si="5"/>
@@ -4412,7 +4409,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B160" s="1">
         <f t="shared" si="5"/>
@@ -4428,7 +4425,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B161" s="1">
         <f t="shared" si="5"/>
@@ -4444,7 +4441,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B162" s="1">
         <f t="shared" si="5"/>
@@ -4460,7 +4457,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B163" s="1">
         <f t="shared" si="5"/>
@@ -4476,7 +4473,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B164" s="1">
         <f t="shared" si="5"/>
@@ -4492,7 +4489,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B165" s="1">
         <f t="shared" si="5"/>
@@ -4508,7 +4505,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B166" s="1">
         <f t="shared" si="5"/>
@@ -4524,7 +4521,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B167" s="1">
         <f t="shared" si="5"/>
@@ -4540,7 +4537,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B168" s="1">
         <f t="shared" si="5"/>
@@ -4556,7 +4553,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B169" s="1">
         <f t="shared" si="5"/>
@@ -4572,7 +4569,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B170" s="1">
         <f t="shared" si="5"/>
@@ -4588,7 +4585,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B171" s="1">
         <f t="shared" si="5"/>
@@ -4604,7 +4601,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B172" s="1">
         <f t="shared" si="5"/>
@@ -4620,7 +4617,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B173" s="1">
         <f t="shared" si="5"/>
@@ -4636,7 +4633,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B174" s="1">
         <f t="shared" si="5"/>
@@ -4652,7 +4649,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B175" s="1">
         <f t="shared" si="5"/>
@@ -4668,7 +4665,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B176" s="1">
         <f t="shared" si="5"/>
@@ -4684,7 +4681,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B177" s="1">
         <f t="shared" si="5"/>
@@ -4700,7 +4697,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B178" s="1">
         <f t="shared" si="5"/>
@@ -4716,7 +4713,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B179" s="1">
         <f t="shared" si="5"/>
@@ -4732,7 +4729,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B180" s="1">
         <f t="shared" si="5"/>
@@ -4748,7 +4745,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B181" s="1">
         <f t="shared" si="5"/>
@@ -4764,7 +4761,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B182" s="1">
         <f t="shared" si="5"/>
@@ -4780,7 +4777,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B183" s="1">
         <f>B182+1</f>
@@ -4796,7 +4793,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B184" s="1">
         <f t="shared" si="5"/>
@@ -4812,7 +4809,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B185" s="1">
         <f t="shared" si="5"/>
@@ -4828,7 +4825,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B186" s="1">
         <f t="shared" si="5"/>
@@ -4844,7 +4841,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B187" s="1">
         <f t="shared" si="5"/>
@@ -4860,7 +4857,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B188" s="1">
         <f t="shared" si="5"/>
@@ -4876,7 +4873,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B189" s="1">
         <f t="shared" si="5"/>
@@ -4892,7 +4889,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B190" s="1">
         <f t="shared" si="5"/>
@@ -4908,7 +4905,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B191" s="1">
         <f t="shared" si="5"/>
@@ -4924,7 +4921,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B192" s="1">
         <f t="shared" si="5"/>
@@ -4940,7 +4937,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B193" s="1">
         <f t="shared" si="5"/>
@@ -4956,7 +4953,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B194" s="1">
         <f t="shared" si="5"/>
@@ -4972,7 +4969,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B195" s="1">
         <f t="shared" si="5"/>
@@ -4988,7 +4985,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B196" s="1">
         <f t="shared" ref="B196:B257" si="7">B195+1</f>
@@ -5004,7 +5001,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B197" s="1">
         <f t="shared" si="7"/>
@@ -5020,7 +5017,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B198" s="1">
         <f t="shared" si="7"/>
@@ -5036,7 +5033,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B199" s="1">
         <f t="shared" si="7"/>
@@ -5052,7 +5049,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B200" s="1">
         <f t="shared" si="7"/>
@@ -5068,7 +5065,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B201" s="1">
         <f t="shared" si="7"/>
@@ -5084,7 +5081,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B202" s="1">
         <f t="shared" si="7"/>
@@ -5100,7 +5097,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B203" s="1">
         <f t="shared" si="7"/>
@@ -5116,7 +5113,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B204" s="1">
         <f t="shared" si="7"/>
@@ -5132,7 +5129,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B205" s="1">
         <f t="shared" si="7"/>
@@ -5148,7 +5145,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B206" s="1">
         <f t="shared" si="7"/>
@@ -5164,7 +5161,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B207" s="1">
         <f t="shared" si="7"/>
@@ -5180,7 +5177,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B208" s="1">
         <f t="shared" si="7"/>
@@ -5196,7 +5193,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B209" s="1">
         <f t="shared" si="7"/>
@@ -5212,7 +5209,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B210" s="1">
         <f t="shared" si="7"/>
@@ -5228,7 +5225,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B211" s="1">
         <f t="shared" si="7"/>
@@ -5244,7 +5241,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B212" s="1">
         <f t="shared" si="7"/>
@@ -5260,7 +5257,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B213" s="1">
         <f t="shared" si="7"/>
@@ -5276,7 +5273,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B214" s="1">
         <f t="shared" si="7"/>
@@ -5292,7 +5289,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B215" s="1">
         <f t="shared" si="7"/>
@@ -5308,7 +5305,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B216" s="1">
         <f t="shared" si="7"/>
@@ -5324,7 +5321,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B217" s="1">
         <f t="shared" si="7"/>
@@ -5340,7 +5337,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B218" s="1">
         <f t="shared" si="7"/>
@@ -5356,7 +5353,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B219" s="1">
         <f t="shared" si="7"/>
@@ -5372,7 +5369,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B220" s="1">
         <f t="shared" si="7"/>
@@ -5388,7 +5385,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B221" s="1">
         <f t="shared" si="7"/>
@@ -5404,7 +5401,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B222" s="1">
         <f t="shared" si="7"/>
@@ -5420,7 +5417,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B223" s="1">
         <f t="shared" si="7"/>
@@ -5436,7 +5433,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B224" s="1">
         <f t="shared" si="7"/>
@@ -5452,7 +5449,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B225" s="1">
         <f t="shared" si="7"/>
@@ -5468,7 +5465,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B226" s="1">
         <f t="shared" si="7"/>
@@ -5484,7 +5481,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B227" s="1">
         <f t="shared" si="7"/>
@@ -5500,7 +5497,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B228" s="1">
         <f t="shared" si="7"/>
@@ -5516,7 +5513,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B229" s="1">
         <f t="shared" si="7"/>
@@ -5532,7 +5529,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B230" s="1">
         <f t="shared" si="7"/>
@@ -5548,7 +5545,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B231" s="1">
         <f t="shared" si="7"/>
@@ -5564,7 +5561,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B232" s="1">
         <f t="shared" si="7"/>
@@ -5580,7 +5577,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B233" s="1">
         <f t="shared" si="7"/>
@@ -5596,7 +5593,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B234" s="1">
         <f t="shared" si="7"/>
@@ -5612,7 +5609,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B235" s="1">
         <f t="shared" si="7"/>
@@ -5628,7 +5625,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B236" s="1">
         <f t="shared" si="7"/>
@@ -5644,7 +5641,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B237" s="1">
         <f t="shared" si="7"/>
@@ -5660,7 +5657,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B238" s="1">
         <f t="shared" si="7"/>
@@ -5676,7 +5673,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B239" s="1">
         <f t="shared" si="7"/>
@@ -5692,7 +5689,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B240" s="1">
         <f t="shared" si="7"/>
@@ -5708,7 +5705,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B241" s="1">
         <f t="shared" si="7"/>
@@ -5724,7 +5721,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B242" s="1">
         <f t="shared" si="7"/>
@@ -5740,7 +5737,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B243" s="1">
         <f t="shared" si="7"/>
@@ -5756,7 +5753,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B244" s="1">
         <f t="shared" si="7"/>
@@ -5772,7 +5769,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B245" s="1">
         <f t="shared" si="7"/>
@@ -5788,7 +5785,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B246" s="1">
         <f t="shared" si="7"/>
@@ -5804,7 +5801,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B247" s="1">
         <f t="shared" si="7"/>
@@ -5820,7 +5817,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B248" s="1">
         <f t="shared" si="7"/>
@@ -5836,7 +5833,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B249" s="1">
         <f t="shared" si="7"/>
@@ -5852,7 +5849,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B250" s="1">
         <f t="shared" si="7"/>
@@ -5868,7 +5865,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B251" s="1">
         <f t="shared" si="7"/>
@@ -5884,7 +5881,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B252" s="1">
         <f t="shared" si="7"/>
@@ -5900,7 +5897,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B253" s="1">
         <f t="shared" si="7"/>
@@ -5916,7 +5913,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B254" s="1">
         <f t="shared" si="7"/>
@@ -5932,7 +5929,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B255" s="1">
         <f t="shared" si="7"/>
@@ -5948,7 +5945,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B256" s="1">
         <f t="shared" si="7"/>
@@ -5964,7 +5961,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B257" s="1">
         <f t="shared" si="7"/>
@@ -5980,7 +5977,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B258" s="1">
         <f t="shared" ref="B258:B319" si="9">B257+1</f>
@@ -5996,7 +5993,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B259" s="1">
         <f t="shared" si="9"/>
@@ -6012,7 +6009,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B260" s="1">
         <f t="shared" si="9"/>
@@ -6028,7 +6025,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B261" s="1">
         <f t="shared" si="9"/>
@@ -6044,7 +6041,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B262" s="1">
         <f t="shared" si="9"/>
@@ -6060,7 +6057,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B263" s="1">
         <f t="shared" si="9"/>
@@ -6076,7 +6073,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B264" s="1">
         <f t="shared" si="9"/>
@@ -6092,7 +6089,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B265" s="1">
         <f t="shared" si="9"/>
@@ -6108,7 +6105,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B266" s="1">
         <f t="shared" si="9"/>
@@ -6124,7 +6121,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B267" s="1">
         <f t="shared" si="9"/>
@@ -6140,7 +6137,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B268" s="1">
         <f t="shared" si="9"/>
@@ -6156,7 +6153,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B269" s="1">
         <f t="shared" si="9"/>
@@ -6172,7 +6169,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B270" s="1">
         <f t="shared" si="9"/>
@@ -6188,7 +6185,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B271" s="1">
         <f t="shared" si="9"/>
@@ -6204,7 +6201,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B272" s="1">
         <f t="shared" si="9"/>
@@ -6220,7 +6217,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B273" s="1">
         <f t="shared" si="9"/>
@@ -6236,7 +6233,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B274" s="1">
         <f t="shared" si="9"/>
@@ -6252,7 +6249,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B275" s="1">
         <f t="shared" si="9"/>
@@ -6268,7 +6265,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B276" s="1">
         <f t="shared" si="9"/>
@@ -6284,7 +6281,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B277" s="1">
         <f t="shared" si="9"/>
@@ -6300,7 +6297,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B278" s="1">
         <f t="shared" si="9"/>
@@ -6316,7 +6313,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B279" s="1">
         <f t="shared" si="9"/>
@@ -6332,7 +6329,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B280" s="1">
         <f t="shared" si="9"/>
@@ -6348,7 +6345,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B281" s="1">
         <f t="shared" si="9"/>
@@ -6364,7 +6361,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B282" s="1">
         <f t="shared" si="9"/>
@@ -6380,7 +6377,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B283" s="1">
         <f t="shared" si="9"/>
@@ -6396,7 +6393,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B284" s="1">
         <f t="shared" si="9"/>
@@ -6412,7 +6409,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B285" s="1">
         <f t="shared" si="9"/>
@@ -6428,7 +6425,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B286" s="1">
         <f t="shared" si="9"/>
@@ -6444,7 +6441,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B287" s="1">
         <f t="shared" si="9"/>
@@ -6460,7 +6457,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B288" s="1">
         <f t="shared" si="9"/>
@@ -6476,7 +6473,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B289" s="1">
         <f t="shared" si="9"/>
@@ -6492,7 +6489,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B290" s="1">
         <f t="shared" si="9"/>
@@ -6508,7 +6505,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B291" s="1">
         <f t="shared" si="9"/>
@@ -6524,7 +6521,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B292" s="1">
         <f t="shared" si="9"/>
@@ -6540,7 +6537,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B293" s="1">
         <f t="shared" si="9"/>
@@ -6556,7 +6553,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B294" s="1">
         <f t="shared" si="9"/>
@@ -6572,7 +6569,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B295" s="1">
         <f t="shared" si="9"/>
@@ -6588,7 +6585,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B296" s="1">
         <f t="shared" si="9"/>
@@ -6604,7 +6601,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B297" s="1">
         <f t="shared" si="9"/>
@@ -6620,7 +6617,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B298" s="1">
         <f t="shared" si="9"/>
@@ -6636,7 +6633,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B299" s="1">
         <f t="shared" si="9"/>
@@ -6652,7 +6649,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B300" s="1">
         <f t="shared" si="9"/>
@@ -6668,7 +6665,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B301" s="1">
         <f t="shared" si="9"/>
@@ -6684,7 +6681,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B302" s="1">
         <f t="shared" si="9"/>
@@ -6700,7 +6697,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B303" s="1">
         <f t="shared" si="9"/>
@@ -6716,7 +6713,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B304" s="1">
         <f t="shared" si="9"/>
@@ -6732,7 +6729,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B305" s="1">
         <f t="shared" si="9"/>
@@ -6748,7 +6745,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B306" s="1">
         <f t="shared" si="9"/>
@@ -6764,7 +6761,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B307" s="1">
         <f t="shared" si="9"/>
@@ -6780,7 +6777,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B308" s="1">
         <f t="shared" si="9"/>
@@ -6796,7 +6793,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B309" s="1">
         <f t="shared" si="9"/>
@@ -6812,7 +6809,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B310" s="1">
         <f t="shared" si="9"/>
@@ -6828,7 +6825,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B311" s="1">
         <f t="shared" si="9"/>
@@ -6844,7 +6841,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B312" s="1">
         <f t="shared" si="9"/>
@@ -6860,7 +6857,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B313" s="1">
         <f t="shared" si="9"/>
@@ -6876,7 +6873,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B314" s="1">
         <f t="shared" si="9"/>
@@ -6892,7 +6889,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B315" s="1">
         <f t="shared" si="9"/>
@@ -6908,7 +6905,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B316" s="1">
         <f t="shared" si="9"/>
@@ -6924,7 +6921,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B317" s="1">
         <f t="shared" si="9"/>
@@ -6940,7 +6937,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B318" s="1">
         <f t="shared" si="9"/>
@@ -6956,7 +6953,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B319" s="1">
         <f t="shared" si="9"/>
@@ -6972,7 +6969,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B320" s="1">
         <f t="shared" ref="B320:B379" si="11">B319+1</f>
@@ -6988,7 +6985,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B321" s="1">
         <f t="shared" si="11"/>
@@ -7004,7 +7001,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B322" s="1">
         <f t="shared" si="11"/>
@@ -7020,7 +7017,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B323" s="1">
         <f t="shared" si="11"/>
@@ -7036,7 +7033,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B324" s="1">
         <f t="shared" si="11"/>
@@ -7052,7 +7049,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B325" s="1">
         <f t="shared" si="11"/>
@@ -7068,7 +7065,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B326" s="1">
         <f t="shared" si="11"/>
@@ -7084,7 +7081,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B327" s="1">
         <f t="shared" si="11"/>
@@ -7100,7 +7097,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B328" s="1">
         <f t="shared" si="11"/>
@@ -7116,7 +7113,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B329" s="1">
         <f t="shared" si="11"/>
@@ -7132,7 +7129,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B330" s="1">
         <f t="shared" si="11"/>
@@ -7148,7 +7145,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B331" s="1">
         <f t="shared" si="11"/>
@@ -7164,7 +7161,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B332" s="1">
         <f t="shared" si="11"/>
@@ -7180,7 +7177,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B333" s="1">
         <f t="shared" si="11"/>
@@ -7196,7 +7193,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B334" s="1">
         <f t="shared" si="11"/>
@@ -7212,7 +7209,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B335" s="1">
         <f t="shared" si="11"/>
@@ -7228,7 +7225,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B336" s="1">
         <f t="shared" si="11"/>
@@ -7244,7 +7241,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B337" s="1">
         <f t="shared" si="11"/>
@@ -7260,7 +7257,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B338" s="1">
         <f t="shared" si="11"/>
@@ -7276,7 +7273,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B339" s="1">
         <f t="shared" si="11"/>
@@ -7292,7 +7289,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B340" s="1">
         <f t="shared" si="11"/>
@@ -7308,7 +7305,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B341" s="1">
         <f t="shared" si="11"/>
@@ -7324,7 +7321,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B342" s="1">
         <f t="shared" si="11"/>
@@ -7340,7 +7337,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B343" s="1">
         <f t="shared" si="11"/>
@@ -7356,7 +7353,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B344" s="1">
         <f t="shared" si="11"/>
@@ -7372,7 +7369,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B345" s="1">
         <f t="shared" si="11"/>
@@ -7388,7 +7385,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B346" s="1">
         <f t="shared" si="11"/>
@@ -7404,7 +7401,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B347" s="1">
         <f t="shared" si="11"/>
@@ -7420,7 +7417,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B348" s="1">
         <f t="shared" si="11"/>
@@ -7436,7 +7433,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B349" s="1">
         <f t="shared" si="11"/>
@@ -7452,7 +7449,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B350" s="1">
         <f t="shared" si="11"/>
@@ -7468,7 +7465,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B351" s="1">
         <f t="shared" si="11"/>
@@ -7484,7 +7481,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B352" s="1">
         <f t="shared" si="11"/>
@@ -7500,7 +7497,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B353" s="1">
         <f t="shared" si="11"/>
@@ -7516,7 +7513,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B354" s="1">
         <f t="shared" si="11"/>
@@ -7532,7 +7529,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B355" s="1">
         <f t="shared" si="11"/>
@@ -7548,7 +7545,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B356" s="1">
         <f t="shared" si="11"/>
@@ -7564,7 +7561,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B357" s="1">
         <f t="shared" si="11"/>
@@ -7580,7 +7577,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B358" s="1">
         <f t="shared" si="11"/>
@@ -7596,7 +7593,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B359" s="1">
         <f t="shared" si="11"/>
@@ -7612,7 +7609,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B360" s="1">
         <f t="shared" si="11"/>
@@ -7628,7 +7625,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B361" s="1">
         <f t="shared" si="11"/>
@@ -7644,7 +7641,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B362" s="1">
         <f t="shared" si="11"/>
@@ -7660,7 +7657,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B363" s="1">
         <f t="shared" si="11"/>
@@ -7676,7 +7673,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B364" s="1">
         <f t="shared" si="11"/>
@@ -7692,7 +7689,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B365" s="1">
         <f t="shared" si="11"/>
@@ -7708,7 +7705,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B366" s="1">
         <f t="shared" si="11"/>
@@ -7724,7 +7721,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B367" s="1">
         <f t="shared" si="11"/>
@@ -7740,7 +7737,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B368" s="1">
         <f t="shared" si="11"/>
@@ -7756,7 +7753,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B369" s="1">
         <f t="shared" si="11"/>
@@ -7772,7 +7769,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B370" s="1">
         <f t="shared" si="11"/>
@@ -7788,7 +7785,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B371" s="1">
         <f t="shared" si="11"/>
@@ -7804,7 +7801,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B372" s="1">
         <f t="shared" si="11"/>
@@ -7820,7 +7817,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B373" s="1">
         <f t="shared" si="11"/>
@@ -7836,7 +7833,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B374" s="1">
         <f t="shared" si="11"/>
@@ -7852,7 +7849,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B375" s="1">
         <f t="shared" si="11"/>
@@ -7868,7 +7865,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B376" s="1">
         <f t="shared" si="11"/>
@@ -7884,7 +7881,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B377" s="1">
         <f t="shared" si="11"/>
@@ -7894,13 +7891,13 @@
         <v>366</v>
       </c>
       <c r="D377" t="str">
-        <f t="shared" ref="D377:D440" si="12">"        "&amp;C377&amp;"="&amp;B377&amp;","</f>
+        <f t="shared" ref="D377:D439" si="12">"        "&amp;C377&amp;"="&amp;B377&amp;","</f>
         <v xml:space="preserve">        REFERENCE=375,</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B378" s="1">
         <f t="shared" si="11"/>
@@ -7916,7 +7913,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B379" s="1">
         <f t="shared" si="11"/>
@@ -7932,10 +7929,10 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B380" s="1">
-        <f t="shared" ref="B380:B442" si="13">B379+1</f>
+        <f t="shared" ref="B380:B441" si="13">B379+1</f>
         <v>378</v>
       </c>
       <c r="C380" t="s">
@@ -7948,7 +7945,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B381" s="1">
         <f t="shared" si="13"/>
@@ -7964,7 +7961,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B382" s="1">
         <f t="shared" si="13"/>
@@ -7980,7 +7977,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B383" s="1">
         <f t="shared" si="13"/>
@@ -7996,7 +7993,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B384" s="1">
         <f t="shared" si="13"/>
@@ -8012,7 +8009,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B385" s="1">
         <f t="shared" si="13"/>
@@ -8028,7 +8025,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B386" s="1">
         <f t="shared" si="13"/>
@@ -8044,7 +8041,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B387" s="1">
         <f t="shared" si="13"/>
@@ -8060,7 +8057,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B388" s="1">
         <f t="shared" si="13"/>
@@ -8076,7 +8073,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B389" s="1">
         <f t="shared" si="13"/>
@@ -8092,7 +8089,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B390" s="1">
         <f t="shared" si="13"/>
@@ -8108,7 +8105,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B391" s="1">
         <f t="shared" si="13"/>
@@ -8124,7 +8121,7 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B392" s="1">
         <f t="shared" si="13"/>
@@ -8140,7 +8137,7 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B393" s="1">
         <f t="shared" si="13"/>
@@ -8156,7 +8153,7 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B394" s="1">
         <f t="shared" si="13"/>
@@ -8172,7 +8169,7 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B395" s="1">
         <f t="shared" si="13"/>
@@ -8188,7 +8185,7 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B396" s="1">
         <f t="shared" si="13"/>
@@ -8204,7 +8201,7 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B397" s="1">
         <f t="shared" si="13"/>
@@ -8220,7 +8217,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B398" s="1">
         <f t="shared" si="13"/>
@@ -8236,7 +8233,7 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B399" s="1">
         <f t="shared" si="13"/>
@@ -8252,7 +8249,7 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B400" s="1">
         <f t="shared" si="13"/>
@@ -8268,7 +8265,7 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B401" s="1">
         <f t="shared" si="13"/>
@@ -8284,7 +8281,7 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B402" s="1">
         <f t="shared" si="13"/>
@@ -8300,7 +8297,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B403" s="1">
         <f t="shared" si="13"/>
@@ -8316,7 +8313,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B404" s="1">
         <f t="shared" si="13"/>
@@ -8332,7 +8329,7 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B405" s="1">
         <f t="shared" si="13"/>
@@ -8348,7 +8345,7 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B406" s="1">
         <f t="shared" si="13"/>
@@ -8364,7 +8361,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B407" s="1">
         <f t="shared" si="13"/>
@@ -8380,7 +8377,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B408" s="1">
         <f t="shared" si="13"/>
@@ -8396,7 +8393,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B409" s="1">
         <f t="shared" si="13"/>
@@ -8412,7 +8409,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B410" s="1">
         <f t="shared" si="13"/>
@@ -8428,7 +8425,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B411" s="1">
         <f t="shared" si="13"/>
@@ -8444,7 +8441,7 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B412" s="1">
         <f t="shared" si="13"/>
@@ -8460,7 +8457,7 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B413" s="1">
         <f t="shared" si="13"/>
@@ -8476,7 +8473,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B414" s="1">
         <f t="shared" si="13"/>
@@ -8492,7 +8489,7 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B415" s="1">
         <f t="shared" si="13"/>
@@ -8508,7 +8505,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B416" s="1">
         <f t="shared" si="13"/>
@@ -8524,7 +8521,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B417" s="1">
         <f t="shared" si="13"/>
@@ -8540,7 +8537,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B418" s="1">
         <f t="shared" si="13"/>
@@ -8556,7 +8553,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B419" s="1">
         <f t="shared" si="13"/>
@@ -8572,7 +8569,7 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B420" s="1">
         <f t="shared" si="13"/>
@@ -8588,7 +8585,7 @@
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B421" s="1">
         <f t="shared" si="13"/>
@@ -8604,7 +8601,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B422" s="1">
         <f t="shared" si="13"/>
@@ -8620,7 +8617,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B423" s="1">
         <f t="shared" si="13"/>
@@ -8636,7 +8633,7 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B424" s="1">
         <f t="shared" si="13"/>
@@ -8652,7 +8649,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B425" s="1">
         <f t="shared" si="13"/>
@@ -8668,7 +8665,7 @@
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B426" s="1">
         <f t="shared" si="13"/>
@@ -8684,7 +8681,7 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B427" s="1">
         <f t="shared" si="13"/>
@@ -8700,7 +8697,7 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B428" s="1">
         <f t="shared" si="13"/>
@@ -8716,7 +8713,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B429" s="1">
         <f t="shared" si="13"/>
@@ -8732,7 +8729,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B430" s="1">
         <f t="shared" si="13"/>
@@ -8748,7 +8745,7 @@
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B431" s="1">
         <f t="shared" si="13"/>
@@ -8764,7 +8761,7 @@
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B432" s="1">
         <f t="shared" si="13"/>
@@ -8780,7 +8777,7 @@
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B433" s="1">
         <f t="shared" si="13"/>
@@ -8796,7 +8793,7 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B434" s="1">
         <f t="shared" si="13"/>
@@ -8812,7 +8809,7 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B435" s="1">
         <f t="shared" si="13"/>
@@ -8823,12 +8820,12 @@
       </c>
       <c r="D435" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALIDATING=433,</v>
+        <v xml:space="preserve">        VALUE=433,</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B436" s="1">
         <f t="shared" si="13"/>
@@ -8839,12 +8836,12 @@
       </c>
       <c r="D436" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALUE=434,</v>
+        <v xml:space="preserve">        VALUES=434,</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B437" s="1">
         <f t="shared" si="13"/>
@@ -8855,28 +8852,28 @@
       </c>
       <c r="D437" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALUES=435,</v>
+        <v xml:space="preserve">        VARYING=435,</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B438" s="1">
         <f t="shared" si="13"/>
         <v>436</v>
       </c>
       <c r="C438" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D438" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VARYING=436,</v>
+        <v xml:space="preserve">        WITH=436,</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B439" s="1">
         <f t="shared" si="13"/>
@@ -8887,12 +8884,12 @@
       </c>
       <c r="D439" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        WITH=437,</v>
+        <v xml:space="preserve">        WORDS=437,</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B440" s="1">
         <f t="shared" si="13"/>
@@ -8902,13 +8899,13 @@
         <v>430</v>
       </c>
       <c r="D440" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">        WORDS=438,</v>
+        <f t="shared" ref="D440:D450" si="14">"        "&amp;C440&amp;"="&amp;B440&amp;","</f>
+        <v xml:space="preserve">        WRITE_ONLY=438,</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B441" s="1">
         <f t="shared" si="13"/>
@@ -8918,16 +8915,16 @@
         <v>431</v>
       </c>
       <c r="D441" t="str">
-        <f t="shared" ref="D441:D451" si="14">"        "&amp;C441&amp;"="&amp;B441&amp;","</f>
-        <v xml:space="preserve">        WRITE_ONLY=439,</v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        XML_SCHEMA=439,</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B442" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="B442:B450" si="15">B441+1</f>
         <v>440</v>
       </c>
       <c r="C442" t="s">
@@ -8935,29 +8932,26 @@
       </c>
       <c r="D442" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        XML_SCHEMA=440,</v>
+        <v xml:space="preserve">        YYYYDDD=440,</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B443" s="1">
-        <f t="shared" ref="B443:B451" si="15">B442+1</f>
+        <f t="shared" si="15"/>
         <v>441</v>
       </c>
       <c r="C443" t="s">
-        <v>433</v>
+        <v>451</v>
       </c>
       <c r="D443" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYDDD=441,</v>
+        <v xml:space="preserve">        YYYYMMDD=441,</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A444" t="s">
-        <v>435</v>
-      </c>
       <c r="B444" s="1">
         <f t="shared" si="15"/>
         <v>442</v>
@@ -8967,7 +8961,7 @@
       </c>
       <c r="D444" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYMMDD=442,</v>
+        <v xml:space="preserve">        TYPEDEF=442,</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -8980,7 +8974,7 @@
       </c>
       <c r="D445" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        TYPEDEF=443,</v>
+        <v xml:space="preserve">        STRONG=443,</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8993,7 +8987,7 @@
       </c>
       <c r="D446" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRONG=444,</v>
+        <v xml:space="preserve">        UNSAFE=444,</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -9002,11 +8996,11 @@
         <v>445</v>
       </c>
       <c r="C447" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D447" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        UNSAFE=445,</v>
+        <v xml:space="preserve">        PUBLIC=445,</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -9019,7 +9013,7 @@
       </c>
       <c r="D448" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PUBLIC=446,</v>
+        <v xml:space="preserve">        PRIVATE=446,</v>
       </c>
     </row>
     <row r="449" spans="2:4" x14ac:dyDescent="0.25">
@@ -9028,11 +9022,11 @@
         <v>447</v>
       </c>
       <c r="C449" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="D449" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PRIVATE=447,</v>
+        <v xml:space="preserve">        IN_OUT=447,</v>
       </c>
     </row>
     <row r="450" spans="2:4" x14ac:dyDescent="0.25">
@@ -9045,33 +9039,33 @@
       </c>
       <c r="D450" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        IN_OUT=448,</v>
+        <v xml:space="preserve">        STRICT=448,</v>
       </c>
     </row>
     <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B451" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B451:B454" si="16">B450+1</f>
         <v>449</v>
       </c>
       <c r="C451" t="s">
         <v>468</v>
       </c>
       <c r="D451" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRICT=449,</v>
+        <f t="shared" ref="D451:D454" si="17">"        "&amp;C451&amp;"="&amp;B451&amp;","</f>
+        <v xml:space="preserve">        QuestionMark=449,</v>
       </c>
     </row>
     <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" s="1">
-        <f t="shared" ref="B452:B455" si="16">B451+1</f>
+        <f t="shared" si="16"/>
         <v>450</v>
       </c>
       <c r="C452" t="s">
         <v>469</v>
       </c>
       <c r="D452" t="str">
-        <f t="shared" ref="D452:D455" si="17">"        "&amp;C452&amp;"="&amp;B452&amp;","</f>
-        <v xml:space="preserve">        QuestionMark=450,</v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">        CompilerDirective=450,</v>
       </c>
     </row>
     <row r="453" spans="2:4" x14ac:dyDescent="0.25">
@@ -9084,7 +9078,7 @@
       </c>
       <c r="D453" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CompilerDirective=451,</v>
+        <v xml:space="preserve">        CopyImportDirective=451,</v>
       </c>
     </row>
     <row r="454" spans="2:4" x14ac:dyDescent="0.25">
@@ -9097,33 +9091,20 @@
       </c>
       <c r="D454" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CopyImportDirective=452,</v>
+        <v xml:space="preserve">        ReplaceDirective=452,</v>
       </c>
     </row>
     <row r="455" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B455" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="B455" si="18">B454+1</f>
         <v>453</v>
       </c>
       <c r="C455" t="s">
         <v>472</v>
       </c>
       <c r="D455" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        ReplaceDirective=453,</v>
-      </c>
-    </row>
-    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B456" s="1">
-        <f t="shared" ref="B456" si="18">B455+1</f>
-        <v>454</v>
-      </c>
-      <c r="C456" t="s">
-        <v>473</v>
-      </c>
-      <c r="D456" t="str">
-        <f t="shared" ref="D456" si="19">"        "&amp;C456&amp;"="&amp;B456&amp;","</f>
-        <v xml:space="preserve">        ContinuationTokenGroup=454,</v>
+        <f t="shared" ref="D455" si="19">"        "&amp;C455&amp;"="&amp;B455&amp;","</f>
+        <v xml:space="preserve">        ContinuationTokenGroup=453,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#578, remove NONNUMERIC Token, add predicate in Xml context
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="472">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -999,9 +999,6 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>NONNUMERIC</t>
   </si>
   <si>
     <t>NOT</t>
@@ -1854,10 +1851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D455"/>
+  <dimension ref="A1:D454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
-      <selection activeCell="A442" sqref="A442"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="H330" sqref="H330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,7 +1869,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B1" s="1">
         <v>-1</v>
@@ -1887,14 +1884,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B2" s="1">
         <f>B1+1</f>
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D2" t="str">
         <f>"        "&amp;C2&amp;"="&amp;B2&amp;","</f>
@@ -1903,7 +1900,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B3" s="1">
         <f>B2+1</f>
@@ -1919,7 +1916,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B67" si="1">B3+1</f>
@@ -1935,7 +1932,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="1"/>
@@ -1951,7 +1948,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="1"/>
@@ -1967,7 +1964,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="1"/>
@@ -1983,7 +1980,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="1"/>
@@ -1999,7 +1996,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="1"/>
@@ -2015,14 +2012,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2031,7 +2028,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="1"/>
@@ -2047,7 +2044,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="1"/>
@@ -2063,7 +2060,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="1"/>
@@ -2079,7 +2076,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
@@ -2095,7 +2092,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
@@ -2111,7 +2108,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
@@ -2127,7 +2124,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
@@ -2143,7 +2140,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
@@ -2159,7 +2156,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
@@ -2175,7 +2172,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="1"/>
@@ -2191,7 +2188,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="1"/>
@@ -2207,7 +2204,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="1"/>
@@ -2223,7 +2220,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="1"/>
@@ -2239,7 +2236,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="1"/>
@@ -2255,7 +2252,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="1"/>
@@ -2271,7 +2268,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="1"/>
@@ -2287,7 +2284,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="1"/>
@@ -2303,7 +2300,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="1"/>
@@ -2332,14 +2329,14 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2348,7 +2345,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" si="1"/>
@@ -2364,7 +2361,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="1"/>
@@ -2380,7 +2377,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" si="1"/>
@@ -2396,7 +2393,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" si="1"/>
@@ -2412,7 +2409,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" si="1"/>
@@ -2441,14 +2438,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2457,14 +2454,14 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2473,7 +2470,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="1"/>
@@ -2489,14 +2486,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2505,7 +2502,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="1"/>
@@ -2521,7 +2518,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" si="1"/>
@@ -2537,7 +2534,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" si="1"/>
@@ -2553,7 +2550,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="1"/>
@@ -2569,7 +2566,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" si="1"/>
@@ -2585,7 +2582,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" si="1"/>
@@ -2601,7 +2598,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" si="1"/>
@@ -2617,7 +2614,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" si="1"/>
@@ -2633,7 +2630,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B49" s="1">
         <f t="shared" si="1"/>
@@ -2649,7 +2646,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" si="1"/>
@@ -2665,7 +2662,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B51" s="1">
         <f t="shared" si="1"/>
@@ -2681,7 +2678,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" si="1"/>
@@ -2697,7 +2694,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B53" s="1">
         <f t="shared" si="1"/>
@@ -2713,7 +2710,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B54" s="1">
         <f t="shared" si="1"/>
@@ -2729,7 +2726,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B55" s="1">
         <f t="shared" si="1"/>
@@ -2745,14 +2742,14 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2761,7 +2758,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B57" s="1">
         <f t="shared" si="1"/>
@@ -2777,7 +2774,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B58" s="1">
         <f t="shared" si="1"/>
@@ -2793,7 +2790,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B59" s="1">
         <f t="shared" si="1"/>
@@ -2809,7 +2806,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B60" s="1">
         <f t="shared" si="1"/>
@@ -2825,7 +2822,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B61" s="1">
         <f t="shared" si="1"/>
@@ -2841,7 +2838,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B62" s="1">
         <f t="shared" si="1"/>
@@ -2857,7 +2854,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B63" s="1">
         <f t="shared" si="1"/>
@@ -2873,7 +2870,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B64" s="1">
         <f t="shared" si="1"/>
@@ -2889,7 +2886,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B65" s="1">
         <f t="shared" si="1"/>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B66" s="1">
         <f t="shared" si="1"/>
@@ -2921,7 +2918,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B67" s="1">
         <f t="shared" si="1"/>
@@ -2937,7 +2934,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B68" s="1">
         <f t="shared" ref="B68:B131" si="3">B67+1</f>
@@ -2953,7 +2950,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
@@ -2969,7 +2966,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
@@ -2985,7 +2982,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
@@ -3001,7 +2998,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
@@ -3017,14 +3014,14 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -3033,7 +3030,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
@@ -3049,7 +3046,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
@@ -3065,7 +3062,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
@@ -3081,7 +3078,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
@@ -3097,7 +3094,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
@@ -3113,7 +3110,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
@@ -3129,7 +3126,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B80" s="1">
         <f t="shared" si="3"/>
@@ -3145,7 +3142,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B81" s="1">
         <f t="shared" si="3"/>
@@ -3161,14 +3158,14 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B82" s="1">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3177,7 +3174,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B83" s="1">
         <f t="shared" si="3"/>
@@ -3193,7 +3190,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B84" s="1">
         <f t="shared" si="3"/>
@@ -3209,7 +3206,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B85" s="1">
         <f t="shared" si="3"/>
@@ -3225,7 +3222,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B86" s="1">
         <f t="shared" si="3"/>
@@ -3241,7 +3238,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B87" s="1">
         <f t="shared" si="3"/>
@@ -3257,7 +3254,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B88" s="1">
         <f t="shared" si="3"/>
@@ -3273,7 +3270,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B89" s="1">
         <f t="shared" si="3"/>
@@ -3289,7 +3286,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B90" s="1">
         <f t="shared" si="3"/>
@@ -3305,7 +3302,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B91" s="1">
         <f t="shared" si="3"/>
@@ -3321,7 +3318,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B92" s="1">
         <f t="shared" si="3"/>
@@ -3337,7 +3334,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B93" s="1">
         <f t="shared" si="3"/>
@@ -3353,7 +3350,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B94" s="1">
         <f t="shared" si="3"/>
@@ -3369,7 +3366,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B95" s="1">
         <f t="shared" si="3"/>
@@ -3385,7 +3382,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B96" s="1">
         <f t="shared" si="3"/>
@@ -3401,7 +3398,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B97" s="1">
         <f t="shared" si="3"/>
@@ -3417,7 +3414,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B98" s="1">
         <f t="shared" si="3"/>
@@ -3433,7 +3430,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B99" s="1">
         <f t="shared" si="3"/>
@@ -3449,7 +3446,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B100" s="1">
         <f t="shared" si="3"/>
@@ -3465,7 +3462,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B101" s="1">
         <f t="shared" si="3"/>
@@ -3481,7 +3478,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B102" s="1">
         <f t="shared" si="3"/>
@@ -3497,7 +3494,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B103" s="1">
         <f t="shared" si="3"/>
@@ -3513,7 +3510,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B104" s="1">
         <f t="shared" si="3"/>
@@ -3529,7 +3526,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B105" s="1">
         <f t="shared" si="3"/>
@@ -3545,7 +3542,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B106" s="1">
         <f t="shared" si="3"/>
@@ -3561,7 +3558,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B107" s="1">
         <f t="shared" si="3"/>
@@ -3577,7 +3574,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B108" s="1">
         <f t="shared" si="3"/>
@@ -3593,7 +3590,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B109" s="1">
         <f t="shared" si="3"/>
@@ -3609,7 +3606,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B110" s="1">
         <f t="shared" si="3"/>
@@ -3625,7 +3622,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B111" s="1">
         <f t="shared" si="3"/>
@@ -3641,7 +3638,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B112" s="1">
         <f t="shared" si="3"/>
@@ -3657,7 +3654,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B113" s="1">
         <f t="shared" si="3"/>
@@ -3673,7 +3670,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B114" s="1">
         <f t="shared" si="3"/>
@@ -3689,7 +3686,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B115" s="1">
         <f t="shared" si="3"/>
@@ -3705,7 +3702,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B116" s="1">
         <f t="shared" si="3"/>
@@ -3721,7 +3718,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B117" s="1">
         <f t="shared" si="3"/>
@@ -3737,7 +3734,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B118" s="1">
         <f t="shared" si="3"/>
@@ -3753,7 +3750,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B119" s="1">
         <f t="shared" si="3"/>
@@ -3769,7 +3766,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B120" s="1">
         <f t="shared" si="3"/>
@@ -3785,7 +3782,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B121" s="1">
         <f t="shared" si="3"/>
@@ -3801,7 +3798,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B122" s="1">
         <f t="shared" si="3"/>
@@ -3817,7 +3814,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B123" s="1">
         <f t="shared" si="3"/>
@@ -3833,7 +3830,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B124" s="1">
         <f t="shared" si="3"/>
@@ -3849,7 +3846,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B125" s="1">
         <f t="shared" si="3"/>
@@ -3865,7 +3862,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B126" s="1">
         <f t="shared" si="3"/>
@@ -3881,7 +3878,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B127" s="1">
         <f t="shared" si="3"/>
@@ -3897,7 +3894,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B128" s="1">
         <f t="shared" si="3"/>
@@ -3913,7 +3910,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B129" s="1">
         <f t="shared" si="3"/>
@@ -3929,14 +3926,14 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B130" s="1">
         <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="C130" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D130" t="str">
         <f t="shared" ref="D130:D193" si="4">"        "&amp;C130&amp;"="&amp;B130&amp;","</f>
@@ -3945,7 +3942,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B131" s="1">
         <f t="shared" si="3"/>
@@ -3961,7 +3958,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B132" s="1">
         <f t="shared" ref="B132:B195" si="5">B131+1</f>
@@ -3977,7 +3974,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B133" s="1">
         <f t="shared" si="5"/>
@@ -3993,7 +3990,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B134" s="1">
         <f t="shared" si="5"/>
@@ -4009,7 +4006,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B135" s="1">
         <f t="shared" si="5"/>
@@ -4025,7 +4022,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B136" s="1">
         <f t="shared" si="5"/>
@@ -4041,7 +4038,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B137" s="1">
         <f t="shared" si="5"/>
@@ -4057,7 +4054,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B138" s="1">
         <f t="shared" si="5"/>
@@ -4073,7 +4070,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B139" s="1">
         <f t="shared" si="5"/>
@@ -4089,7 +4086,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B140" s="1">
         <f t="shared" si="5"/>
@@ -4105,7 +4102,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B141" s="1">
         <f t="shared" si="5"/>
@@ -4121,7 +4118,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B142" s="1">
         <f t="shared" si="5"/>
@@ -4137,7 +4134,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B143" s="1">
         <f t="shared" si="5"/>
@@ -4153,7 +4150,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B144" s="1">
         <f t="shared" si="5"/>
@@ -4169,7 +4166,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B145" s="1">
         <f t="shared" si="5"/>
@@ -4185,7 +4182,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B146" s="1">
         <f t="shared" si="5"/>
@@ -4201,7 +4198,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B147" s="1">
         <f t="shared" si="5"/>
@@ -4217,7 +4214,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B148" s="1">
         <f t="shared" si="5"/>
@@ -4233,7 +4230,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B149" s="1">
         <f t="shared" si="5"/>
@@ -4249,7 +4246,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B150" s="1">
         <f t="shared" si="5"/>
@@ -4265,7 +4262,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B151" s="1">
         <f t="shared" si="5"/>
@@ -4281,14 +4278,14 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B152" s="1">
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="C152" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="4"/>
@@ -4297,7 +4294,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B153" s="1">
         <f t="shared" si="5"/>
@@ -4313,7 +4310,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B154" s="1">
         <f t="shared" si="5"/>
@@ -4329,7 +4326,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B155" s="1">
         <f t="shared" si="5"/>
@@ -4345,7 +4342,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B156" s="1">
         <f t="shared" si="5"/>
@@ -4361,7 +4358,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B157" s="1">
         <f t="shared" si="5"/>
@@ -4377,7 +4374,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B158" s="1">
         <f t="shared" si="5"/>
@@ -4393,7 +4390,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B159" s="1">
         <f t="shared" si="5"/>
@@ -4409,7 +4406,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B160" s="1">
         <f t="shared" si="5"/>
@@ -4425,7 +4422,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B161" s="1">
         <f t="shared" si="5"/>
@@ -4441,7 +4438,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B162" s="1">
         <f t="shared" si="5"/>
@@ -4457,7 +4454,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B163" s="1">
         <f t="shared" si="5"/>
@@ -4473,7 +4470,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B164" s="1">
         <f t="shared" si="5"/>
@@ -4489,7 +4486,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B165" s="1">
         <f t="shared" si="5"/>
@@ -4505,7 +4502,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B166" s="1">
         <f t="shared" si="5"/>
@@ -4521,7 +4518,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B167" s="1">
         <f t="shared" si="5"/>
@@ -4537,7 +4534,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B168" s="1">
         <f t="shared" si="5"/>
@@ -4553,7 +4550,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B169" s="1">
         <f t="shared" si="5"/>
@@ -4569,7 +4566,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B170" s="1">
         <f t="shared" si="5"/>
@@ -4585,7 +4582,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B171" s="1">
         <f t="shared" si="5"/>
@@ -4601,7 +4598,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B172" s="1">
         <f t="shared" si="5"/>
@@ -4617,7 +4614,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B173" s="1">
         <f t="shared" si="5"/>
@@ -4633,7 +4630,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B174" s="1">
         <f t="shared" si="5"/>
@@ -4649,7 +4646,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B175" s="1">
         <f t="shared" si="5"/>
@@ -4665,7 +4662,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B176" s="1">
         <f t="shared" si="5"/>
@@ -4681,7 +4678,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B177" s="1">
         <f t="shared" si="5"/>
@@ -4697,7 +4694,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B178" s="1">
         <f t="shared" si="5"/>
@@ -4713,7 +4710,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B179" s="1">
         <f t="shared" si="5"/>
@@ -4729,7 +4726,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B180" s="1">
         <f t="shared" si="5"/>
@@ -4745,7 +4742,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B181" s="1">
         <f t="shared" si="5"/>
@@ -4761,7 +4758,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B182" s="1">
         <f t="shared" si="5"/>
@@ -4777,7 +4774,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B183" s="1">
         <f>B182+1</f>
@@ -4793,7 +4790,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B184" s="1">
         <f t="shared" si="5"/>
@@ -4809,7 +4806,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B185" s="1">
         <f t="shared" si="5"/>
@@ -4825,7 +4822,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B186" s="1">
         <f t="shared" si="5"/>
@@ -4841,7 +4838,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B187" s="1">
         <f t="shared" si="5"/>
@@ -4857,7 +4854,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B188" s="1">
         <f t="shared" si="5"/>
@@ -4873,7 +4870,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B189" s="1">
         <f t="shared" si="5"/>
@@ -4889,7 +4886,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B190" s="1">
         <f t="shared" si="5"/>
@@ -4905,7 +4902,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B191" s="1">
         <f t="shared" si="5"/>
@@ -4921,7 +4918,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B192" s="1">
         <f t="shared" si="5"/>
@@ -4937,7 +4934,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B193" s="1">
         <f t="shared" si="5"/>
@@ -4953,7 +4950,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B194" s="1">
         <f t="shared" si="5"/>
@@ -4969,7 +4966,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B195" s="1">
         <f t="shared" si="5"/>
@@ -4985,7 +4982,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B196" s="1">
         <f t="shared" ref="B196:B257" si="7">B195+1</f>
@@ -5001,7 +4998,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B197" s="1">
         <f t="shared" si="7"/>
@@ -5017,7 +5014,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B198" s="1">
         <f t="shared" si="7"/>
@@ -5033,7 +5030,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B199" s="1">
         <f t="shared" si="7"/>
@@ -5049,7 +5046,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B200" s="1">
         <f t="shared" si="7"/>
@@ -5065,7 +5062,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B201" s="1">
         <f t="shared" si="7"/>
@@ -5081,7 +5078,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B202" s="1">
         <f t="shared" si="7"/>
@@ -5097,7 +5094,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B203" s="1">
         <f t="shared" si="7"/>
@@ -5113,7 +5110,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B204" s="1">
         <f t="shared" si="7"/>
@@ -5129,7 +5126,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B205" s="1">
         <f t="shared" si="7"/>
@@ -5145,7 +5142,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B206" s="1">
         <f t="shared" si="7"/>
@@ -5161,7 +5158,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B207" s="1">
         <f t="shared" si="7"/>
@@ -5177,7 +5174,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B208" s="1">
         <f t="shared" si="7"/>
@@ -5193,7 +5190,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B209" s="1">
         <f t="shared" si="7"/>
@@ -5209,7 +5206,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B210" s="1">
         <f t="shared" si="7"/>
@@ -5225,7 +5222,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B211" s="1">
         <f t="shared" si="7"/>
@@ -5241,7 +5238,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B212" s="1">
         <f t="shared" si="7"/>
@@ -5257,7 +5254,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B213" s="1">
         <f t="shared" si="7"/>
@@ -5273,7 +5270,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B214" s="1">
         <f t="shared" si="7"/>
@@ -5289,7 +5286,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B215" s="1">
         <f t="shared" si="7"/>
@@ -5305,7 +5302,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B216" s="1">
         <f t="shared" si="7"/>
@@ -5321,7 +5318,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B217" s="1">
         <f t="shared" si="7"/>
@@ -5337,7 +5334,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B218" s="1">
         <f t="shared" si="7"/>
@@ -5353,7 +5350,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B219" s="1">
         <f t="shared" si="7"/>
@@ -5369,7 +5366,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B220" s="1">
         <f t="shared" si="7"/>
@@ -5385,7 +5382,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B221" s="1">
         <f t="shared" si="7"/>
@@ -5401,7 +5398,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B222" s="1">
         <f t="shared" si="7"/>
@@ -5417,7 +5414,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B223" s="1">
         <f t="shared" si="7"/>
@@ -5433,7 +5430,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B224" s="1">
         <f t="shared" si="7"/>
@@ -5449,7 +5446,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B225" s="1">
         <f t="shared" si="7"/>
@@ -5465,7 +5462,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B226" s="1">
         <f t="shared" si="7"/>
@@ -5481,7 +5478,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B227" s="1">
         <f t="shared" si="7"/>
@@ -5497,7 +5494,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B228" s="1">
         <f t="shared" si="7"/>
@@ -5513,7 +5510,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B229" s="1">
         <f t="shared" si="7"/>
@@ -5529,7 +5526,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B230" s="1">
         <f t="shared" si="7"/>
@@ -5545,7 +5542,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B231" s="1">
         <f t="shared" si="7"/>
@@ -5561,7 +5558,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B232" s="1">
         <f t="shared" si="7"/>
@@ -5577,7 +5574,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B233" s="1">
         <f t="shared" si="7"/>
@@ -5593,7 +5590,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B234" s="1">
         <f t="shared" si="7"/>
@@ -5609,7 +5606,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B235" s="1">
         <f t="shared" si="7"/>
@@ -5625,7 +5622,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B236" s="1">
         <f t="shared" si="7"/>
@@ -5641,7 +5638,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B237" s="1">
         <f t="shared" si="7"/>
@@ -5657,7 +5654,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B238" s="1">
         <f t="shared" si="7"/>
@@ -5673,7 +5670,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B239" s="1">
         <f t="shared" si="7"/>
@@ -5689,7 +5686,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B240" s="1">
         <f t="shared" si="7"/>
@@ -5705,7 +5702,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B241" s="1">
         <f t="shared" si="7"/>
@@ -5721,7 +5718,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B242" s="1">
         <f t="shared" si="7"/>
@@ -5737,7 +5734,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B243" s="1">
         <f t="shared" si="7"/>
@@ -5753,7 +5750,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B244" s="1">
         <f t="shared" si="7"/>
@@ -5769,7 +5766,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B245" s="1">
         <f t="shared" si="7"/>
@@ -5785,7 +5782,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B246" s="1">
         <f t="shared" si="7"/>
@@ -5801,7 +5798,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B247" s="1">
         <f t="shared" si="7"/>
@@ -5817,7 +5814,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B248" s="1">
         <f t="shared" si="7"/>
@@ -5833,7 +5830,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B249" s="1">
         <f t="shared" si="7"/>
@@ -5849,7 +5846,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B250" s="1">
         <f t="shared" si="7"/>
@@ -5865,7 +5862,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B251" s="1">
         <f t="shared" si="7"/>
@@ -5881,7 +5878,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B252" s="1">
         <f t="shared" si="7"/>
@@ -5897,7 +5894,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B253" s="1">
         <f t="shared" si="7"/>
@@ -5913,7 +5910,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B254" s="1">
         <f t="shared" si="7"/>
@@ -5929,7 +5926,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B255" s="1">
         <f t="shared" si="7"/>
@@ -5945,7 +5942,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B256" s="1">
         <f t="shared" si="7"/>
@@ -5961,7 +5958,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B257" s="1">
         <f t="shared" si="7"/>
@@ -5977,7 +5974,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B258" s="1">
         <f t="shared" ref="B258:B319" si="9">B257+1</f>
@@ -5993,7 +5990,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B259" s="1">
         <f t="shared" si="9"/>
@@ -6009,7 +6006,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B260" s="1">
         <f t="shared" si="9"/>
@@ -6025,7 +6022,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B261" s="1">
         <f t="shared" si="9"/>
@@ -6041,7 +6038,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B262" s="1">
         <f t="shared" si="9"/>
@@ -6057,7 +6054,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B263" s="1">
         <f t="shared" si="9"/>
@@ -6073,7 +6070,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B264" s="1">
         <f t="shared" si="9"/>
@@ -6089,7 +6086,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B265" s="1">
         <f t="shared" si="9"/>
@@ -6105,7 +6102,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B266" s="1">
         <f t="shared" si="9"/>
@@ -6121,7 +6118,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B267" s="1">
         <f t="shared" si="9"/>
@@ -6137,7 +6134,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B268" s="1">
         <f t="shared" si="9"/>
@@ -6153,7 +6150,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B269" s="1">
         <f t="shared" si="9"/>
@@ -6169,7 +6166,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B270" s="1">
         <f t="shared" si="9"/>
@@ -6185,7 +6182,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B271" s="1">
         <f t="shared" si="9"/>
@@ -6201,7 +6198,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B272" s="1">
         <f t="shared" si="9"/>
@@ -6217,7 +6214,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B273" s="1">
         <f t="shared" si="9"/>
@@ -6233,7 +6230,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B274" s="1">
         <f t="shared" si="9"/>
@@ -6249,7 +6246,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B275" s="1">
         <f t="shared" si="9"/>
@@ -6265,7 +6262,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B276" s="1">
         <f t="shared" si="9"/>
@@ -6281,7 +6278,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B277" s="1">
         <f t="shared" si="9"/>
@@ -6297,7 +6294,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B278" s="1">
         <f t="shared" si="9"/>
@@ -6313,7 +6310,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B279" s="1">
         <f t="shared" si="9"/>
@@ -6329,7 +6326,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B280" s="1">
         <f t="shared" si="9"/>
@@ -6345,7 +6342,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B281" s="1">
         <f t="shared" si="9"/>
@@ -6361,7 +6358,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B282" s="1">
         <f t="shared" si="9"/>
@@ -6377,7 +6374,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B283" s="1">
         <f t="shared" si="9"/>
@@ -6393,7 +6390,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B284" s="1">
         <f t="shared" si="9"/>
@@ -6409,7 +6406,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B285" s="1">
         <f t="shared" si="9"/>
@@ -6425,7 +6422,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B286" s="1">
         <f t="shared" si="9"/>
@@ -6441,7 +6438,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B287" s="1">
         <f t="shared" si="9"/>
@@ -6457,7 +6454,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B288" s="1">
         <f t="shared" si="9"/>
@@ -6473,7 +6470,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B289" s="1">
         <f t="shared" si="9"/>
@@ -6489,7 +6486,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B290" s="1">
         <f t="shared" si="9"/>
@@ -6505,7 +6502,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B291" s="1">
         <f t="shared" si="9"/>
@@ -6521,7 +6518,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B292" s="1">
         <f t="shared" si="9"/>
@@ -6537,7 +6534,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B293" s="1">
         <f t="shared" si="9"/>
@@ -6553,7 +6550,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B294" s="1">
         <f t="shared" si="9"/>
@@ -6569,7 +6566,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B295" s="1">
         <f t="shared" si="9"/>
@@ -6585,7 +6582,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B296" s="1">
         <f t="shared" si="9"/>
@@ -6601,7 +6598,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B297" s="1">
         <f t="shared" si="9"/>
@@ -6617,7 +6614,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B298" s="1">
         <f t="shared" si="9"/>
@@ -6633,7 +6630,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B299" s="1">
         <f t="shared" si="9"/>
@@ -6649,7 +6646,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B300" s="1">
         <f t="shared" si="9"/>
@@ -6665,7 +6662,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B301" s="1">
         <f t="shared" si="9"/>
@@ -6681,7 +6678,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B302" s="1">
         <f t="shared" si="9"/>
@@ -6697,7 +6694,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B303" s="1">
         <f t="shared" si="9"/>
@@ -6713,7 +6710,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B304" s="1">
         <f t="shared" si="9"/>
@@ -6729,7 +6726,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B305" s="1">
         <f t="shared" si="9"/>
@@ -6745,7 +6742,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B306" s="1">
         <f t="shared" si="9"/>
@@ -6761,7 +6758,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B307" s="1">
         <f t="shared" si="9"/>
@@ -6777,7 +6774,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B308" s="1">
         <f t="shared" si="9"/>
@@ -6793,7 +6790,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B309" s="1">
         <f t="shared" si="9"/>
@@ -6809,7 +6806,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B310" s="1">
         <f t="shared" si="9"/>
@@ -6825,7 +6822,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B311" s="1">
         <f t="shared" si="9"/>
@@ -6841,7 +6838,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B312" s="1">
         <f t="shared" si="9"/>
@@ -6857,7 +6854,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B313" s="1">
         <f t="shared" si="9"/>
@@ -6873,7 +6870,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B314" s="1">
         <f t="shared" si="9"/>
@@ -6889,7 +6886,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B315" s="1">
         <f t="shared" si="9"/>
@@ -6905,7 +6902,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B316" s="1">
         <f t="shared" si="9"/>
@@ -6921,7 +6918,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B317" s="1">
         <f t="shared" si="9"/>
@@ -6931,13 +6928,13 @@
         <v>304</v>
       </c>
       <c r="D317" t="str">
-        <f t="shared" ref="D317:D376" si="10">"        "&amp;C317&amp;"="&amp;B317&amp;","</f>
+        <f t="shared" ref="D317:D375" si="10">"        "&amp;C317&amp;"="&amp;B317&amp;","</f>
         <v xml:space="preserve">        LABEL=315,</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B318" s="1">
         <f t="shared" si="9"/>
@@ -6953,7 +6950,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B319" s="1">
         <f t="shared" si="9"/>
@@ -6969,10 +6966,10 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B320" s="1">
-        <f t="shared" ref="B320:B379" si="11">B319+1</f>
+        <f t="shared" ref="B320:B378" si="11">B319+1</f>
         <v>318</v>
       </c>
       <c r="C320" t="s">
@@ -6985,7 +6982,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B321" s="1">
         <f t="shared" si="11"/>
@@ -7001,7 +6998,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B322" s="1">
         <f t="shared" si="11"/>
@@ -7017,7 +7014,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B323" s="1">
         <f t="shared" si="11"/>
@@ -7033,7 +7030,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B324" s="1">
         <f t="shared" si="11"/>
@@ -7049,7 +7046,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B325" s="1">
         <f t="shared" si="11"/>
@@ -7065,7 +7062,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B326" s="1">
         <f t="shared" si="11"/>
@@ -7081,7 +7078,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B327" s="1">
         <f t="shared" si="11"/>
@@ -7097,7 +7094,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B328" s="1">
         <f t="shared" si="11"/>
@@ -7113,7 +7110,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B329" s="1">
         <f t="shared" si="11"/>
@@ -7129,7 +7126,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B330" s="1">
         <f t="shared" si="11"/>
@@ -7145,7 +7142,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B331" s="1">
         <f t="shared" si="11"/>
@@ -7161,7 +7158,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B332" s="1">
         <f t="shared" si="11"/>
@@ -7177,7 +7174,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B333" s="1">
         <f t="shared" si="11"/>
@@ -7193,7 +7190,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B334" s="1">
         <f t="shared" si="11"/>
@@ -7209,7 +7206,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B335" s="1">
         <f t="shared" si="11"/>
@@ -7225,7 +7222,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B336" s="1">
         <f t="shared" si="11"/>
@@ -7241,7 +7238,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B337" s="1">
         <f t="shared" si="11"/>
@@ -7252,12 +7249,12 @@
       </c>
       <c r="D337" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        NONNUMERIC=335,</v>
+        <v xml:space="preserve">        NOT=335,</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B338" s="1">
         <f t="shared" si="11"/>
@@ -7268,12 +7265,12 @@
       </c>
       <c r="D338" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        NOT=336,</v>
+        <v xml:space="preserve">        NUMERIC=336,</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B339" s="1">
         <f t="shared" si="11"/>
@@ -7284,12 +7281,12 @@
       </c>
       <c r="D339" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        NUMERIC=337,</v>
+        <v xml:space="preserve">        NUMERIC_EDITED=337,</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B340" s="1">
         <f t="shared" si="11"/>
@@ -7300,12 +7297,12 @@
       </c>
       <c r="D340" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        NUMERIC_EDITED=338,</v>
+        <v xml:space="preserve">        OBJECT=338,</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B341" s="1">
         <f t="shared" si="11"/>
@@ -7316,12 +7313,12 @@
       </c>
       <c r="D341" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OBJECT=339,</v>
+        <v xml:space="preserve">        OCCURS=339,</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B342" s="1">
         <f t="shared" si="11"/>
@@ -7332,12 +7329,12 @@
       </c>
       <c r="D342" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OCCURS=340,</v>
+        <v xml:space="preserve">        OF=340,</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B343" s="1">
         <f t="shared" si="11"/>
@@ -7348,12 +7345,12 @@
       </c>
       <c r="D343" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OF=341,</v>
+        <v xml:space="preserve">        OFF=341,</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B344" s="1">
         <f t="shared" si="11"/>
@@ -7364,12 +7361,12 @@
       </c>
       <c r="D344" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OFF=342,</v>
+        <v xml:space="preserve">        OMITTED=342,</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B345" s="1">
         <f t="shared" si="11"/>
@@ -7380,12 +7377,12 @@
       </c>
       <c r="D345" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OMITTED=343,</v>
+        <v xml:space="preserve">        ON=343,</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B346" s="1">
         <f t="shared" si="11"/>
@@ -7396,12 +7393,12 @@
       </c>
       <c r="D346" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        ON=344,</v>
+        <v xml:space="preserve">        OPTIONAL=344,</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B347" s="1">
         <f t="shared" si="11"/>
@@ -7412,12 +7409,12 @@
       </c>
       <c r="D347" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OPTIONAL=345,</v>
+        <v xml:space="preserve">        OR=345,</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B348" s="1">
         <f t="shared" si="11"/>
@@ -7428,12 +7425,12 @@
       </c>
       <c r="D348" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OR=346,</v>
+        <v xml:space="preserve">        ORDER=346,</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B349" s="1">
         <f t="shared" si="11"/>
@@ -7444,12 +7441,12 @@
       </c>
       <c r="D349" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        ORDER=347,</v>
+        <v xml:space="preserve">        ORGANIZATION=347,</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B350" s="1">
         <f t="shared" si="11"/>
@@ -7460,12 +7457,12 @@
       </c>
       <c r="D350" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        ORGANIZATION=348,</v>
+        <v xml:space="preserve">        OTHER=348,</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B351" s="1">
         <f t="shared" si="11"/>
@@ -7476,12 +7473,12 @@
       </c>
       <c r="D351" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OTHER=349,</v>
+        <v xml:space="preserve">        OUTPUT=349,</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B352" s="1">
         <f t="shared" si="11"/>
@@ -7492,12 +7489,12 @@
       </c>
       <c r="D352" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OUTPUT=350,</v>
+        <v xml:space="preserve">        OVERFLOW=350,</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B353" s="1">
         <f t="shared" si="11"/>
@@ -7508,12 +7505,12 @@
       </c>
       <c r="D353" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OVERFLOW=351,</v>
+        <v xml:space="preserve">        OVERRIDE=351,</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B354" s="1">
         <f t="shared" si="11"/>
@@ -7524,12 +7521,12 @@
       </c>
       <c r="D354" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        OVERRIDE=352,</v>
+        <v xml:space="preserve">        PACKED_DECIMAL=352,</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B355" s="1">
         <f t="shared" si="11"/>
@@ -7540,12 +7537,12 @@
       </c>
       <c r="D355" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PACKED_DECIMAL=353,</v>
+        <v xml:space="preserve">        PADDING=353,</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B356" s="1">
         <f t="shared" si="11"/>
@@ -7556,12 +7553,12 @@
       </c>
       <c r="D356" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PADDING=354,</v>
+        <v xml:space="preserve">        PAGE=354,</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B357" s="1">
         <f t="shared" si="11"/>
@@ -7572,12 +7569,12 @@
       </c>
       <c r="D357" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PAGE=355,</v>
+        <v xml:space="preserve">        PASSWORD=355,</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B358" s="1">
         <f t="shared" si="11"/>
@@ -7588,12 +7585,12 @@
       </c>
       <c r="D358" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PASSWORD=356,</v>
+        <v xml:space="preserve">        PIC=356,</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B359" s="1">
         <f t="shared" si="11"/>
@@ -7604,12 +7601,12 @@
       </c>
       <c r="D359" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PIC=357,</v>
+        <v xml:space="preserve">        PICTURE=357,</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B360" s="1">
         <f t="shared" si="11"/>
@@ -7620,12 +7617,12 @@
       </c>
       <c r="D360" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PICTURE=358,</v>
+        <v xml:space="preserve">        POINTER=358,</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B361" s="1">
         <f t="shared" si="11"/>
@@ -7636,12 +7633,12 @@
       </c>
       <c r="D361" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        POINTER=359,</v>
+        <v xml:space="preserve">        POSITION=359,</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B362" s="1">
         <f t="shared" si="11"/>
@@ -7652,28 +7649,28 @@
       </c>
       <c r="D362" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        POSITION=360,</v>
+        <v xml:space="preserve">        POSITIVE=360,</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B363" s="1">
         <f t="shared" si="11"/>
         <v>361</v>
       </c>
       <c r="C363" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D363" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        POSITIVE=361,</v>
+        <v xml:space="preserve">        PROCEDURE_POINTER=361,</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B364" s="1">
         <f t="shared" si="11"/>
@@ -7684,12 +7681,12 @@
       </c>
       <c r="D364" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCEDURE_POINTER=362,</v>
+        <v xml:space="preserve">        PROCEDURES=362,</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B365" s="1">
         <f t="shared" si="11"/>
@@ -7700,12 +7697,12 @@
       </c>
       <c r="D365" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCEDURES=363,</v>
+        <v xml:space="preserve">        PROCEED=363,</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B366" s="1">
         <f t="shared" si="11"/>
@@ -7716,12 +7713,12 @@
       </c>
       <c r="D366" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCEED=364,</v>
+        <v xml:space="preserve">        PROCESSING=364,</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B367" s="1">
         <f t="shared" si="11"/>
@@ -7732,12 +7729,12 @@
       </c>
       <c r="D367" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROCESSING=365,</v>
+        <v xml:space="preserve">        PROGRAM=365,</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B368" s="1">
         <f t="shared" si="11"/>
@@ -7748,12 +7745,12 @@
       </c>
       <c r="D368" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROGRAM=366,</v>
+        <v xml:space="preserve">        PROGRAM_ID=366,</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B369" s="1">
         <f t="shared" si="11"/>
@@ -7764,12 +7761,12 @@
       </c>
       <c r="D369" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        PROGRAM_ID=367,</v>
+        <v xml:space="preserve">        RANDOM=367,</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B370" s="1">
         <f t="shared" si="11"/>
@@ -7780,12 +7777,12 @@
       </c>
       <c r="D370" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RANDOM=368,</v>
+        <v xml:space="preserve">        RECORD=368,</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B371" s="1">
         <f t="shared" si="11"/>
@@ -7796,12 +7793,12 @@
       </c>
       <c r="D371" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECORD=369,</v>
+        <v xml:space="preserve">        RECORDING=369,</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B372" s="1">
         <f t="shared" si="11"/>
@@ -7812,12 +7809,12 @@
       </c>
       <c r="D372" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECORDING=370,</v>
+        <v xml:space="preserve">        RECORDS=370,</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B373" s="1">
         <f t="shared" si="11"/>
@@ -7828,12 +7825,12 @@
       </c>
       <c r="D373" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECORDS=371,</v>
+        <v xml:space="preserve">        RECURSIVE=371,</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B374" s="1">
         <f t="shared" si="11"/>
@@ -7844,12 +7841,12 @@
       </c>
       <c r="D374" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        RECURSIVE=372,</v>
+        <v xml:space="preserve">        REDEFINES=372,</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B375" s="1">
         <f t="shared" si="11"/>
@@ -7860,12 +7857,12 @@
       </c>
       <c r="D375" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">        REDEFINES=373,</v>
+        <v xml:space="preserve">        REEL=373,</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B376" s="1">
         <f t="shared" si="11"/>
@@ -7875,13 +7872,13 @@
         <v>365</v>
       </c>
       <c r="D376" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">        REEL=374,</v>
+        <f t="shared" ref="D376:D438" si="12">"        "&amp;C376&amp;"="&amp;B376&amp;","</f>
+        <v xml:space="preserve">        REFERENCE=374,</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B377" s="1">
         <f t="shared" si="11"/>
@@ -7891,13 +7888,13 @@
         <v>366</v>
       </c>
       <c r="D377" t="str">
-        <f t="shared" ref="D377:D439" si="12">"        "&amp;C377&amp;"="&amp;B377&amp;","</f>
-        <v xml:space="preserve">        REFERENCE=375,</v>
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">        REFERENCES=375,</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B378" s="1">
         <f t="shared" si="11"/>
@@ -7908,15 +7905,15 @@
       </c>
       <c r="D378" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REFERENCES=376,</v>
+        <v xml:space="preserve">        RELATIVE=376,</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B379" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="B379:B440" si="13">B378+1</f>
         <v>377</v>
       </c>
       <c r="C379" t="s">
@@ -7924,15 +7921,15 @@
       </c>
       <c r="D379" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RELATIVE=377,</v>
+        <v xml:space="preserve">        RELOAD=377,</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B380" s="1">
-        <f t="shared" ref="B380:B441" si="13">B379+1</f>
+        <f t="shared" si="13"/>
         <v>378</v>
       </c>
       <c r="C380" t="s">
@@ -7940,12 +7937,12 @@
       </c>
       <c r="D380" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RELOAD=378,</v>
+        <v xml:space="preserve">        REMAINDER=378,</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B381" s="1">
         <f t="shared" si="13"/>
@@ -7956,12 +7953,12 @@
       </c>
       <c r="D381" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REMAINDER=379,</v>
+        <v xml:space="preserve">        REMOVAL=379,</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B382" s="1">
         <f t="shared" si="13"/>
@@ -7972,12 +7969,12 @@
       </c>
       <c r="D382" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REMOVAL=380,</v>
+        <v xml:space="preserve">        RENAMES=380,</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B383" s="1">
         <f t="shared" si="13"/>
@@ -7988,12 +7985,12 @@
       </c>
       <c r="D383" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RENAMES=381,</v>
+        <v xml:space="preserve">        REPLACING=381,</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B384" s="1">
         <f t="shared" si="13"/>
@@ -8004,12 +8001,12 @@
       </c>
       <c r="D384" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REPLACING=382,</v>
+        <v xml:space="preserve">        RESERVE=382,</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B385" s="1">
         <f t="shared" si="13"/>
@@ -8020,12 +8017,12 @@
       </c>
       <c r="D385" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RESERVE=383,</v>
+        <v xml:space="preserve">        RETURNING=383,</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B386" s="1">
         <f t="shared" si="13"/>
@@ -8036,12 +8033,12 @@
       </c>
       <c r="D386" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RETURNING=384,</v>
+        <v xml:space="preserve">        REVERSED=384,</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B387" s="1">
         <f t="shared" si="13"/>
@@ -8052,12 +8049,12 @@
       </c>
       <c r="D387" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REVERSED=385,</v>
+        <v xml:space="preserve">        REWIND=385,</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B388" s="1">
         <f t="shared" si="13"/>
@@ -8068,12 +8065,12 @@
       </c>
       <c r="D388" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        REWIND=386,</v>
+        <v xml:space="preserve">        RIGHT=386,</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B389" s="1">
         <f t="shared" si="13"/>
@@ -8084,12 +8081,12 @@
       </c>
       <c r="D389" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RIGHT=387,</v>
+        <v xml:space="preserve">        ROUNDED=387,</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B390" s="1">
         <f t="shared" si="13"/>
@@ -8100,12 +8097,12 @@
       </c>
       <c r="D390" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        ROUNDED=388,</v>
+        <v xml:space="preserve">        RUN=388,</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B391" s="1">
         <f t="shared" si="13"/>
@@ -8116,12 +8113,12 @@
       </c>
       <c r="D391" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        RUN=389,</v>
+        <v xml:space="preserve">        SECTION=389,</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B392" s="1">
         <f t="shared" si="13"/>
@@ -8132,12 +8129,12 @@
       </c>
       <c r="D392" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SECTION=390,</v>
+        <v xml:space="preserve">        SECURITY=390,</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B393" s="1">
         <f t="shared" si="13"/>
@@ -8148,12 +8145,12 @@
       </c>
       <c r="D393" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SECURITY=391,</v>
+        <v xml:space="preserve">        SEGMENT_LIMIT=391,</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B394" s="1">
         <f t="shared" si="13"/>
@@ -8164,12 +8161,12 @@
       </c>
       <c r="D394" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEGMENT_LIMIT=392,</v>
+        <v xml:space="preserve">        SENTENCE=392,</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B395" s="1">
         <f t="shared" si="13"/>
@@ -8180,12 +8177,12 @@
       </c>
       <c r="D395" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SENTENCE=393,</v>
+        <v xml:space="preserve">        SEPARATE=393,</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B396" s="1">
         <f t="shared" si="13"/>
@@ -8196,12 +8193,12 @@
       </c>
       <c r="D396" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEPARATE=394,</v>
+        <v xml:space="preserve">        SEQUENCE=394,</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B397" s="1">
         <f t="shared" si="13"/>
@@ -8212,12 +8209,12 @@
       </c>
       <c r="D397" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEQUENCE=395,</v>
+        <v xml:space="preserve">        SEQUENTIAL=395,</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B398" s="1">
         <f t="shared" si="13"/>
@@ -8228,12 +8225,12 @@
       </c>
       <c r="D398" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SEQUENTIAL=396,</v>
+        <v xml:space="preserve">        SIGN=396,</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B399" s="1">
         <f t="shared" si="13"/>
@@ -8244,12 +8241,12 @@
       </c>
       <c r="D399" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SIGN=397,</v>
+        <v xml:space="preserve">        SIZE=397,</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B400" s="1">
         <f t="shared" si="13"/>
@@ -8260,12 +8257,12 @@
       </c>
       <c r="D400" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SIZE=398,</v>
+        <v xml:space="preserve">        SORT_MERGE=398,</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B401" s="1">
         <f t="shared" si="13"/>
@@ -8276,12 +8273,12 @@
       </c>
       <c r="D401" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SORT_MERGE=399,</v>
+        <v xml:space="preserve">        SQL=399,</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B402" s="1">
         <f t="shared" si="13"/>
@@ -8292,12 +8289,12 @@
       </c>
       <c r="D402" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SQL=400,</v>
+        <v xml:space="preserve">        SQLIMS=400,</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B403" s="1">
         <f t="shared" si="13"/>
@@ -8308,12 +8305,12 @@
       </c>
       <c r="D403" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SQLIMS=401,</v>
+        <v xml:space="preserve">        STANDARD=401,</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B404" s="1">
         <f t="shared" si="13"/>
@@ -8324,12 +8321,12 @@
       </c>
       <c r="D404" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STANDARD=402,</v>
+        <v xml:space="preserve">        STANDARD_1=402,</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B405" s="1">
         <f t="shared" si="13"/>
@@ -8340,12 +8337,12 @@
       </c>
       <c r="D405" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STANDARD_1=403,</v>
+        <v xml:space="preserve">        STANDARD_2=403,</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B406" s="1">
         <f t="shared" si="13"/>
@@ -8356,12 +8353,12 @@
       </c>
       <c r="D406" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STANDARD_2=404,</v>
+        <v xml:space="preserve">        STATUS=404,</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B407" s="1">
         <f t="shared" si="13"/>
@@ -8372,12 +8369,12 @@
       </c>
       <c r="D407" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        STATUS=405,</v>
+        <v xml:space="preserve">        SUPPRESS=405,</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B408" s="1">
         <f t="shared" si="13"/>
@@ -8388,12 +8385,12 @@
       </c>
       <c r="D408" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SUPPRESS=406,</v>
+        <v xml:space="preserve">        SYMBOL=406,</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B409" s="1">
         <f t="shared" si="13"/>
@@ -8404,12 +8401,12 @@
       </c>
       <c r="D409" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYMBOL=407,</v>
+        <v xml:space="preserve">        SYMBOLIC=407,</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B410" s="1">
         <f t="shared" si="13"/>
@@ -8420,12 +8417,12 @@
       </c>
       <c r="D410" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYMBOLIC=408,</v>
+        <v xml:space="preserve">        SYNC=408,</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B411" s="1">
         <f t="shared" si="13"/>
@@ -8436,12 +8433,12 @@
       </c>
       <c r="D411" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYNC=409,</v>
+        <v xml:space="preserve">        SYNCHRONIZED=409,</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B412" s="1">
         <f t="shared" si="13"/>
@@ -8452,12 +8449,12 @@
       </c>
       <c r="D412" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        SYNCHRONIZED=410,</v>
+        <v xml:space="preserve">        TALLYING=410,</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B413" s="1">
         <f t="shared" si="13"/>
@@ -8468,12 +8465,12 @@
       </c>
       <c r="D413" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TALLYING=411,</v>
+        <v xml:space="preserve">        TAPE=411,</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B414" s="1">
         <f t="shared" si="13"/>
@@ -8484,12 +8481,12 @@
       </c>
       <c r="D414" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TAPE=412,</v>
+        <v xml:space="preserve">        TEST=412,</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B415" s="1">
         <f t="shared" si="13"/>
@@ -8500,12 +8497,12 @@
       </c>
       <c r="D415" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TEST=413,</v>
+        <v xml:space="preserve">        THAN=413,</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B416" s="1">
         <f t="shared" si="13"/>
@@ -8516,12 +8513,12 @@
       </c>
       <c r="D416" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THAN=414,</v>
+        <v xml:space="preserve">        THEN=414,</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B417" s="1">
         <f t="shared" si="13"/>
@@ -8532,12 +8529,12 @@
       </c>
       <c r="D417" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THEN=415,</v>
+        <v xml:space="preserve">        THROUGH=415,</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B418" s="1">
         <f t="shared" si="13"/>
@@ -8548,12 +8545,12 @@
       </c>
       <c r="D418" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THROUGH=416,</v>
+        <v xml:space="preserve">        THRU=416,</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B419" s="1">
         <f t="shared" si="13"/>
@@ -8564,12 +8561,12 @@
       </c>
       <c r="D419" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        THRU=417,</v>
+        <v xml:space="preserve">        TIME=417,</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B420" s="1">
         <f t="shared" si="13"/>
@@ -8580,12 +8577,12 @@
       </c>
       <c r="D420" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TIME=418,</v>
+        <v xml:space="preserve">        TIMES=418,</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B421" s="1">
         <f t="shared" si="13"/>
@@ -8596,12 +8593,12 @@
       </c>
       <c r="D421" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TIMES=419,</v>
+        <v xml:space="preserve">        TO=419,</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B422" s="1">
         <f t="shared" si="13"/>
@@ -8612,12 +8609,12 @@
       </c>
       <c r="D422" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TO=420,</v>
+        <v xml:space="preserve">        TOP=420,</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B423" s="1">
         <f t="shared" si="13"/>
@@ -8628,12 +8625,12 @@
       </c>
       <c r="D423" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TOP=421,</v>
+        <v xml:space="preserve">        TRACE=421,</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B424" s="1">
         <f t="shared" si="13"/>
@@ -8644,12 +8641,12 @@
       </c>
       <c r="D424" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TRACE=422,</v>
+        <v xml:space="preserve">        TRAILING=422,</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B425" s="1">
         <f t="shared" si="13"/>
@@ -8660,12 +8657,12 @@
       </c>
       <c r="D425" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TRAILING=423,</v>
+        <v xml:space="preserve">        TRUE=423,</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B426" s="1">
         <f t="shared" si="13"/>
@@ -8676,12 +8673,12 @@
       </c>
       <c r="D426" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TRUE=424,</v>
+        <v xml:space="preserve">        TYPE=424,</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B427" s="1">
         <f t="shared" si="13"/>
@@ -8692,12 +8689,12 @@
       </c>
       <c r="D427" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        TYPE=425,</v>
+        <v xml:space="preserve">        UNBOUNDED=425,</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B428" s="1">
         <f t="shared" si="13"/>
@@ -8708,12 +8705,12 @@
       </c>
       <c r="D428" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UNBOUNDED=426,</v>
+        <v xml:space="preserve">        UNIT=426,</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B429" s="1">
         <f t="shared" si="13"/>
@@ -8724,12 +8721,12 @@
       </c>
       <c r="D429" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UNIT=427,</v>
+        <v xml:space="preserve">        UNTIL=427,</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B430" s="1">
         <f t="shared" si="13"/>
@@ -8740,12 +8737,12 @@
       </c>
       <c r="D430" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UNTIL=428,</v>
+        <v xml:space="preserve">        UP=428,</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B431" s="1">
         <f t="shared" si="13"/>
@@ -8756,12 +8753,12 @@
       </c>
       <c r="D431" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UP=429,</v>
+        <v xml:space="preserve">        UPON=429,</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B432" s="1">
         <f t="shared" si="13"/>
@@ -8772,12 +8769,12 @@
       </c>
       <c r="D432" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        UPON=430,</v>
+        <v xml:space="preserve">        USAGE=430,</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B433" s="1">
         <f t="shared" si="13"/>
@@ -8788,12 +8785,12 @@
       </c>
       <c r="D433" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        USAGE=431,</v>
+        <v xml:space="preserve">        USING=431,</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B434" s="1">
         <f t="shared" si="13"/>
@@ -8804,12 +8801,12 @@
       </c>
       <c r="D434" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        USING=432,</v>
+        <v xml:space="preserve">        VALUE=432,</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B435" s="1">
         <f t="shared" si="13"/>
@@ -8820,12 +8817,12 @@
       </c>
       <c r="D435" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALUE=433,</v>
+        <v xml:space="preserve">        VALUES=433,</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B436" s="1">
         <f t="shared" si="13"/>
@@ -8836,28 +8833,28 @@
       </c>
       <c r="D436" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VALUES=434,</v>
+        <v xml:space="preserve">        VARYING=434,</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B437" s="1">
         <f t="shared" si="13"/>
         <v>435</v>
       </c>
       <c r="C437" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D437" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        VARYING=435,</v>
+        <v xml:space="preserve">        WITH=435,</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B438" s="1">
         <f t="shared" si="13"/>
@@ -8868,12 +8865,12 @@
       </c>
       <c r="D438" t="str">
         <f t="shared" si="12"/>
-        <v xml:space="preserve">        WITH=436,</v>
+        <v xml:space="preserve">        WORDS=436,</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B439" s="1">
         <f t="shared" si="13"/>
@@ -8883,13 +8880,13 @@
         <v>429</v>
       </c>
       <c r="D439" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">        WORDS=437,</v>
+        <f t="shared" ref="D439:D449" si="14">"        "&amp;C439&amp;"="&amp;B439&amp;","</f>
+        <v xml:space="preserve">        WRITE_ONLY=437,</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B440" s="1">
         <f t="shared" si="13"/>
@@ -8899,16 +8896,16 @@
         <v>430</v>
       </c>
       <c r="D440" t="str">
-        <f t="shared" ref="D440:D450" si="14">"        "&amp;C440&amp;"="&amp;B440&amp;","</f>
-        <v xml:space="preserve">        WRITE_ONLY=438,</v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        XML_SCHEMA=438,</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B441" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="B441:B449" si="15">B440+1</f>
         <v>439</v>
       </c>
       <c r="C441" t="s">
@@ -8916,29 +8913,26 @@
       </c>
       <c r="D441" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        XML_SCHEMA=439,</v>
+        <v xml:space="preserve">        YYYYDDD=439,</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B442" s="1">
-        <f t="shared" ref="B442:B450" si="15">B441+1</f>
+        <f t="shared" si="15"/>
         <v>440</v>
       </c>
       <c r="C442" t="s">
-        <v>432</v>
+        <v>450</v>
       </c>
       <c r="D442" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYDDD=440,</v>
+        <v xml:space="preserve">        YYYYMMDD=440,</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A443" t="s">
-        <v>434</v>
-      </c>
       <c r="B443" s="1">
         <f t="shared" si="15"/>
         <v>441</v>
@@ -8948,7 +8942,7 @@
       </c>
       <c r="D443" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYMMDD=441,</v>
+        <v xml:space="preserve">        TYPEDEF=441,</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
@@ -8961,7 +8955,7 @@
       </c>
       <c r="D444" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        TYPEDEF=442,</v>
+        <v xml:space="preserve">        STRONG=442,</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -8974,7 +8968,7 @@
       </c>
       <c r="D445" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRONG=443,</v>
+        <v xml:space="preserve">        UNSAFE=443,</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8983,11 +8977,11 @@
         <v>444</v>
       </c>
       <c r="C446" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D446" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        UNSAFE=444,</v>
+        <v xml:space="preserve">        PUBLIC=444,</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -9000,7 +8994,7 @@
       </c>
       <c r="D447" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PUBLIC=445,</v>
+        <v xml:space="preserve">        PRIVATE=445,</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -9009,11 +9003,11 @@
         <v>446</v>
       </c>
       <c r="C448" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="D448" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PRIVATE=446,</v>
+        <v xml:space="preserve">        IN_OUT=446,</v>
       </c>
     </row>
     <row r="449" spans="2:4" x14ac:dyDescent="0.25">
@@ -9026,33 +9020,33 @@
       </c>
       <c r="D449" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        IN_OUT=447,</v>
+        <v xml:space="preserve">        STRICT=447,</v>
       </c>
     </row>
     <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B450" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B450:B453" si="16">B449+1</f>
         <v>448</v>
       </c>
       <c r="C450" t="s">
         <v>467</v>
       </c>
       <c r="D450" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRICT=448,</v>
+        <f t="shared" ref="D450:D453" si="17">"        "&amp;C450&amp;"="&amp;B450&amp;","</f>
+        <v xml:space="preserve">        QuestionMark=448,</v>
       </c>
     </row>
     <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B451" s="1">
-        <f t="shared" ref="B451:B454" si="16">B450+1</f>
+        <f t="shared" si="16"/>
         <v>449</v>
       </c>
       <c r="C451" t="s">
         <v>468</v>
       </c>
       <c r="D451" t="str">
-        <f t="shared" ref="D451:D454" si="17">"        "&amp;C451&amp;"="&amp;B451&amp;","</f>
-        <v xml:space="preserve">        QuestionMark=449,</v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">        CompilerDirective=449,</v>
       </c>
     </row>
     <row r="452" spans="2:4" x14ac:dyDescent="0.25">
@@ -9065,7 +9059,7 @@
       </c>
       <c r="D452" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CompilerDirective=450,</v>
+        <v xml:space="preserve">        CopyImportDirective=450,</v>
       </c>
     </row>
     <row r="453" spans="2:4" x14ac:dyDescent="0.25">
@@ -9078,33 +9072,20 @@
       </c>
       <c r="D453" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CopyImportDirective=451,</v>
+        <v xml:space="preserve">        ReplaceDirective=451,</v>
       </c>
     </row>
     <row r="454" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B454" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="B454" si="18">B453+1</f>
         <v>452</v>
       </c>
       <c r="C454" t="s">
         <v>471</v>
       </c>
       <c r="D454" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        ReplaceDirective=452,</v>
-      </c>
-    </row>
-    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B455" s="1">
-        <f t="shared" ref="B455" si="18">B454+1</f>
-        <v>453</v>
-      </c>
-      <c r="C455" t="s">
-        <v>472</v>
-      </c>
-      <c r="D455" t="str">
-        <f t="shared" ref="D455" si="19">"        "&amp;C455&amp;"="&amp;B455&amp;","</f>
-        <v xml:space="preserve">        ContinuationTokenGroup=453,</v>
+        <f t="shared" ref="D454" si="19">"        "&amp;C454&amp;"="&amp;B454&amp;","</f>
+        <v xml:space="preserve">        ContinuationTokenGroup=452,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#578, remove YYYYMMDD Token, add predicate
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="471">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1374,9 +1374,6 @@
   </si>
   <si>
     <t>// Keywords - Syntax tokens</t>
-  </si>
-  <si>
-    <t>YYYYMMDD</t>
   </si>
   <si>
     <t>TYPEDEF</t>
@@ -1851,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D454"/>
+  <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
-      <selection activeCell="H330" sqref="H330"/>
+    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
+      <selection activeCell="C455" sqref="C455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D2" t="str">
         <f>"        "&amp;C2&amp;"="&amp;B2&amp;","</f>
@@ -2019,7 +2016,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2336,7 +2333,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2445,7 +2442,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2461,7 +2458,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2493,7 +2490,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2749,7 +2746,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -3021,7 +3018,7 @@
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -3165,7 +3162,7 @@
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -8880,7 +8877,7 @@
         <v>429</v>
       </c>
       <c r="D439" t="str">
-        <f t="shared" ref="D439:D449" si="14">"        "&amp;C439&amp;"="&amp;B439&amp;","</f>
+        <f t="shared" ref="D439:D448" si="14">"        "&amp;C439&amp;"="&amp;B439&amp;","</f>
         <v xml:space="preserve">        WRITE_ONLY=437,</v>
       </c>
     </row>
@@ -8905,7 +8902,7 @@
         <v>433</v>
       </c>
       <c r="B441" s="1">
-        <f t="shared" ref="B441:B449" si="15">B440+1</f>
+        <f t="shared" ref="B441:B448" si="15">B440+1</f>
         <v>439</v>
       </c>
       <c r="C441" t="s">
@@ -8917,9 +8914,6 @@
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A442" t="s">
-        <v>433</v>
-      </c>
       <c r="B442" s="1">
         <f t="shared" si="15"/>
         <v>440</v>
@@ -8929,7 +8923,7 @@
       </c>
       <c r="D442" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYMMDD=440,</v>
+        <v xml:space="preserve">        TYPEDEF=440,</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
@@ -8942,7 +8936,7 @@
       </c>
       <c r="D443" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        TYPEDEF=441,</v>
+        <v xml:space="preserve">        STRONG=441,</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
@@ -8955,7 +8949,7 @@
       </c>
       <c r="D444" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRONG=442,</v>
+        <v xml:space="preserve">        UNSAFE=442,</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -8964,11 +8958,11 @@
         <v>443</v>
       </c>
       <c r="C445" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D445" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        UNSAFE=443,</v>
+        <v xml:space="preserve">        PUBLIC=443,</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8981,7 +8975,7 @@
       </c>
       <c r="D446" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PUBLIC=444,</v>
+        <v xml:space="preserve">        PRIVATE=444,</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -8990,11 +8984,11 @@
         <v>445</v>
       </c>
       <c r="C447" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D447" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PRIVATE=445,</v>
+        <v xml:space="preserve">        IN_OUT=445,</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -9007,33 +9001,33 @@
       </c>
       <c r="D448" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        IN_OUT=446,</v>
+        <v xml:space="preserve">        STRICT=446,</v>
       </c>
     </row>
     <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B449:B452" si="16">B448+1</f>
         <v>447</v>
       </c>
       <c r="C449" t="s">
         <v>466</v>
       </c>
       <c r="D449" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRICT=447,</v>
+        <f t="shared" ref="D449:D452" si="17">"        "&amp;C449&amp;"="&amp;B449&amp;","</f>
+        <v xml:space="preserve">        QuestionMark=447,</v>
       </c>
     </row>
     <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B450" s="1">
-        <f t="shared" ref="B450:B453" si="16">B449+1</f>
+        <f t="shared" si="16"/>
         <v>448</v>
       </c>
       <c r="C450" t="s">
         <v>467</v>
       </c>
       <c r="D450" t="str">
-        <f t="shared" ref="D450:D453" si="17">"        "&amp;C450&amp;"="&amp;B450&amp;","</f>
-        <v xml:space="preserve">        QuestionMark=448,</v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">        CompilerDirective=448,</v>
       </c>
     </row>
     <row r="451" spans="2:4" x14ac:dyDescent="0.25">
@@ -9046,7 +9040,7 @@
       </c>
       <c r="D451" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CompilerDirective=449,</v>
+        <v xml:space="preserve">        CopyImportDirective=449,</v>
       </c>
     </row>
     <row r="452" spans="2:4" x14ac:dyDescent="0.25">
@@ -9059,33 +9053,20 @@
       </c>
       <c r="D452" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CopyImportDirective=450,</v>
+        <v xml:space="preserve">        ReplaceDirective=450,</v>
       </c>
     </row>
     <row r="453" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B453" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="B453" si="18">B452+1</f>
         <v>451</v>
       </c>
       <c r="C453" t="s">
         <v>470</v>
       </c>
       <c r="D453" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        ReplaceDirective=451,</v>
-      </c>
-    </row>
-    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B454" s="1">
-        <f t="shared" ref="B454" si="18">B453+1</f>
-        <v>452</v>
-      </c>
-      <c r="C454" t="s">
-        <v>471</v>
-      </c>
-      <c r="D454" t="str">
-        <f t="shared" ref="D454" si="19">"        "&amp;C454&amp;"="&amp;B454&amp;","</f>
-        <v xml:space="preserve">        ContinuationTokenGroup=452,</v>
+        <f t="shared" ref="D453" si="19">"        "&amp;C453&amp;"="&amp;B453&amp;","</f>
+        <v xml:space="preserve">        ContinuationTokenGroup=451,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#578, remove YYYYDDD Token, add predicate
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="470">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1317,9 +1317,6 @@
   </si>
   <si>
     <t>XML_SCHEMA</t>
-  </si>
-  <si>
-    <t>YYYYDDD</t>
   </si>
   <si>
     <t>// Separators - Whitespace</t>
@@ -1848,10 +1845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D453"/>
+  <dimension ref="A1:D452"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
-      <selection activeCell="C455" sqref="C455"/>
+      <selection activeCell="D423" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,7 +1863,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B1" s="1">
         <v>-1</v>
@@ -1881,14 +1878,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B2" s="1">
         <f>B1+1</f>
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D2" t="str">
         <f>"        "&amp;C2&amp;"="&amp;B2&amp;","</f>
@@ -1897,7 +1894,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B3" s="1">
         <f>B2+1</f>
@@ -1913,7 +1910,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B67" si="1">B3+1</f>
@@ -1929,7 +1926,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="1"/>
@@ -1945,7 +1942,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="1"/>
@@ -1961,7 +1958,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="1"/>
@@ -1977,7 +1974,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="1"/>
@@ -1993,7 +1990,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="1"/>
@@ -2009,14 +2006,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2025,7 +2022,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="1"/>
@@ -2041,7 +2038,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="1"/>
@@ -2057,7 +2054,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="1"/>
@@ -2073,7 +2070,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
@@ -2089,7 +2086,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
@@ -2121,7 +2118,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
@@ -2137,7 +2134,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
@@ -2153,7 +2150,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
@@ -2169,7 +2166,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="1"/>
@@ -2185,7 +2182,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="1"/>
@@ -2201,7 +2198,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="1"/>
@@ -2217,7 +2214,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="1"/>
@@ -2233,7 +2230,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="1"/>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="1"/>
@@ -2265,7 +2262,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B26" s="1">
         <f t="shared" si="1"/>
@@ -2281,7 +2278,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="1"/>
@@ -2297,7 +2294,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="1"/>
@@ -2326,14 +2323,14 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B30" s="1">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2342,7 +2339,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B31" s="1">
         <f t="shared" si="1"/>
@@ -2358,7 +2355,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B32" s="1">
         <f t="shared" si="1"/>
@@ -2374,7 +2371,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" si="1"/>
@@ -2390,7 +2387,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" si="1"/>
@@ -2406,7 +2403,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" si="1"/>
@@ -2435,14 +2432,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2451,14 +2448,14 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2467,7 +2464,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="1"/>
@@ -2483,14 +2480,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2499,7 +2496,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="1"/>
@@ -2515,7 +2512,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B42" s="1">
         <f t="shared" si="1"/>
@@ -2531,7 +2528,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B43" s="1">
         <f t="shared" si="1"/>
@@ -2547,7 +2544,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="1"/>
@@ -2563,7 +2560,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B45" s="1">
         <f t="shared" si="1"/>
@@ -2579,7 +2576,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B46" s="1">
         <f t="shared" si="1"/>
@@ -2595,7 +2592,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B47" s="1">
         <f t="shared" si="1"/>
@@ -2611,7 +2608,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B48" s="1">
         <f t="shared" si="1"/>
@@ -2627,7 +2624,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B49" s="1">
         <f t="shared" si="1"/>
@@ -2643,7 +2640,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B50" s="1">
         <f t="shared" si="1"/>
@@ -2659,7 +2656,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B51" s="1">
         <f t="shared" si="1"/>
@@ -2675,7 +2672,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" si="1"/>
@@ -2691,7 +2688,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B53" s="1">
         <f t="shared" si="1"/>
@@ -2707,7 +2704,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B54" s="1">
         <f t="shared" si="1"/>
@@ -2723,7 +2720,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B55" s="1">
         <f t="shared" si="1"/>
@@ -2739,14 +2736,14 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B56" s="1">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2755,7 +2752,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B57" s="1">
         <f t="shared" si="1"/>
@@ -2771,7 +2768,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B58" s="1">
         <f t="shared" si="1"/>
@@ -2787,7 +2784,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B59" s="1">
         <f t="shared" si="1"/>
@@ -2803,7 +2800,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B60" s="1">
         <f t="shared" si="1"/>
@@ -2819,7 +2816,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B61" s="1">
         <f t="shared" si="1"/>
@@ -2835,7 +2832,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B62" s="1">
         <f t="shared" si="1"/>
@@ -2851,7 +2848,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B63" s="1">
         <f t="shared" si="1"/>
@@ -2867,7 +2864,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B64" s="1">
         <f t="shared" si="1"/>
@@ -2883,7 +2880,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B65" s="1">
         <f t="shared" si="1"/>
@@ -2899,7 +2896,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B66" s="1">
         <f t="shared" si="1"/>
@@ -2915,7 +2912,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B67" s="1">
         <f t="shared" si="1"/>
@@ -2931,7 +2928,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B68" s="1">
         <f t="shared" ref="B68:B131" si="3">B67+1</f>
@@ -2947,7 +2944,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B69" s="1">
         <f t="shared" si="3"/>
@@ -2963,7 +2960,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B70" s="1">
         <f t="shared" si="3"/>
@@ -2979,7 +2976,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B71" s="1">
         <f t="shared" si="3"/>
@@ -2995,7 +2992,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B72" s="1">
         <f t="shared" si="3"/>
@@ -3011,14 +3008,14 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B73" s="1">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -3027,7 +3024,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B74" s="1">
         <f t="shared" si="3"/>
@@ -3043,7 +3040,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B75" s="1">
         <f t="shared" si="3"/>
@@ -3059,7 +3056,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B76" s="1">
         <f t="shared" si="3"/>
@@ -3075,7 +3072,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B77" s="1">
         <f t="shared" si="3"/>
@@ -3091,7 +3088,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B78" s="1">
         <f t="shared" si="3"/>
@@ -3107,7 +3104,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B79" s="1">
         <f t="shared" si="3"/>
@@ -3123,7 +3120,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B80" s="1">
         <f t="shared" si="3"/>
@@ -3139,7 +3136,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B81" s="1">
         <f t="shared" si="3"/>
@@ -3155,14 +3152,14 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B82" s="1">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3171,7 +3168,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B83" s="1">
         <f t="shared" si="3"/>
@@ -3187,7 +3184,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B84" s="1">
         <f t="shared" si="3"/>
@@ -3203,7 +3200,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B85" s="1">
         <f t="shared" si="3"/>
@@ -3219,7 +3216,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B86" s="1">
         <f t="shared" si="3"/>
@@ -3235,7 +3232,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B87" s="1">
         <f t="shared" si="3"/>
@@ -3251,7 +3248,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B88" s="1">
         <f t="shared" si="3"/>
@@ -3267,7 +3264,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B89" s="1">
         <f t="shared" si="3"/>
@@ -3283,7 +3280,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B90" s="1">
         <f t="shared" si="3"/>
@@ -3299,7 +3296,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B91" s="1">
         <f t="shared" si="3"/>
@@ -3315,7 +3312,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B92" s="1">
         <f t="shared" si="3"/>
@@ -3331,7 +3328,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B93" s="1">
         <f t="shared" si="3"/>
@@ -3347,7 +3344,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B94" s="1">
         <f t="shared" si="3"/>
@@ -3363,7 +3360,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B95" s="1">
         <f t="shared" si="3"/>
@@ -3379,7 +3376,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B96" s="1">
         <f t="shared" si="3"/>
@@ -3395,7 +3392,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B97" s="1">
         <f t="shared" si="3"/>
@@ -3411,7 +3408,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B98" s="1">
         <f t="shared" si="3"/>
@@ -3427,7 +3424,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B99" s="1">
         <f t="shared" si="3"/>
@@ -3443,7 +3440,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B100" s="1">
         <f t="shared" si="3"/>
@@ -3459,7 +3456,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B101" s="1">
         <f t="shared" si="3"/>
@@ -3475,7 +3472,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B102" s="1">
         <f t="shared" si="3"/>
@@ -3491,7 +3488,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B103" s="1">
         <f t="shared" si="3"/>
@@ -3507,7 +3504,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B104" s="1">
         <f t="shared" si="3"/>
@@ -3523,7 +3520,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B105" s="1">
         <f t="shared" si="3"/>
@@ -3539,7 +3536,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B106" s="1">
         <f t="shared" si="3"/>
@@ -3555,7 +3552,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B107" s="1">
         <f t="shared" si="3"/>
@@ -3571,7 +3568,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B108" s="1">
         <f t="shared" si="3"/>
@@ -3587,7 +3584,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B109" s="1">
         <f t="shared" si="3"/>
@@ -3603,7 +3600,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B110" s="1">
         <f t="shared" si="3"/>
@@ -3619,7 +3616,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B111" s="1">
         <f t="shared" si="3"/>
@@ -3635,7 +3632,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B112" s="1">
         <f t="shared" si="3"/>
@@ -3651,7 +3648,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B113" s="1">
         <f t="shared" si="3"/>
@@ -3667,7 +3664,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B114" s="1">
         <f t="shared" si="3"/>
@@ -3683,7 +3680,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B115" s="1">
         <f t="shared" si="3"/>
@@ -3699,7 +3696,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B116" s="1">
         <f t="shared" si="3"/>
@@ -3715,7 +3712,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B117" s="1">
         <f t="shared" si="3"/>
@@ -3731,7 +3728,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B118" s="1">
         <f t="shared" si="3"/>
@@ -3747,7 +3744,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B119" s="1">
         <f t="shared" si="3"/>
@@ -3763,7 +3760,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B120" s="1">
         <f t="shared" si="3"/>
@@ -3779,7 +3776,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B121" s="1">
         <f t="shared" si="3"/>
@@ -3795,7 +3792,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B122" s="1">
         <f t="shared" si="3"/>
@@ -3811,7 +3808,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B123" s="1">
         <f t="shared" si="3"/>
@@ -3827,7 +3824,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B124" s="1">
         <f t="shared" si="3"/>
@@ -3843,7 +3840,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B125" s="1">
         <f t="shared" si="3"/>
@@ -3859,7 +3856,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B126" s="1">
         <f t="shared" si="3"/>
@@ -3875,7 +3872,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B127" s="1">
         <f t="shared" si="3"/>
@@ -3891,7 +3888,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B128" s="1">
         <f t="shared" si="3"/>
@@ -3907,7 +3904,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B129" s="1">
         <f t="shared" si="3"/>
@@ -3923,7 +3920,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B130" s="1">
         <f t="shared" si="3"/>
@@ -3939,7 +3936,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B131" s="1">
         <f t="shared" si="3"/>
@@ -3955,7 +3952,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B132" s="1">
         <f t="shared" ref="B132:B195" si="5">B131+1</f>
@@ -3971,7 +3968,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B133" s="1">
         <f t="shared" si="5"/>
@@ -3987,7 +3984,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B134" s="1">
         <f t="shared" si="5"/>
@@ -4003,7 +4000,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B135" s="1">
         <f t="shared" si="5"/>
@@ -4019,7 +4016,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B136" s="1">
         <f t="shared" si="5"/>
@@ -4035,7 +4032,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B137" s="1">
         <f t="shared" si="5"/>
@@ -4051,7 +4048,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B138" s="1">
         <f t="shared" si="5"/>
@@ -4067,7 +4064,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B139" s="1">
         <f t="shared" si="5"/>
@@ -4083,7 +4080,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B140" s="1">
         <f t="shared" si="5"/>
@@ -4099,7 +4096,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B141" s="1">
         <f t="shared" si="5"/>
@@ -4115,7 +4112,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B142" s="1">
         <f t="shared" si="5"/>
@@ -4131,7 +4128,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B143" s="1">
         <f t="shared" si="5"/>
@@ -4147,7 +4144,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B144" s="1">
         <f t="shared" si="5"/>
@@ -4163,7 +4160,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B145" s="1">
         <f t="shared" si="5"/>
@@ -4179,7 +4176,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B146" s="1">
         <f t="shared" si="5"/>
@@ -4195,7 +4192,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B147" s="1">
         <f t="shared" si="5"/>
@@ -4211,7 +4208,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B148" s="1">
         <f t="shared" si="5"/>
@@ -4227,7 +4224,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B149" s="1">
         <f t="shared" si="5"/>
@@ -4243,7 +4240,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B150" s="1">
         <f t="shared" si="5"/>
@@ -4259,7 +4256,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B151" s="1">
         <f t="shared" si="5"/>
@@ -4275,7 +4272,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B152" s="1">
         <f t="shared" si="5"/>
@@ -4291,7 +4288,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B153" s="1">
         <f t="shared" si="5"/>
@@ -4307,7 +4304,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B154" s="1">
         <f t="shared" si="5"/>
@@ -4323,7 +4320,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B155" s="1">
         <f t="shared" si="5"/>
@@ -4339,7 +4336,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B156" s="1">
         <f t="shared" si="5"/>
@@ -4355,7 +4352,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B157" s="1">
         <f t="shared" si="5"/>
@@ -4371,7 +4368,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B158" s="1">
         <f t="shared" si="5"/>
@@ -4387,7 +4384,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B159" s="1">
         <f t="shared" si="5"/>
@@ -4403,7 +4400,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B160" s="1">
         <f t="shared" si="5"/>
@@ -4419,7 +4416,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B161" s="1">
         <f t="shared" si="5"/>
@@ -4435,7 +4432,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B162" s="1">
         <f t="shared" si="5"/>
@@ -4451,7 +4448,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B163" s="1">
         <f t="shared" si="5"/>
@@ -4467,7 +4464,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B164" s="1">
         <f t="shared" si="5"/>
@@ -4483,7 +4480,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B165" s="1">
         <f t="shared" si="5"/>
@@ -4499,7 +4496,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B166" s="1">
         <f t="shared" si="5"/>
@@ -4515,7 +4512,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B167" s="1">
         <f t="shared" si="5"/>
@@ -4531,7 +4528,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B168" s="1">
         <f t="shared" si="5"/>
@@ -4547,7 +4544,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B169" s="1">
         <f t="shared" si="5"/>
@@ -4563,7 +4560,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B170" s="1">
         <f t="shared" si="5"/>
@@ -4579,7 +4576,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B171" s="1">
         <f t="shared" si="5"/>
@@ -4595,7 +4592,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B172" s="1">
         <f t="shared" si="5"/>
@@ -4611,7 +4608,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B173" s="1">
         <f t="shared" si="5"/>
@@ -4627,7 +4624,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B174" s="1">
         <f t="shared" si="5"/>
@@ -4643,7 +4640,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B175" s="1">
         <f t="shared" si="5"/>
@@ -4659,7 +4656,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B176" s="1">
         <f t="shared" si="5"/>
@@ -4675,7 +4672,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B177" s="1">
         <f t="shared" si="5"/>
@@ -4691,7 +4688,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B178" s="1">
         <f t="shared" si="5"/>
@@ -4707,7 +4704,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B179" s="1">
         <f t="shared" si="5"/>
@@ -4723,7 +4720,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B180" s="1">
         <f t="shared" si="5"/>
@@ -4739,7 +4736,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B181" s="1">
         <f t="shared" si="5"/>
@@ -4755,7 +4752,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B182" s="1">
         <f t="shared" si="5"/>
@@ -4771,7 +4768,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B183" s="1">
         <f>B182+1</f>
@@ -4787,7 +4784,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B184" s="1">
         <f t="shared" si="5"/>
@@ -4803,7 +4800,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B185" s="1">
         <f t="shared" si="5"/>
@@ -4819,7 +4816,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B186" s="1">
         <f t="shared" si="5"/>
@@ -4835,7 +4832,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B187" s="1">
         <f t="shared" si="5"/>
@@ -4851,7 +4848,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B188" s="1">
         <f t="shared" si="5"/>
@@ -4867,7 +4864,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B189" s="1">
         <f t="shared" si="5"/>
@@ -4883,7 +4880,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B190" s="1">
         <f t="shared" si="5"/>
@@ -4899,7 +4896,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B191" s="1">
         <f t="shared" si="5"/>
@@ -4915,7 +4912,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B192" s="1">
         <f t="shared" si="5"/>
@@ -4931,7 +4928,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B193" s="1">
         <f t="shared" si="5"/>
@@ -4947,7 +4944,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B194" s="1">
         <f t="shared" si="5"/>
@@ -4963,7 +4960,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B195" s="1">
         <f t="shared" si="5"/>
@@ -4979,7 +4976,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B196" s="1">
         <f t="shared" ref="B196:B257" si="7">B195+1</f>
@@ -4995,7 +4992,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B197" s="1">
         <f t="shared" si="7"/>
@@ -5011,7 +5008,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B198" s="1">
         <f t="shared" si="7"/>
@@ -5027,7 +5024,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B199" s="1">
         <f t="shared" si="7"/>
@@ -5043,7 +5040,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B200" s="1">
         <f t="shared" si="7"/>
@@ -5059,7 +5056,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B201" s="1">
         <f t="shared" si="7"/>
@@ -5075,7 +5072,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B202" s="1">
         <f t="shared" si="7"/>
@@ -5091,7 +5088,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B203" s="1">
         <f t="shared" si="7"/>
@@ -5107,7 +5104,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B204" s="1">
         <f t="shared" si="7"/>
@@ -5123,7 +5120,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B205" s="1">
         <f t="shared" si="7"/>
@@ -5139,7 +5136,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B206" s="1">
         <f t="shared" si="7"/>
@@ -5155,7 +5152,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B207" s="1">
         <f t="shared" si="7"/>
@@ -5171,7 +5168,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B208" s="1">
         <f t="shared" si="7"/>
@@ -5187,7 +5184,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B209" s="1">
         <f t="shared" si="7"/>
@@ -5203,7 +5200,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B210" s="1">
         <f t="shared" si="7"/>
@@ -5219,7 +5216,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B211" s="1">
         <f t="shared" si="7"/>
@@ -5235,7 +5232,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B212" s="1">
         <f t="shared" si="7"/>
@@ -5251,7 +5248,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B213" s="1">
         <f t="shared" si="7"/>
@@ -5267,7 +5264,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B214" s="1">
         <f t="shared" si="7"/>
@@ -5283,7 +5280,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B215" s="1">
         <f t="shared" si="7"/>
@@ -5299,7 +5296,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B216" s="1">
         <f t="shared" si="7"/>
@@ -5315,7 +5312,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B217" s="1">
         <f t="shared" si="7"/>
@@ -5331,7 +5328,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B218" s="1">
         <f t="shared" si="7"/>
@@ -5347,7 +5344,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B219" s="1">
         <f t="shared" si="7"/>
@@ -5363,7 +5360,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B220" s="1">
         <f t="shared" si="7"/>
@@ -5379,7 +5376,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B221" s="1">
         <f t="shared" si="7"/>
@@ -5395,7 +5392,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B222" s="1">
         <f t="shared" si="7"/>
@@ -5411,7 +5408,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B223" s="1">
         <f t="shared" si="7"/>
@@ -5427,7 +5424,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B224" s="1">
         <f t="shared" si="7"/>
@@ -5443,7 +5440,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B225" s="1">
         <f t="shared" si="7"/>
@@ -5459,7 +5456,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B226" s="1">
         <f t="shared" si="7"/>
@@ -5475,7 +5472,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B227" s="1">
         <f t="shared" si="7"/>
@@ -5491,7 +5488,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B228" s="1">
         <f t="shared" si="7"/>
@@ -5507,7 +5504,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B229" s="1">
         <f t="shared" si="7"/>
@@ -5523,7 +5520,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B230" s="1">
         <f t="shared" si="7"/>
@@ -5539,7 +5536,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B231" s="1">
         <f t="shared" si="7"/>
@@ -5555,7 +5552,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B232" s="1">
         <f t="shared" si="7"/>
@@ -5571,7 +5568,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B233" s="1">
         <f t="shared" si="7"/>
@@ -5587,7 +5584,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B234" s="1">
         <f t="shared" si="7"/>
@@ -5603,7 +5600,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B235" s="1">
         <f t="shared" si="7"/>
@@ -5619,7 +5616,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B236" s="1">
         <f t="shared" si="7"/>
@@ -5635,7 +5632,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B237" s="1">
         <f t="shared" si="7"/>
@@ -5651,7 +5648,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B238" s="1">
         <f t="shared" si="7"/>
@@ -5667,7 +5664,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B239" s="1">
         <f t="shared" si="7"/>
@@ -5683,7 +5680,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B240" s="1">
         <f t="shared" si="7"/>
@@ -5699,7 +5696,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B241" s="1">
         <f t="shared" si="7"/>
@@ -5715,7 +5712,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B242" s="1">
         <f t="shared" si="7"/>
@@ -5731,7 +5728,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B243" s="1">
         <f t="shared" si="7"/>
@@ -5747,7 +5744,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B244" s="1">
         <f t="shared" si="7"/>
@@ -5763,7 +5760,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B245" s="1">
         <f t="shared" si="7"/>
@@ -5779,7 +5776,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B246" s="1">
         <f t="shared" si="7"/>
@@ -5795,7 +5792,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B247" s="1">
         <f t="shared" si="7"/>
@@ -5811,7 +5808,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B248" s="1">
         <f t="shared" si="7"/>
@@ -5827,7 +5824,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B249" s="1">
         <f t="shared" si="7"/>
@@ -5843,7 +5840,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B250" s="1">
         <f t="shared" si="7"/>
@@ -5859,7 +5856,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B251" s="1">
         <f t="shared" si="7"/>
@@ -5875,7 +5872,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B252" s="1">
         <f t="shared" si="7"/>
@@ -5891,7 +5888,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B253" s="1">
         <f t="shared" si="7"/>
@@ -5907,7 +5904,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B254" s="1">
         <f t="shared" si="7"/>
@@ -5923,7 +5920,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B255" s="1">
         <f t="shared" si="7"/>
@@ -5939,7 +5936,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B256" s="1">
         <f t="shared" si="7"/>
@@ -5955,7 +5952,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B257" s="1">
         <f t="shared" si="7"/>
@@ -5971,7 +5968,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B258" s="1">
         <f t="shared" ref="B258:B319" si="9">B257+1</f>
@@ -5987,7 +5984,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B259" s="1">
         <f t="shared" si="9"/>
@@ -6003,7 +6000,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B260" s="1">
         <f t="shared" si="9"/>
@@ -6019,7 +6016,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B261" s="1">
         <f t="shared" si="9"/>
@@ -6035,7 +6032,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B262" s="1">
         <f t="shared" si="9"/>
@@ -6051,7 +6048,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B263" s="1">
         <f t="shared" si="9"/>
@@ -6067,7 +6064,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B264" s="1">
         <f t="shared" si="9"/>
@@ -6083,7 +6080,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B265" s="1">
         <f t="shared" si="9"/>
@@ -6099,7 +6096,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B266" s="1">
         <f t="shared" si="9"/>
@@ -6115,7 +6112,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B267" s="1">
         <f t="shared" si="9"/>
@@ -6131,7 +6128,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B268" s="1">
         <f t="shared" si="9"/>
@@ -6147,7 +6144,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B269" s="1">
         <f t="shared" si="9"/>
@@ -6163,7 +6160,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B270" s="1">
         <f t="shared" si="9"/>
@@ -6179,7 +6176,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B271" s="1">
         <f t="shared" si="9"/>
@@ -6195,7 +6192,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B272" s="1">
         <f t="shared" si="9"/>
@@ -6211,7 +6208,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B273" s="1">
         <f t="shared" si="9"/>
@@ -6227,7 +6224,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B274" s="1">
         <f t="shared" si="9"/>
@@ -6243,7 +6240,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B275" s="1">
         <f t="shared" si="9"/>
@@ -6259,7 +6256,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B276" s="1">
         <f t="shared" si="9"/>
@@ -6275,7 +6272,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B277" s="1">
         <f t="shared" si="9"/>
@@ -6291,7 +6288,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B278" s="1">
         <f t="shared" si="9"/>
@@ -6307,7 +6304,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B279" s="1">
         <f t="shared" si="9"/>
@@ -6323,7 +6320,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B280" s="1">
         <f t="shared" si="9"/>
@@ -6339,7 +6336,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B281" s="1">
         <f t="shared" si="9"/>
@@ -6355,7 +6352,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B282" s="1">
         <f t="shared" si="9"/>
@@ -6371,7 +6368,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B283" s="1">
         <f t="shared" si="9"/>
@@ -6387,7 +6384,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B284" s="1">
         <f t="shared" si="9"/>
@@ -6403,7 +6400,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B285" s="1">
         <f t="shared" si="9"/>
@@ -6419,7 +6416,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B286" s="1">
         <f t="shared" si="9"/>
@@ -6435,7 +6432,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B287" s="1">
         <f t="shared" si="9"/>
@@ -6451,7 +6448,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B288" s="1">
         <f t="shared" si="9"/>
@@ -6467,7 +6464,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B289" s="1">
         <f t="shared" si="9"/>
@@ -6483,7 +6480,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B290" s="1">
         <f t="shared" si="9"/>
@@ -6499,7 +6496,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B291" s="1">
         <f t="shared" si="9"/>
@@ -6515,7 +6512,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B292" s="1">
         <f t="shared" si="9"/>
@@ -6531,7 +6528,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B293" s="1">
         <f t="shared" si="9"/>
@@ -6547,7 +6544,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B294" s="1">
         <f t="shared" si="9"/>
@@ -6563,7 +6560,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B295" s="1">
         <f t="shared" si="9"/>
@@ -6579,7 +6576,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B296" s="1">
         <f t="shared" si="9"/>
@@ -6595,7 +6592,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B297" s="1">
         <f t="shared" si="9"/>
@@ -6611,7 +6608,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B298" s="1">
         <f t="shared" si="9"/>
@@ -6627,7 +6624,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B299" s="1">
         <f t="shared" si="9"/>
@@ -6643,7 +6640,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B300" s="1">
         <f t="shared" si="9"/>
@@ -6659,7 +6656,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B301" s="1">
         <f t="shared" si="9"/>
@@ -6675,7 +6672,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B302" s="1">
         <f t="shared" si="9"/>
@@ -6691,7 +6688,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B303" s="1">
         <f t="shared" si="9"/>
@@ -6707,7 +6704,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B304" s="1">
         <f t="shared" si="9"/>
@@ -6723,7 +6720,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B305" s="1">
         <f t="shared" si="9"/>
@@ -6739,7 +6736,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B306" s="1">
         <f t="shared" si="9"/>
@@ -6755,7 +6752,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B307" s="1">
         <f t="shared" si="9"/>
@@ -6771,7 +6768,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B308" s="1">
         <f t="shared" si="9"/>
@@ -6787,7 +6784,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B309" s="1">
         <f t="shared" si="9"/>
@@ -6803,7 +6800,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B310" s="1">
         <f t="shared" si="9"/>
@@ -6819,7 +6816,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B311" s="1">
         <f t="shared" si="9"/>
@@ -6835,7 +6832,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B312" s="1">
         <f t="shared" si="9"/>
@@ -6851,7 +6848,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B313" s="1">
         <f t="shared" si="9"/>
@@ -6867,7 +6864,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B314" s="1">
         <f t="shared" si="9"/>
@@ -6883,7 +6880,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B315" s="1">
         <f t="shared" si="9"/>
@@ -6899,7 +6896,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B316" s="1">
         <f t="shared" si="9"/>
@@ -6915,7 +6912,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B317" s="1">
         <f t="shared" si="9"/>
@@ -6931,7 +6928,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B318" s="1">
         <f t="shared" si="9"/>
@@ -6947,7 +6944,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B319" s="1">
         <f t="shared" si="9"/>
@@ -6963,7 +6960,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B320" s="1">
         <f t="shared" ref="B320:B378" si="11">B319+1</f>
@@ -6979,7 +6976,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B321" s="1">
         <f t="shared" si="11"/>
@@ -6995,7 +6992,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B322" s="1">
         <f t="shared" si="11"/>
@@ -7011,7 +7008,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B323" s="1">
         <f t="shared" si="11"/>
@@ -7027,7 +7024,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B324" s="1">
         <f t="shared" si="11"/>
@@ -7043,7 +7040,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B325" s="1">
         <f t="shared" si="11"/>
@@ -7059,7 +7056,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B326" s="1">
         <f t="shared" si="11"/>
@@ -7075,7 +7072,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B327" s="1">
         <f t="shared" si="11"/>
@@ -7091,7 +7088,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B328" s="1">
         <f t="shared" si="11"/>
@@ -7107,7 +7104,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B329" s="1">
         <f t="shared" si="11"/>
@@ -7123,7 +7120,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B330" s="1">
         <f t="shared" si="11"/>
@@ -7139,7 +7136,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B331" s="1">
         <f t="shared" si="11"/>
@@ -7155,7 +7152,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B332" s="1">
         <f t="shared" si="11"/>
@@ -7171,7 +7168,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B333" s="1">
         <f t="shared" si="11"/>
@@ -7187,7 +7184,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B334" s="1">
         <f t="shared" si="11"/>
@@ -7203,7 +7200,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B335" s="1">
         <f t="shared" si="11"/>
@@ -7219,7 +7216,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B336" s="1">
         <f t="shared" si="11"/>
@@ -7235,7 +7232,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B337" s="1">
         <f t="shared" si="11"/>
@@ -7251,7 +7248,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B338" s="1">
         <f t="shared" si="11"/>
@@ -7267,7 +7264,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B339" s="1">
         <f t="shared" si="11"/>
@@ -7283,7 +7280,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B340" s="1">
         <f t="shared" si="11"/>
@@ -7299,7 +7296,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B341" s="1">
         <f t="shared" si="11"/>
@@ -7315,7 +7312,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B342" s="1">
         <f t="shared" si="11"/>
@@ -7331,7 +7328,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B343" s="1">
         <f t="shared" si="11"/>
@@ -7347,7 +7344,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B344" s="1">
         <f t="shared" si="11"/>
@@ -7363,7 +7360,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B345" s="1">
         <f t="shared" si="11"/>
@@ -7379,7 +7376,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B346" s="1">
         <f t="shared" si="11"/>
@@ -7395,7 +7392,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B347" s="1">
         <f t="shared" si="11"/>
@@ -7411,7 +7408,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B348" s="1">
         <f t="shared" si="11"/>
@@ -7427,7 +7424,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B349" s="1">
         <f t="shared" si="11"/>
@@ -7443,7 +7440,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B350" s="1">
         <f t="shared" si="11"/>
@@ -7459,7 +7456,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B351" s="1">
         <f t="shared" si="11"/>
@@ -7475,7 +7472,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B352" s="1">
         <f t="shared" si="11"/>
@@ -7491,7 +7488,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B353" s="1">
         <f t="shared" si="11"/>
@@ -7507,7 +7504,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B354" s="1">
         <f t="shared" si="11"/>
@@ -7523,7 +7520,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B355" s="1">
         <f t="shared" si="11"/>
@@ -7539,7 +7536,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B356" s="1">
         <f t="shared" si="11"/>
@@ -7555,7 +7552,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B357" s="1">
         <f t="shared" si="11"/>
@@ -7571,7 +7568,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B358" s="1">
         <f t="shared" si="11"/>
@@ -7587,7 +7584,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B359" s="1">
         <f t="shared" si="11"/>
@@ -7603,7 +7600,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B360" s="1">
         <f t="shared" si="11"/>
@@ -7619,7 +7616,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B361" s="1">
         <f t="shared" si="11"/>
@@ -7635,7 +7632,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B362" s="1">
         <f t="shared" si="11"/>
@@ -7651,7 +7648,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B363" s="1">
         <f t="shared" si="11"/>
@@ -7667,7 +7664,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B364" s="1">
         <f t="shared" si="11"/>
@@ -7683,7 +7680,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B365" s="1">
         <f t="shared" si="11"/>
@@ -7699,7 +7696,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B366" s="1">
         <f t="shared" si="11"/>
@@ -7715,7 +7712,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B367" s="1">
         <f t="shared" si="11"/>
@@ -7731,7 +7728,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B368" s="1">
         <f t="shared" si="11"/>
@@ -7747,7 +7744,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B369" s="1">
         <f t="shared" si="11"/>
@@ -7763,7 +7760,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B370" s="1">
         <f t="shared" si="11"/>
@@ -7779,7 +7776,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B371" s="1">
         <f t="shared" si="11"/>
@@ -7795,7 +7792,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B372" s="1">
         <f t="shared" si="11"/>
@@ -7811,7 +7808,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B373" s="1">
         <f t="shared" si="11"/>
@@ -7827,7 +7824,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B374" s="1">
         <f t="shared" si="11"/>
@@ -7843,7 +7840,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B375" s="1">
         <f t="shared" si="11"/>
@@ -7859,7 +7856,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B376" s="1">
         <f t="shared" si="11"/>
@@ -7875,7 +7872,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B377" s="1">
         <f t="shared" si="11"/>
@@ -7891,7 +7888,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B378" s="1">
         <f t="shared" si="11"/>
@@ -7907,10 +7904,10 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B379" s="1">
-        <f t="shared" ref="B379:B440" si="13">B378+1</f>
+        <f t="shared" ref="B379:B441" si="13">B378+1</f>
         <v>377</v>
       </c>
       <c r="C379" t="s">
@@ -7923,7 +7920,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B380" s="1">
         <f t="shared" si="13"/>
@@ -7939,7 +7936,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B381" s="1">
         <f t="shared" si="13"/>
@@ -7955,7 +7952,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B382" s="1">
         <f t="shared" si="13"/>
@@ -7971,7 +7968,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B383" s="1">
         <f t="shared" si="13"/>
@@ -7987,7 +7984,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B384" s="1">
         <f t="shared" si="13"/>
@@ -8003,7 +8000,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B385" s="1">
         <f t="shared" si="13"/>
@@ -8019,7 +8016,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B386" s="1">
         <f t="shared" si="13"/>
@@ -8035,7 +8032,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B387" s="1">
         <f t="shared" si="13"/>
@@ -8051,7 +8048,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B388" s="1">
         <f t="shared" si="13"/>
@@ -8067,7 +8064,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B389" s="1">
         <f t="shared" si="13"/>
@@ -8083,7 +8080,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B390" s="1">
         <f t="shared" si="13"/>
@@ -8099,7 +8096,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B391" s="1">
         <f t="shared" si="13"/>
@@ -8115,7 +8112,7 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B392" s="1">
         <f t="shared" si="13"/>
@@ -8131,7 +8128,7 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B393" s="1">
         <f t="shared" si="13"/>
@@ -8147,7 +8144,7 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B394" s="1">
         <f t="shared" si="13"/>
@@ -8163,7 +8160,7 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B395" s="1">
         <f t="shared" si="13"/>
@@ -8179,7 +8176,7 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B396" s="1">
         <f t="shared" si="13"/>
@@ -8195,7 +8192,7 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B397" s="1">
         <f t="shared" si="13"/>
@@ -8211,7 +8208,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B398" s="1">
         <f t="shared" si="13"/>
@@ -8227,7 +8224,7 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B399" s="1">
         <f t="shared" si="13"/>
@@ -8243,7 +8240,7 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B400" s="1">
         <f t="shared" si="13"/>
@@ -8259,7 +8256,7 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B401" s="1">
         <f t="shared" si="13"/>
@@ -8275,7 +8272,7 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B402" s="1">
         <f t="shared" si="13"/>
@@ -8291,7 +8288,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B403" s="1">
         <f t="shared" si="13"/>
@@ -8307,7 +8304,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B404" s="1">
         <f t="shared" si="13"/>
@@ -8323,7 +8320,7 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B405" s="1">
         <f t="shared" si="13"/>
@@ -8339,7 +8336,7 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B406" s="1">
         <f t="shared" si="13"/>
@@ -8355,7 +8352,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B407" s="1">
         <f t="shared" si="13"/>
@@ -8371,7 +8368,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B408" s="1">
         <f t="shared" si="13"/>
@@ -8387,7 +8384,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B409" s="1">
         <f t="shared" si="13"/>
@@ -8403,7 +8400,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B410" s="1">
         <f t="shared" si="13"/>
@@ -8419,7 +8416,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B411" s="1">
         <f t="shared" si="13"/>
@@ -8435,7 +8432,7 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B412" s="1">
         <f t="shared" si="13"/>
@@ -8451,7 +8448,7 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B413" s="1">
         <f t="shared" si="13"/>
@@ -8467,7 +8464,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B414" s="1">
         <f t="shared" si="13"/>
@@ -8483,7 +8480,7 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B415" s="1">
         <f t="shared" si="13"/>
@@ -8499,7 +8496,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B416" s="1">
         <f t="shared" si="13"/>
@@ -8515,7 +8512,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B417" s="1">
         <f t="shared" si="13"/>
@@ -8531,7 +8528,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B418" s="1">
         <f t="shared" si="13"/>
@@ -8547,7 +8544,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B419" s="1">
         <f t="shared" si="13"/>
@@ -8563,7 +8560,7 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B420" s="1">
         <f t="shared" si="13"/>
@@ -8579,7 +8576,7 @@
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B421" s="1">
         <f t="shared" si="13"/>
@@ -8595,7 +8592,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B422" s="1">
         <f t="shared" si="13"/>
@@ -8611,7 +8608,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B423" s="1">
         <f t="shared" si="13"/>
@@ -8627,7 +8624,7 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B424" s="1">
         <f t="shared" si="13"/>
@@ -8643,7 +8640,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B425" s="1">
         <f t="shared" si="13"/>
@@ -8659,7 +8656,7 @@
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B426" s="1">
         <f t="shared" si="13"/>
@@ -8675,7 +8672,7 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B427" s="1">
         <f t="shared" si="13"/>
@@ -8691,7 +8688,7 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B428" s="1">
         <f t="shared" si="13"/>
@@ -8707,7 +8704,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B429" s="1">
         <f t="shared" si="13"/>
@@ -8723,7 +8720,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B430" s="1">
         <f t="shared" si="13"/>
@@ -8739,7 +8736,7 @@
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B431" s="1">
         <f t="shared" si="13"/>
@@ -8755,7 +8752,7 @@
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B432" s="1">
         <f t="shared" si="13"/>
@@ -8771,7 +8768,7 @@
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B433" s="1">
         <f t="shared" si="13"/>
@@ -8787,7 +8784,7 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B434" s="1">
         <f t="shared" si="13"/>
@@ -8803,7 +8800,7 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B435" s="1">
         <f t="shared" si="13"/>
@@ -8819,7 +8816,7 @@
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B436" s="1">
         <f t="shared" si="13"/>
@@ -8835,7 +8832,7 @@
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B437" s="1">
         <f t="shared" si="13"/>
@@ -8851,7 +8848,7 @@
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B438" s="1">
         <f t="shared" si="13"/>
@@ -8867,7 +8864,7 @@
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B439" s="1">
         <f t="shared" si="13"/>
@@ -8877,13 +8874,13 @@
         <v>429</v>
       </c>
       <c r="D439" t="str">
-        <f t="shared" ref="D439:D448" si="14">"        "&amp;C439&amp;"="&amp;B439&amp;","</f>
+        <f t="shared" ref="D439:D447" si="14">"        "&amp;C439&amp;"="&amp;B439&amp;","</f>
         <v xml:space="preserve">        WRITE_ONLY=437,</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B440" s="1">
         <f t="shared" si="13"/>
@@ -8898,24 +8895,21 @@
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A441" t="s">
-        <v>433</v>
-      </c>
       <c r="B441" s="1">
-        <f t="shared" ref="B441:B448" si="15">B440+1</f>
+        <f t="shared" si="13"/>
         <v>439</v>
       </c>
       <c r="C441" t="s">
-        <v>431</v>
+        <v>449</v>
       </c>
       <c r="D441" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        YYYYDDD=439,</v>
+        <v xml:space="preserve">        TYPEDEF=439,</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B442" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B442:B447" si="15">B441+1</f>
         <v>440</v>
       </c>
       <c r="C442" t="s">
@@ -8923,7 +8917,7 @@
       </c>
       <c r="D442" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        TYPEDEF=440,</v>
+        <v xml:space="preserve">        STRONG=440,</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
@@ -8936,7 +8930,7 @@
       </c>
       <c r="D443" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRONG=441,</v>
+        <v xml:space="preserve">        UNSAFE=441,</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
@@ -8945,11 +8939,11 @@
         <v>442</v>
       </c>
       <c r="C444" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D444" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        UNSAFE=442,</v>
+        <v xml:space="preserve">        PUBLIC=442,</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -8962,7 +8956,7 @@
       </c>
       <c r="D445" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PUBLIC=443,</v>
+        <v xml:space="preserve">        PRIVATE=443,</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8971,11 +8965,11 @@
         <v>444</v>
       </c>
       <c r="C446" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="D446" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PRIVATE=444,</v>
+        <v xml:space="preserve">        IN_OUT=444,</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -8988,33 +8982,33 @@
       </c>
       <c r="D447" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        IN_OUT=445,</v>
+        <v xml:space="preserve">        STRICT=445,</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B448" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B448:B451" si="16">B447+1</f>
         <v>446</v>
       </c>
       <c r="C448" t="s">
         <v>465</v>
       </c>
       <c r="D448" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRICT=446,</v>
+        <f t="shared" ref="D448:D451" si="17">"        "&amp;C448&amp;"="&amp;B448&amp;","</f>
+        <v xml:space="preserve">        QuestionMark=446,</v>
       </c>
     </row>
     <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" s="1">
-        <f t="shared" ref="B449:B452" si="16">B448+1</f>
+        <f t="shared" si="16"/>
         <v>447</v>
       </c>
       <c r="C449" t="s">
         <v>466</v>
       </c>
       <c r="D449" t="str">
-        <f t="shared" ref="D449:D452" si="17">"        "&amp;C449&amp;"="&amp;B449&amp;","</f>
-        <v xml:space="preserve">        QuestionMark=447,</v>
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">        CompilerDirective=447,</v>
       </c>
     </row>
     <row r="450" spans="2:4" x14ac:dyDescent="0.25">
@@ -9027,7 +9021,7 @@
       </c>
       <c r="D450" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CompilerDirective=448,</v>
+        <v xml:space="preserve">        CopyImportDirective=448,</v>
       </c>
     </row>
     <row r="451" spans="2:4" x14ac:dyDescent="0.25">
@@ -9040,33 +9034,20 @@
       </c>
       <c r="D451" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">        CopyImportDirective=449,</v>
+        <v xml:space="preserve">        ReplaceDirective=449,</v>
       </c>
     </row>
     <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="B452" si="18">B451+1</f>
         <v>450</v>
       </c>
       <c r="C452" t="s">
         <v>469</v>
       </c>
       <c r="D452" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        ReplaceDirective=450,</v>
-      </c>
-    </row>
-    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B453" s="1">
-        <f t="shared" ref="B453" si="18">B452+1</f>
-        <v>451</v>
-      </c>
-      <c r="C453" t="s">
-        <v>470</v>
-      </c>
-      <c r="D453" t="str">
-        <f t="shared" ref="D453" si="19">"        "&amp;C453&amp;"="&amp;B453&amp;","</f>
-        <v xml:space="preserve">        ContinuationTokenGroup=451,</v>
+        <f t="shared" ref="D452" si="19">"        "&amp;C452&amp;"="&amp;B452&amp;","</f>
+        <v xml:space="preserve">        ContinuationTokenGroup=450,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#578, add 59 new Cobol words, update unit tests
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="532">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1434,6 +1437,192 @@
   </si>
   <si>
     <t>EXEC_SQL</t>
+  </si>
+  <si>
+    <t>ALLOCATE</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>CLOCK_UNITS</t>
+  </si>
+  <si>
+    <t>COLUMN</t>
+  </si>
+  <si>
+    <t>COMMUNICATION</t>
+  </si>
+  <si>
+    <t>CONTROL</t>
+  </si>
+  <si>
+    <t>CONTROLS</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>DESTINATION</t>
+  </si>
+  <si>
+    <t>DETAIL</t>
+  </si>
+  <si>
+    <t>DISABLE</t>
+  </si>
+  <si>
+    <t>EGI</t>
+  </si>
+  <si>
+    <t>EMI</t>
+  </si>
+  <si>
+    <t>ENABLE</t>
+  </si>
+  <si>
+    <t>END_RECEIVE</t>
+  </si>
+  <si>
+    <t>ESI</t>
+  </si>
+  <si>
+    <t>FINAL</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>GROUP</t>
+  </si>
+  <si>
+    <t>HEADING</t>
+  </si>
+  <si>
+    <t>INDICATE</t>
+  </si>
+  <si>
+    <t>INITIATE</t>
+  </si>
+  <si>
+    <t>LAST</t>
+  </si>
+  <si>
+    <t>LIMIT</t>
+  </si>
+  <si>
+    <t>LIMITS</t>
+  </si>
+  <si>
+    <t>LINE_COUNTER</t>
+  </si>
+  <si>
+    <t>MESSAGE</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>PAGE_COUNTER</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>PLUS</t>
+  </si>
+  <si>
+    <t>PRINTING</t>
+  </si>
+  <si>
+    <t>PURGE</t>
+  </si>
+  <si>
+    <t>QUEUE</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>RECEIVE</t>
+  </si>
+  <si>
+    <t>REPORT</t>
+  </si>
+  <si>
+    <t>REPORTING</t>
+  </si>
+  <si>
+    <t>REPORTS</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>SEGMENT</t>
+  </si>
+  <si>
+    <t>SEND</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>SUB_QUEUE_1</t>
+  </si>
+  <si>
+    <t>SUB_QUEUE_2</t>
+  </si>
+  <si>
+    <t>SUB_QUEUE_3</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>TABLE</t>
+  </si>
+  <si>
+    <t>TERMINAL</t>
+  </si>
+  <si>
+    <t>TERMINATE</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>END_JSON</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>VOLATILE</t>
+  </si>
+  <si>
+    <t>//Cobol V6</t>
+  </si>
+  <si>
+    <t>//Cobol 2002</t>
+  </si>
+  <si>
+    <t>//TypeCobol</t>
   </si>
 </sst>
 </file>
@@ -1580,6 +1769,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Feuil1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1845,10 +2047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D452"/>
+  <dimension ref="A1:D511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A477" workbookViewId="0">
+      <selection activeCell="C503" sqref="C503"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,6 +2059,8 @@
     <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="54.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
     <col min="13" max="13" width="46.85546875" customWidth="1"/>
     <col min="14" max="14" width="36.7109375" customWidth="1"/>
   </cols>
@@ -7907,7 +8111,7 @@
         <v>431</v>
       </c>
       <c r="B379" s="1">
-        <f t="shared" ref="B379:B441" si="13">B378+1</f>
+        <f t="shared" ref="B379:B442" si="13">B378+1</f>
         <v>377</v>
       </c>
       <c r="C379" t="s">
@@ -8874,7 +9078,7 @@
         <v>428</v>
       </c>
       <c r="D439" t="str">
-        <f t="shared" ref="D439:D447" si="14">"        "&amp;C439&amp;"="&amp;B439&amp;","</f>
+        <f t="shared" ref="D439:D502" si="14">"        "&amp;C439&amp;"="&amp;B439&amp;","</f>
         <v xml:space="preserve">        WRITE_ONLY=437,</v>
       </c>
     </row>
@@ -8900,37 +9104,37 @@
         <v>439</v>
       </c>
       <c r="C441" t="s">
-        <v>448</v>
+        <v>470</v>
       </c>
       <c r="D441" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        TYPEDEF=439,</v>
+        <v xml:space="preserve">        ALLOCATE=439,</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B442" s="1">
-        <f t="shared" ref="B442:B447" si="15">B441+1</f>
+        <f t="shared" si="13"/>
         <v>440</v>
       </c>
       <c r="C442" t="s">
-        <v>449</v>
+        <v>471</v>
       </c>
       <c r="D442" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRONG=440,</v>
+        <v xml:space="preserve">        CD=440,</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B443" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="B443:B506" si="15">B442+1</f>
         <v>441</v>
       </c>
       <c r="C443" t="s">
-        <v>450</v>
+        <v>472</v>
       </c>
       <c r="D443" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        UNSAFE=441,</v>
+        <v xml:space="preserve">        CF=441,</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
@@ -8939,11 +9143,11 @@
         <v>442</v>
       </c>
       <c r="C444" t="s">
-        <v>453</v>
+        <v>473</v>
       </c>
       <c r="D444" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PUBLIC=442,</v>
+        <v xml:space="preserve">        CH=442,</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -8952,11 +9156,11 @@
         <v>443</v>
       </c>
       <c r="C445" t="s">
-        <v>454</v>
+        <v>474</v>
       </c>
       <c r="D445" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        PRIVATE=443,</v>
+        <v xml:space="preserve">        CLOCK_UNITS=443,</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8965,11 +9169,11 @@
         <v>444</v>
       </c>
       <c r="C446" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="D446" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        IN_OUT=444,</v>
+        <v xml:space="preserve">        COLUMN=444,</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -8978,85 +9182,867 @@
         <v>445</v>
       </c>
       <c r="C447" t="s">
-        <v>463</v>
+        <v>476</v>
       </c>
       <c r="D447" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">        STRICT=445,</v>
+        <v xml:space="preserve">        COMMUNICATION=445,</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B448" s="1">
-        <f t="shared" ref="B448:B451" si="16">B447+1</f>
+        <f t="shared" si="15"/>
         <v>446</v>
       </c>
       <c r="C448" t="s">
-        <v>464</v>
+        <v>477</v>
       </c>
       <c r="D448" t="str">
-        <f t="shared" ref="D448:D451" si="17">"        "&amp;C448&amp;"="&amp;B448&amp;","</f>
-        <v xml:space="preserve">        QuestionMark=446,</v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        CONTROL=446,</v>
       </c>
     </row>
     <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>447</v>
       </c>
       <c r="C449" t="s">
-        <v>465</v>
+        <v>478</v>
       </c>
       <c r="D449" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        CompilerDirective=447,</v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        CONTROLS=447,</v>
       </c>
     </row>
     <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B450" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>448</v>
       </c>
       <c r="C450" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="D450" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        CopyImportDirective=448,</v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        DE=448,</v>
       </c>
     </row>
     <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B451" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>449</v>
       </c>
       <c r="C451" t="s">
-        <v>467</v>
+        <v>480</v>
       </c>
       <c r="D451" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">        ReplaceDirective=449,</v>
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        DEFAULT=449,</v>
       </c>
     </row>
     <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" s="1">
-        <f t="shared" ref="B452" si="18">B451+1</f>
+        <f t="shared" si="15"/>
         <v>450</v>
       </c>
       <c r="C452" t="s">
+        <v>481</v>
+      </c>
+      <c r="D452" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        DESTINATION=450,</v>
+      </c>
+    </row>
+    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B453" s="1">
+        <f t="shared" si="15"/>
+        <v>451</v>
+      </c>
+      <c r="C453" t="s">
+        <v>482</v>
+      </c>
+      <c r="D453" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        DETAIL=451,</v>
+      </c>
+    </row>
+    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B454" s="1">
+        <f t="shared" si="15"/>
+        <v>452</v>
+      </c>
+      <c r="C454" t="s">
+        <v>483</v>
+      </c>
+      <c r="D454" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        DISABLE=452,</v>
+      </c>
+    </row>
+    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B455" s="1">
+        <f t="shared" si="15"/>
+        <v>453</v>
+      </c>
+      <c r="C455" t="s">
+        <v>484</v>
+      </c>
+      <c r="D455" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        EGI=453,</v>
+      </c>
+    </row>
+    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B456" s="1">
+        <f t="shared" si="15"/>
+        <v>454</v>
+      </c>
+      <c r="C456" t="s">
+        <v>485</v>
+      </c>
+      <c r="D456" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        EMI=454,</v>
+      </c>
+    </row>
+    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B457" s="1">
+        <f t="shared" si="15"/>
+        <v>455</v>
+      </c>
+      <c r="C457" t="s">
+        <v>486</v>
+      </c>
+      <c r="D457" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        ENABLE=455,</v>
+      </c>
+    </row>
+    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B458" s="1">
+        <f t="shared" si="15"/>
+        <v>456</v>
+      </c>
+      <c r="C458" t="s">
+        <v>487</v>
+      </c>
+      <c r="D458" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        END_RECEIVE=456,</v>
+      </c>
+    </row>
+    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B459" s="1">
+        <f t="shared" si="15"/>
+        <v>457</v>
+      </c>
+      <c r="C459" t="s">
+        <v>488</v>
+      </c>
+      <c r="D459" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        ESI=457,</v>
+      </c>
+    </row>
+    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B460" s="1">
+        <f t="shared" si="15"/>
+        <v>458</v>
+      </c>
+      <c r="C460" t="s">
+        <v>489</v>
+      </c>
+      <c r="D460" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        FINAL=458,</v>
+      </c>
+    </row>
+    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B461" s="1">
+        <f t="shared" si="15"/>
+        <v>459</v>
+      </c>
+      <c r="C461" t="s">
+        <v>490</v>
+      </c>
+      <c r="D461" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        FREE=459,</v>
+      </c>
+    </row>
+    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B462" s="1">
+        <f t="shared" si="15"/>
+        <v>460</v>
+      </c>
+      <c r="C462" t="s">
+        <v>491</v>
+      </c>
+      <c r="D462" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        GROUP=460,</v>
+      </c>
+    </row>
+    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B463" s="1">
+        <f t="shared" si="15"/>
+        <v>461</v>
+      </c>
+      <c r="C463" t="s">
+        <v>492</v>
+      </c>
+      <c r="D463" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        HEADING=461,</v>
+      </c>
+    </row>
+    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B464" s="1">
+        <f t="shared" si="15"/>
+        <v>462</v>
+      </c>
+      <c r="C464" t="s">
+        <v>493</v>
+      </c>
+      <c r="D464" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        INDICATE=462,</v>
+      </c>
+    </row>
+    <row r="465" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B465" s="1">
+        <f t="shared" si="15"/>
+        <v>463</v>
+      </c>
+      <c r="C465" t="s">
+        <v>494</v>
+      </c>
+      <c r="D465" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        INITIATE=463,</v>
+      </c>
+    </row>
+    <row r="466" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B466" s="1">
+        <f t="shared" si="15"/>
+        <v>464</v>
+      </c>
+      <c r="C466" t="s">
+        <v>495</v>
+      </c>
+      <c r="D466" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        LAST=464,</v>
+      </c>
+    </row>
+    <row r="467" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B467" s="1">
+        <f t="shared" si="15"/>
+        <v>465</v>
+      </c>
+      <c r="C467" t="s">
+        <v>496</v>
+      </c>
+      <c r="D467" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        LIMIT=465,</v>
+      </c>
+    </row>
+    <row r="468" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B468" s="1">
+        <f t="shared" si="15"/>
+        <v>466</v>
+      </c>
+      <c r="C468" t="s">
+        <v>497</v>
+      </c>
+      <c r="D468" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        LIMITS=466,</v>
+      </c>
+    </row>
+    <row r="469" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B469" s="1">
+        <f t="shared" si="15"/>
+        <v>467</v>
+      </c>
+      <c r="C469" t="s">
+        <v>498</v>
+      </c>
+      <c r="D469" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        LINE_COUNTER=467,</v>
+      </c>
+    </row>
+    <row r="470" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B470" s="1">
+        <f t="shared" si="15"/>
         <v>468</v>
       </c>
-      <c r="D452" t="str">
-        <f t="shared" ref="D452" si="19">"        "&amp;C452&amp;"="&amp;B452&amp;","</f>
-        <v xml:space="preserve">        ContinuationTokenGroup=450,</v>
+      <c r="C470" t="s">
+        <v>499</v>
+      </c>
+      <c r="D470" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        MESSAGE=468,</v>
+      </c>
+    </row>
+    <row r="471" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B471" s="1">
+        <f t="shared" si="15"/>
+        <v>469</v>
+      </c>
+      <c r="C471" t="s">
+        <v>500</v>
+      </c>
+      <c r="D471" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        NUMBER=469,</v>
+      </c>
+    </row>
+    <row r="472" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B472" s="1">
+        <f t="shared" si="15"/>
+        <v>470</v>
+      </c>
+      <c r="C472" t="s">
+        <v>501</v>
+      </c>
+      <c r="D472" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        PAGE_COUNTER=470,</v>
+      </c>
+    </row>
+    <row r="473" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B473" s="1">
+        <f t="shared" si="15"/>
+        <v>471</v>
+      </c>
+      <c r="C473" t="s">
+        <v>502</v>
+      </c>
+      <c r="D473" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        PF=471,</v>
+      </c>
+    </row>
+    <row r="474" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B474" s="1">
+        <f t="shared" si="15"/>
+        <v>472</v>
+      </c>
+      <c r="C474" t="s">
+        <v>503</v>
+      </c>
+      <c r="D474" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        PH=472,</v>
+      </c>
+    </row>
+    <row r="475" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B475" s="1">
+        <f t="shared" si="15"/>
+        <v>473</v>
+      </c>
+      <c r="C475" t="s">
+        <v>504</v>
+      </c>
+      <c r="D475" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        PLUS=473,</v>
+      </c>
+    </row>
+    <row r="476" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B476" s="1">
+        <f t="shared" si="15"/>
+        <v>474</v>
+      </c>
+      <c r="C476" t="s">
+        <v>505</v>
+      </c>
+      <c r="D476" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        PRINTING=474,</v>
+      </c>
+    </row>
+    <row r="477" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B477" s="1">
+        <f t="shared" si="15"/>
+        <v>475</v>
+      </c>
+      <c r="C477" t="s">
+        <v>506</v>
+      </c>
+      <c r="D477" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        PURGE=475,</v>
+      </c>
+    </row>
+    <row r="478" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B478" s="1">
+        <f t="shared" si="15"/>
+        <v>476</v>
+      </c>
+      <c r="C478" t="s">
+        <v>507</v>
+      </c>
+      <c r="D478" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        QUEUE=476,</v>
+      </c>
+    </row>
+    <row r="479" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B479" s="1">
+        <f t="shared" si="15"/>
+        <v>477</v>
+      </c>
+      <c r="C479" t="s">
+        <v>508</v>
+      </c>
+      <c r="D479" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        RD=477,</v>
+      </c>
+    </row>
+    <row r="480" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B480" s="1">
+        <f t="shared" si="15"/>
+        <v>478</v>
+      </c>
+      <c r="C480" t="s">
+        <v>509</v>
+      </c>
+      <c r="D480" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        RECEIVE=478,</v>
+      </c>
+    </row>
+    <row r="481" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B481" s="1">
+        <f t="shared" si="15"/>
+        <v>479</v>
+      </c>
+      <c r="C481" t="s">
+        <v>510</v>
+      </c>
+      <c r="D481" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        REPORT=479,</v>
+      </c>
+    </row>
+    <row r="482" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B482" s="1">
+        <f t="shared" si="15"/>
+        <v>480</v>
+      </c>
+      <c r="C482" t="s">
+        <v>511</v>
+      </c>
+      <c r="D482" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        REPORTING=480,</v>
+      </c>
+    </row>
+    <row r="483" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B483" s="1">
+        <f t="shared" si="15"/>
+        <v>481</v>
+      </c>
+      <c r="C483" t="s">
+        <v>512</v>
+      </c>
+      <c r="D483" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        REPORTS=481,</v>
+      </c>
+    </row>
+    <row r="484" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B484" s="1">
+        <f t="shared" si="15"/>
+        <v>482</v>
+      </c>
+      <c r="C484" t="s">
+        <v>513</v>
+      </c>
+      <c r="D484" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        RF=482,</v>
+      </c>
+    </row>
+    <row r="485" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B485" s="1">
+        <f t="shared" si="15"/>
+        <v>483</v>
+      </c>
+      <c r="C485" t="s">
+        <v>514</v>
+      </c>
+      <c r="D485" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        RH=483,</v>
+      </c>
+    </row>
+    <row r="486" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B486" s="1">
+        <f t="shared" si="15"/>
+        <v>484</v>
+      </c>
+      <c r="C486" t="s">
+        <v>515</v>
+      </c>
+      <c r="D486" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        SEGMENT=484,</v>
+      </c>
+    </row>
+    <row r="487" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B487" s="1">
+        <f t="shared" si="15"/>
+        <v>485</v>
+      </c>
+      <c r="C487" t="s">
+        <v>516</v>
+      </c>
+      <c r="D487" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        SEND=485,</v>
+      </c>
+    </row>
+    <row r="488" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B488" s="1">
+        <f t="shared" si="15"/>
+        <v>486</v>
+      </c>
+      <c r="C488" t="s">
+        <v>517</v>
+      </c>
+      <c r="D488" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        SOURCE=486,</v>
+      </c>
+    </row>
+    <row r="489" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B489" s="1">
+        <f t="shared" si="15"/>
+        <v>487</v>
+      </c>
+      <c r="C489" t="s">
+        <v>518</v>
+      </c>
+      <c r="D489" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        SUB_QUEUE_1=487,</v>
+      </c>
+    </row>
+    <row r="490" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B490" s="1">
+        <f t="shared" si="15"/>
+        <v>488</v>
+      </c>
+      <c r="C490" t="s">
+        <v>519</v>
+      </c>
+      <c r="D490" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        SUB_QUEUE_2=488,</v>
+      </c>
+    </row>
+    <row r="491" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B491" s="1">
+        <f t="shared" si="15"/>
+        <v>489</v>
+      </c>
+      <c r="C491" t="s">
+        <v>520</v>
+      </c>
+      <c r="D491" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        SUB_QUEUE_3=489,</v>
+      </c>
+    </row>
+    <row r="492" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B492" s="1">
+        <f t="shared" si="15"/>
+        <v>490</v>
+      </c>
+      <c r="C492" t="s">
+        <v>521</v>
+      </c>
+      <c r="D492" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        SUM=490,</v>
+      </c>
+    </row>
+    <row r="493" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B493" s="1">
+        <f t="shared" si="15"/>
+        <v>491</v>
+      </c>
+      <c r="C493" t="s">
+        <v>522</v>
+      </c>
+      <c r="D493" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        TABLE=491,</v>
+      </c>
+    </row>
+    <row r="494" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B494" s="1">
+        <f t="shared" si="15"/>
+        <v>492</v>
+      </c>
+      <c r="C494" t="s">
+        <v>523</v>
+      </c>
+      <c r="D494" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        TERMINAL=492,</v>
+      </c>
+    </row>
+    <row r="495" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B495" s="1">
+        <f t="shared" si="15"/>
+        <v>493</v>
+      </c>
+      <c r="C495" t="s">
+        <v>524</v>
+      </c>
+      <c r="D495" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        TERMINATE=493,</v>
+      </c>
+    </row>
+    <row r="496" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B496" s="1">
+        <f t="shared" si="15"/>
+        <v>494</v>
+      </c>
+      <c r="C496" t="s">
+        <v>525</v>
+      </c>
+      <c r="D496" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        TEXT=494,</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>529</v>
+      </c>
+      <c r="B497" s="1">
+        <f t="shared" si="15"/>
+        <v>495</v>
+      </c>
+      <c r="C497" t="s">
+        <v>526</v>
+      </c>
+      <c r="D497" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        END_JSON=495,</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B498" s="1">
+        <f t="shared" si="15"/>
+        <v>496</v>
+      </c>
+      <c r="C498" t="s">
+        <v>527</v>
+      </c>
+      <c r="D498" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        JSON=496,</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B499" s="1">
+        <f t="shared" si="15"/>
+        <v>497</v>
+      </c>
+      <c r="C499" t="s">
+        <v>528</v>
+      </c>
+      <c r="D499" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        VOLATILE=497,</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>530</v>
+      </c>
+      <c r="B500" s="1">
+        <f t="shared" si="15"/>
+        <v>498</v>
+      </c>
+      <c r="C500" t="s">
+        <v>448</v>
+      </c>
+      <c r="D500" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        TYPEDEF=498,</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B501" s="1">
+        <f t="shared" si="15"/>
+        <v>499</v>
+      </c>
+      <c r="C501" t="s">
+        <v>449</v>
+      </c>
+      <c r="D501" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        STRONG=499,</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>531</v>
+      </c>
+      <c r="B502" s="1">
+        <f t="shared" si="15"/>
+        <v>500</v>
+      </c>
+      <c r="C502" t="s">
+        <v>450</v>
+      </c>
+      <c r="D502" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">        UNSAFE=500,</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B503" s="1">
+        <f t="shared" si="15"/>
+        <v>501</v>
+      </c>
+      <c r="C503" t="s">
+        <v>453</v>
+      </c>
+      <c r="D503" t="str">
+        <f t="shared" ref="D503:D511" si="16">"        "&amp;C503&amp;"="&amp;B503&amp;","</f>
+        <v xml:space="preserve">        PUBLIC=501,</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B504" s="1">
+        <f t="shared" si="15"/>
+        <v>502</v>
+      </c>
+      <c r="C504" t="s">
+        <v>454</v>
+      </c>
+      <c r="D504" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        PRIVATE=502,</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B505" s="1">
+        <f t="shared" si="15"/>
+        <v>503</v>
+      </c>
+      <c r="C505" t="s">
+        <v>462</v>
+      </c>
+      <c r="D505" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        IN_OUT=503,</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B506" s="1">
+        <f t="shared" si="15"/>
+        <v>504</v>
+      </c>
+      <c r="C506" t="s">
+        <v>463</v>
+      </c>
+      <c r="D506" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        STRICT=504,</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B507" s="1">
+        <f t="shared" ref="B507:B511" si="17">B506+1</f>
+        <v>505</v>
+      </c>
+      <c r="C507" t="s">
+        <v>464</v>
+      </c>
+      <c r="D507" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        QuestionMark=505,</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B508" s="1">
+        <f t="shared" si="17"/>
+        <v>506</v>
+      </c>
+      <c r="C508" t="s">
+        <v>465</v>
+      </c>
+      <c r="D508" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        CompilerDirective=506,</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B509" s="1">
+        <f t="shared" si="17"/>
+        <v>507</v>
+      </c>
+      <c r="C509" t="s">
+        <v>466</v>
+      </c>
+      <c r="D509" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        CopyImportDirective=507,</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B510" s="1">
+        <f t="shared" si="17"/>
+        <v>508</v>
+      </c>
+      <c r="C510" t="s">
+        <v>467</v>
+      </c>
+      <c r="D510" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        ReplaceDirective=508,</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B511" s="1">
+        <f t="shared" si="17"/>
+        <v>509</v>
+      </c>
+      <c r="C511" t="s">
+        <v>468</v>
+      </c>
+      <c r="D511" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        ContinuationTokenGroup=509,</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  <conditionalFormatting sqref="C1:C441 C454:C496 C552:C1048576 C500:C539">
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C441 C454:C496 C552:C1048576 C500:C539">
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C497:C499">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#805, add GlobalStorageSection CodeElement + Node
</commit_message>
<xml_diff>
--- a/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
+++ b/TypeCobol.Grammar/Grammars/Cobol/TokenTypes.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="533">
   <si>
     <t>SpaceSeparator</t>
   </si>
@@ -1623,6 +1620,9 @@
   </si>
   <si>
     <t>//TypeCobol</t>
+  </si>
+  <si>
+    <t>GLOBAL_STORAGE</t>
   </si>
 </sst>
 </file>
@@ -1667,47 +1667,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1769,19 +1729,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Feuil1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2047,10 +1994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D511"/>
+  <dimension ref="A1:D512"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A477" workbookViewId="0">
-      <selection activeCell="C503" sqref="C503"/>
+      <selection activeCell="C507" sqref="C507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9126,7 +9073,7 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B443" s="1">
-        <f t="shared" ref="B443:B506" si="15">B442+1</f>
+        <f t="shared" ref="B443:B505" si="15">B442+1</f>
         <v>441</v>
       </c>
       <c r="C443" t="s">
@@ -9922,7 +9869,7 @@
         <v>453</v>
       </c>
       <c r="D503" t="str">
-        <f t="shared" ref="D503:D511" si="16">"        "&amp;C503&amp;"="&amp;B503&amp;","</f>
+        <f t="shared" ref="D503:D512" si="16">"        "&amp;C503&amp;"="&amp;B503&amp;","</f>
         <v xml:space="preserve">        PUBLIC=501,</v>
       </c>
     </row>
@@ -9954,7 +9901,7 @@
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B506" s="1">
-        <f t="shared" si="15"/>
+        <f>B505+1</f>
         <v>504</v>
       </c>
       <c r="C506" t="s">
@@ -9967,15 +9914,15 @@
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B507" s="1">
-        <f t="shared" ref="B507:B511" si="17">B506+1</f>
+        <f t="shared" ref="B507:B512" si="17">B506+1</f>
         <v>505</v>
       </c>
       <c r="C507" t="s">
-        <v>464</v>
+        <v>532</v>
       </c>
       <c r="D507" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">        QuestionMark=505,</v>
+        <v xml:space="preserve">        GLOBAL_STORAGE=505,</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.25">
@@ -9984,11 +9931,11 @@
         <v>506</v>
       </c>
       <c r="C508" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D508" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">        CompilerDirective=506,</v>
+        <v xml:space="preserve">        QuestionMark=506,</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.25">
@@ -9997,11 +9944,11 @@
         <v>507</v>
       </c>
       <c r="C509" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D509" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">        CopyImportDirective=507,</v>
+        <v xml:space="preserve">        CompilerDirective=507,</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.25">
@@ -10010,11 +9957,11 @@
         <v>508</v>
       </c>
       <c r="C510" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D510" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">        ReplaceDirective=508,</v>
+        <v xml:space="preserve">        CopyImportDirective=508,</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.25">
@@ -10023,23 +9970,36 @@
         <v>509</v>
       </c>
       <c r="C511" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D511" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">        ContinuationTokenGroup=509,</v>
+        <v xml:space="preserve">        ReplaceDirective=509,</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B512" s="1">
+        <f t="shared" si="17"/>
+        <v>510</v>
+      </c>
+      <c r="C512" t="s">
+        <v>468</v>
+      </c>
+      <c r="D512" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">        ContinuationTokenGroup=510,</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C441 C454:C496 C552:C1048576 C500:C539">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+  <conditionalFormatting sqref="C553:C1048576 C1:C441 C454:C496 C500:C540">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C441 C454:C496 C552:C1048576 C500:C539">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+  <conditionalFormatting sqref="C553:C1048576 C1:C441 C454:C496 C500:C540">
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C497:C499">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>